<commit_message>
Updated with latest obs data and started modelling two treatments
</commit_message>
<xml_diff>
--- a/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
+++ b/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Prototypes\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4FF52D-DDA2-4DAC-9B16-E23DCCF26106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2661C39-2762-480F-9945-B52C647C247C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="17">
   <si>
     <t>SimulationName</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Cotton.Leaf.Height</t>
   </si>
   <si>
-    <t>ForestHill2023Irrigated</t>
-  </si>
-  <si>
     <t>Cotton.Leaf.NodeNumber</t>
   </si>
   <si>
@@ -84,6 +81,12 @@
   </si>
   <si>
     <t>Cotton.AboveGround.Wt</t>
+  </si>
+  <si>
+    <t>ForestHill2023IrrigationFull</t>
+  </si>
+  <si>
+    <t>ForestHill2023IrrigationPartial</t>
   </si>
 </sst>
 </file>
@@ -119,9 +122,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,8 +442,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C911DF83-7300-4B7A-8A42-16858D40307A}">
   <dimension ref="A1:O1655"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="9970" ySplit="760" topLeftCell="I1" activePane="bottomRight"/>
+      <selection sqref="A1:A1048576"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -450,7 +458,7 @@
     <col min="4" max="4" width="25.73046875" bestFit="1" customWidth="1"/>
     <col min="5" max="9" width="25.73046875" customWidth="1"/>
     <col min="10" max="10" width="38.1328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.06640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="36.265625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="32.3984375" bestFit="1" customWidth="1"/>
@@ -583,414 +591,787 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
-      </c>
-      <c r="O1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1">
         <v>45236</v>
       </c>
       <c r="J2">
-        <v>99.508333333333326</v>
+        <v>105.68333333333334</v>
       </c>
       <c r="K2">
-        <v>89.491666666666674</v>
+        <v>96.683333333333337</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1">
         <v>45243</v>
       </c>
       <c r="J3">
-        <v>112.71666666666668</v>
+        <v>120.93333333333334</v>
       </c>
       <c r="K3">
-        <v>137.26666666666665</v>
+        <v>139.43333333333331</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1">
         <v>45248</v>
       </c>
       <c r="J4">
-        <v>134.56666666666663</v>
+        <v>144.7833333333333</v>
       </c>
       <c r="K4">
-        <v>160.47499999999999</v>
+        <v>162.56666666666666</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1">
         <v>45254</v>
       </c>
       <c r="C5">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="D5">
-        <v>1.3249999999999997</v>
-      </c>
-      <c r="E5">
-        <f>D5</f>
-        <v>1.3249999999999997</v>
+        <v>1.45</v>
       </c>
       <c r="J5">
-        <v>161.20833333333334</v>
+        <v>163.91666666666666</v>
       </c>
       <c r="K5">
-        <v>177.06666666666669</v>
+        <v>183.21666666666667</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1">
         <v>45259</v>
       </c>
       <c r="C6">
-        <v>137.75</v>
+        <v>153</v>
       </c>
       <c r="D6">
-        <v>2.7</v>
-      </c>
-      <c r="E6">
-        <f>D6</f>
-        <v>2.7</v>
+        <v>2.85</v>
       </c>
       <c r="F6">
-        <v>0.10537249175836584</v>
+        <v>0.10276899785187731</v>
       </c>
       <c r="G6">
-        <v>1.5362836185331781E-2</v>
+        <v>2.4123522851920851E-2</v>
       </c>
       <c r="J6">
-        <v>172.19166666666669</v>
+        <v>178.29999999999998</v>
       </c>
       <c r="K6">
-        <v>171.61666666666667</v>
+        <v>172.93333333333331</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1">
         <v>45266</v>
       </c>
       <c r="C7">
-        <v>249.75</v>
+        <v>250</v>
       </c>
       <c r="D7">
-        <v>5.7</v>
-      </c>
-      <c r="E7">
-        <f>D7+0.4</f>
-        <v>6.1000000000000005</v>
+        <v>6.05</v>
       </c>
       <c r="F7">
-        <v>0.22133904244420988</v>
+        <v>0.22487305131812216</v>
       </c>
       <c r="G7">
-        <v>2.2078938884477262E-2</v>
+        <v>1.3732764172807894E-2</v>
       </c>
       <c r="H7">
-        <f>209/1080</f>
-        <v>0.19351851851851851</v>
+        <v>0.19663461538461538</v>
       </c>
       <c r="I7">
-        <f>37/1080</f>
-        <v>3.425925925925926E-2</v>
+        <v>3.5770618361488406E-2</v>
       </c>
       <c r="J7">
-        <v>180.39166666666665</v>
+        <v>178.16666666666666</v>
       </c>
       <c r="K7">
-        <v>180.11666666666665</v>
+        <v>192.94999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1">
         <v>45273</v>
       </c>
       <c r="C8">
-        <v>341.79487179487177</v>
+        <v>337</v>
       </c>
       <c r="D8">
-        <v>8.02</v>
+        <v>8</v>
+      </c>
+      <c r="G8">
+        <v>3.605272908788857E-2</v>
       </c>
       <c r="H8">
-        <f>303/1080</f>
-        <v>0.28055555555555556</v>
+        <v>0.27596153846153848</v>
       </c>
       <c r="I8">
-        <f>50.3/1080</f>
-        <v>4.6574074074074073E-2</v>
+        <v>4.7629496970109417E-2</v>
       </c>
       <c r="J8">
-        <v>175.76666666666665</v>
+        <v>182.6</v>
       </c>
       <c r="K8">
-        <v>159.64166666666668</v>
+        <v>161.20000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1">
         <v>45274</v>
       </c>
       <c r="F9">
-        <v>0.48768159019795621</v>
+        <v>0.5190413407082255</v>
       </c>
       <c r="G9">
-        <v>4.7652068115226938E-2</v>
+        <v>3.605272908788857E-2</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1">
         <v>45279</v>
       </c>
       <c r="C10">
-        <v>455.25</v>
+        <v>448.5</v>
       </c>
       <c r="D10">
-        <v>10.050000000000001</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="E10">
-        <v>20.5</v>
+        <v>19.8</v>
       </c>
       <c r="F10">
-        <v>0.87627310990763219</v>
+        <v>0.93459622187351832</v>
       </c>
       <c r="G10">
-        <v>5.594878235236022E-2</v>
+        <v>0.14620537270042952</v>
       </c>
       <c r="H10">
-        <f>427/1080</f>
-        <v>0.39537037037037037</v>
+        <v>0.41602564102564105</v>
       </c>
       <c r="I10">
-        <f>51.1/1080</f>
-        <v>4.7314814814814816E-2</v>
+        <v>4.632333044943851E-2</v>
       </c>
       <c r="J10">
-        <v>168.3923076923077</v>
+        <v>176.85714285714286</v>
       </c>
       <c r="K10">
-        <v>140.16153846153844</v>
+        <v>142.31428571428572</v>
       </c>
       <c r="L10">
-        <v>66</v>
+        <v>61.869882044725493</v>
       </c>
       <c r="M10">
-        <v>51.12</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
+        <v>47.219165425471701</v>
       </c>
       <c r="O10">
-        <f>L10+M10+N10</f>
-        <v>117.12</v>
+        <v>109.08904747019719</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1">
         <v>45288</v>
       </c>
-      <c r="C11">
-        <v>586.5</v>
-      </c>
-      <c r="D11">
-        <v>12.2</v>
-      </c>
       <c r="F11">
-        <v>2.1887556760641602</v>
+        <v>2.2807749309999026</v>
       </c>
       <c r="G11">
-        <v>0.11200411112333544</v>
-      </c>
-      <c r="H11">
-        <f>644/1080</f>
-        <v>0.59629629629629632</v>
-      </c>
-      <c r="I11">
-        <f>60.6/1080</f>
-        <v>5.6111111111111112E-2</v>
+        <v>4.1026933330751199E-2</v>
       </c>
       <c r="J11">
-        <v>191.15</v>
+        <v>198.48333333333335</v>
       </c>
       <c r="K11">
-        <v>188.20000000000005</v>
+        <v>190.58333333333337</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1">
         <v>45296</v>
       </c>
       <c r="C12">
-        <v>781.75</v>
-      </c>
-      <c r="D12">
-        <v>14.15</v>
+        <v>770.5</v>
       </c>
       <c r="E12">
-        <v>40.6</v>
+        <v>41.2</v>
       </c>
       <c r="F12">
-        <v>3.0549311199492775</v>
+        <v>2.9598787282147736</v>
       </c>
       <c r="G12">
-        <v>8.8688985328476785E-2</v>
+        <v>7.4730791031138666E-2</v>
       </c>
       <c r="H12">
-        <f>787/1080</f>
-        <v>0.72870370370370374</v>
+        <v>0.75</v>
       </c>
       <c r="I12">
-        <f>81.4/1080</f>
-        <v>7.5370370370370379E-2</v>
+        <v>8.4403488823438802E-2</v>
       </c>
       <c r="J12">
-        <v>185.00833333333335</v>
+        <v>195.43333333333337</v>
       </c>
       <c r="K12">
-        <v>147.51666666666668</v>
+        <v>145.15</v>
       </c>
       <c r="L12">
-        <v>157.80000000000001</v>
+        <v>148.32379686792672</v>
       </c>
       <c r="M12">
-        <v>196.7</v>
+        <v>182.30627017799995</v>
       </c>
       <c r="O12">
-        <f>L12+M12+N12</f>
-        <v>354.5</v>
+        <v>330.63006704592664</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1">
         <v>45302</v>
       </c>
       <c r="C13">
-        <v>962</v>
+        <v>973</v>
       </c>
       <c r="D13">
-        <v>16.233333333333334</v>
+        <v>16.3</v>
       </c>
       <c r="H13">
-        <f>919/1080</f>
-        <v>0.85092592592592597</v>
+        <v>0.92307692307692313</v>
       </c>
       <c r="I13">
-        <f>80/1080</f>
-        <v>7.407407407407407E-2</v>
+        <v>0.10013140610136738</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B14" s="1">
         <v>45306</v>
       </c>
       <c r="C14">
-        <v>1008.6666666666666</v>
+        <v>1014</v>
       </c>
       <c r="H14">
-        <f>955/1080</f>
-        <v>0.8842592592592593</v>
+        <v>0.9028846153846154</v>
       </c>
       <c r="I14">
-        <f>58.6/1080</f>
-        <v>5.4259259259259264E-2</v>
+        <v>7.0723752109358815E-2</v>
       </c>
       <c r="J14">
-        <v>145.87499999999997</v>
+        <v>158.63333333333333</v>
       </c>
       <c r="K14">
-        <v>102.64999999999999</v>
+        <v>104.5</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1">
         <v>45307</v>
       </c>
       <c r="D15">
-        <v>16.95</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="E15">
-        <v>53.7</v>
+        <v>52.9</v>
       </c>
       <c r="F15">
-        <v>4.16</v>
+        <v>4.2869858289235543</v>
       </c>
       <c r="G15">
-        <v>0.41499999999999998</v>
+        <v>0.46875655267478084</v>
+      </c>
+      <c r="L15">
+        <v>235.61860053445332</v>
+      </c>
+      <c r="M15">
+        <v>329.13664247461998</v>
+      </c>
+      <c r="N15">
+        <v>39.927173460593856</v>
+      </c>
+      <c r="O15">
+        <v>604.68241646966715</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>45314</v>
+      </c>
+      <c r="C16">
+        <v>1175.5</v>
+      </c>
+      <c r="D16">
+        <v>18.149999999999999</v>
+      </c>
+      <c r="H16">
+        <v>0.98701923076923082</v>
+      </c>
+      <c r="I16">
+        <v>7.2646492320450506E-2</v>
+      </c>
+      <c r="J16">
+        <v>202.79999999999998</v>
+      </c>
+      <c r="K16">
+        <v>173.93333333333331</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>45236</v>
+      </c>
+      <c r="J17">
+        <v>93.333333333333329</v>
+      </c>
+      <c r="K17" s="2">
+        <v>82.300000000000011</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1">
+        <v>45243</v>
+      </c>
+      <c r="J18">
+        <v>104.5</v>
+      </c>
+      <c r="K18" s="2">
+        <v>135.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="1">
+        <v>45248</v>
+      </c>
+      <c r="J19">
+        <v>124.35000000000002</v>
+      </c>
+      <c r="K19" s="2">
+        <v>158.38333333333333</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="1">
+        <v>45254</v>
+      </c>
+      <c r="C20">
+        <v>70</v>
+      </c>
+      <c r="D20">
+        <v>1.2</v>
+      </c>
+      <c r="J20">
+        <v>158.5</v>
+      </c>
+      <c r="K20" s="2">
+        <v>170.91666666666666</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="1">
+        <v>45259</v>
+      </c>
+      <c r="C21">
+        <v>122.5</v>
+      </c>
+      <c r="D21">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="F21">
+        <v>0.10798078444273128</v>
+      </c>
+      <c r="G21">
+        <v>1.0286612192528072E-2</v>
+      </c>
+      <c r="J21">
+        <v>166.08333333333334</v>
+      </c>
+      <c r="K21" s="2">
+        <v>170.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="1">
+        <v>45266</v>
+      </c>
+      <c r="C22">
+        <v>249.5</v>
+      </c>
+      <c r="D22">
+        <v>5.4</v>
+      </c>
+      <c r="F22">
+        <v>0.21781349165461303</v>
+      </c>
+      <c r="G22">
+        <v>3.0473870842271603E-2</v>
+      </c>
+      <c r="H22">
+        <v>0.20528846153846153</v>
+      </c>
+      <c r="I22">
+        <v>3.5743400843100848E-2</v>
+      </c>
+      <c r="J22">
+        <v>182.61666666666667</v>
+      </c>
+      <c r="K22" s="2">
+        <v>167.28333333333333</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="1">
+        <v>45273</v>
+      </c>
+      <c r="C23">
+        <v>346.84210526315792</v>
+      </c>
+      <c r="D23">
+        <v>8.0526315789473681</v>
+      </c>
+      <c r="H23">
+        <v>0.30819838056680166</v>
+      </c>
+      <c r="I23">
+        <v>4.4581672466543681E-2</v>
+      </c>
+      <c r="J23">
+        <v>168.93333333333331</v>
+      </c>
+      <c r="K23" s="2">
+        <v>158.08333333333334</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="1">
+        <v>45274</v>
+      </c>
+      <c r="F24">
+        <v>0.45692237396557861</v>
+      </c>
+      <c r="G24">
+        <v>5.1146750325636835E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="1">
+        <v>45279</v>
+      </c>
+      <c r="C25">
+        <v>462</v>
+      </c>
+      <c r="D25">
+        <v>10.15</v>
+      </c>
+      <c r="E25">
+        <v>21.25</v>
+      </c>
+      <c r="F25">
+        <v>0.90377009469093894</v>
+      </c>
+      <c r="G25">
+        <v>0.17957612594849667</v>
+      </c>
+      <c r="H25">
+        <v>0.40192307692307694</v>
+      </c>
+      <c r="I25">
+        <v>5.4543711246622169E-2</v>
+      </c>
+      <c r="J25">
+        <v>158.51666666666665</v>
+      </c>
+      <c r="K25">
+        <v>137.65</v>
+      </c>
+      <c r="L25">
+        <v>60.377926120494841</v>
+      </c>
+      <c r="M25">
+        <v>47.44502885132195</v>
+      </c>
+      <c r="O25">
+        <v>107.82295497181678</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="1">
+        <v>45288</v>
+      </c>
+      <c r="C26">
+        <v>586.5</v>
+      </c>
+      <c r="D26">
+        <v>12.2</v>
+      </c>
+      <c r="F26">
+        <v>2.1000585963396539</v>
+      </c>
+      <c r="G26">
+        <v>0.16175497233014249</v>
+      </c>
+      <c r="H26">
+        <v>0.61923076923076925</v>
+      </c>
+      <c r="I26">
+        <v>5.8313123992568404E-2</v>
+      </c>
+      <c r="J26">
+        <v>183.81666666666663</v>
+      </c>
+      <c r="K26" s="2">
+        <v>185.81666666666663</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="1">
+        <v>45296</v>
+      </c>
+      <c r="C27">
+        <v>793</v>
+      </c>
+      <c r="E27">
+        <v>40</v>
+      </c>
+      <c r="F27">
+        <v>3.0317071477592523</v>
+      </c>
+      <c r="G27">
+        <v>0.33366923094714623</v>
+      </c>
+      <c r="H27">
+        <v>0.76298076923076918</v>
+      </c>
+      <c r="I27">
+        <v>7.3246859198435113E-2</v>
+      </c>
+      <c r="J27">
+        <v>174.58333333333334</v>
+      </c>
+      <c r="K27" s="2">
+        <v>149.88333333333335</v>
+      </c>
+      <c r="L27">
+        <v>143.94914186456293</v>
+      </c>
+      <c r="M27">
+        <v>181.99552389227946</v>
+      </c>
+      <c r="O27">
+        <v>325.94466575684237</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="1">
+        <v>45302</v>
+      </c>
+      <c r="C28">
+        <v>956.5</v>
+      </c>
+      <c r="D28">
+        <v>16.2</v>
+      </c>
+      <c r="H28">
+        <v>0.86442307692307696</v>
+      </c>
+      <c r="I28">
+        <v>5.5622450987683897E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="1">
+        <v>45306</v>
+      </c>
+      <c r="C29">
+        <v>1006</v>
+      </c>
+      <c r="H29">
+        <v>0.9259615384615385</v>
+      </c>
+      <c r="I29">
+        <v>4.7935013232664241E-2</v>
+      </c>
+      <c r="J29">
+        <v>133.11666666666665</v>
+      </c>
+      <c r="K29" s="2">
+        <v>100.80000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="1">
+        <v>45307</v>
+      </c>
+      <c r="D30">
+        <v>17</v>
+      </c>
+      <c r="E30">
+        <v>54.5</v>
+      </c>
+      <c r="F30">
+        <v>4.0425206810776277</v>
+      </c>
+      <c r="G30">
+        <v>0.37827040810057388</v>
+      </c>
+      <c r="L30">
+        <v>216.8302565533308</v>
+      </c>
+      <c r="M30">
+        <v>304.20829456947212</v>
+      </c>
+      <c r="N30">
+        <v>35.676835928243406</v>
+      </c>
+      <c r="O30">
+        <v>556.71538705104638</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="1">
+        <v>45314</v>
+      </c>
+      <c r="C31">
+        <v>1191.5</v>
+      </c>
+      <c r="D31">
+        <v>18.25</v>
+      </c>
+      <c r="H31">
+        <v>0.9802884615384615</v>
+      </c>
+      <c r="I31">
+        <v>6.4726008422452033E-2</v>
+      </c>
+      <c r="J31">
+        <v>150.83333333333334</v>
+      </c>
+      <c r="K31">
+        <v>119.81666666666666</v>
       </c>
     </row>
     <row r="1655" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Added new height data for 1-2-24
</commit_message>
<xml_diff>
--- a/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
+++ b/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Prototypes\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2661C39-2762-480F-9945-B52C647C247C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C956BF-F5FD-49FA-953D-9DD29E30F496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="CottonObserved" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CottonObserved!$A$1:$EP$2576</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CottonObserved!$A$1:$EP$2577</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="17">
   <si>
     <t>SimulationName</t>
   </si>
@@ -93,8 +93,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -122,10 +130,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,14 +449,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C911DF83-7300-4B7A-8A42-16858D40307A}">
-  <dimension ref="A1:O1655"/>
+  <dimension ref="A1:O1656"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="9970" ySplit="760" topLeftCell="I1" activePane="bottomRight"/>
+      <pane xSplit="9970" ySplit="760" topLeftCell="B1" activePane="bottomRight"/>
       <selection sqref="A1:A1048576"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="K31" sqref="K31"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -998,30 +1007,27 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1">
+        <v>45323</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B18" s="1">
         <v>45236</v>
       </c>
-      <c r="J17">
+      <c r="C18">
+        <v>1246.5</v>
+      </c>
+      <c r="J18">
         <v>93.333333333333329</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K18" s="2">
         <v>82.300000000000011</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="1">
-        <v>45243</v>
-      </c>
-      <c r="J18">
-        <v>104.5</v>
-      </c>
-      <c r="K18" s="2">
-        <v>135.1</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.45">
@@ -1029,13 +1035,13 @@
         <v>16</v>
       </c>
       <c r="B19" s="1">
-        <v>45248</v>
+        <v>45243</v>
       </c>
       <c r="J19">
-        <v>124.35000000000002</v>
+        <v>104.5</v>
       </c>
       <c r="K19" s="2">
-        <v>158.38333333333333</v>
+        <v>135.1</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.45">
@@ -1043,19 +1049,13 @@
         <v>16</v>
       </c>
       <c r="B20" s="1">
-        <v>45254</v>
-      </c>
-      <c r="C20">
-        <v>70</v>
-      </c>
-      <c r="D20">
-        <v>1.2</v>
+        <v>45248</v>
       </c>
       <c r="J20">
-        <v>158.5</v>
+        <v>124.35000000000002</v>
       </c>
       <c r="K20" s="2">
-        <v>170.91666666666666</v>
+        <v>158.38333333333333</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.45">
@@ -1063,25 +1063,19 @@
         <v>16</v>
       </c>
       <c r="B21" s="1">
-        <v>45259</v>
+        <v>45254</v>
       </c>
       <c r="C21">
-        <v>122.5</v>
+        <v>70</v>
       </c>
       <c r="D21">
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="F21">
-        <v>0.10798078444273128</v>
-      </c>
-      <c r="G21">
-        <v>1.0286612192528072E-2</v>
+        <v>1.2</v>
       </c>
       <c r="J21">
-        <v>166.08333333333334</v>
+        <v>158.5</v>
       </c>
       <c r="K21" s="2">
-        <v>170.3</v>
+        <v>170.91666666666666</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.45">
@@ -1089,31 +1083,25 @@
         <v>16</v>
       </c>
       <c r="B22" s="1">
-        <v>45266</v>
+        <v>45259</v>
       </c>
       <c r="C22">
-        <v>249.5</v>
+        <v>122.5</v>
       </c>
       <c r="D22">
-        <v>5.4</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="F22">
-        <v>0.21781349165461303</v>
+        <v>0.10798078444273128</v>
       </c>
       <c r="G22">
-        <v>3.0473870842271603E-2</v>
-      </c>
-      <c r="H22">
-        <v>0.20528846153846153</v>
-      </c>
-      <c r="I22">
-        <v>3.5743400843100848E-2</v>
+        <v>1.0286612192528072E-2</v>
       </c>
       <c r="J22">
-        <v>182.61666666666667</v>
+        <v>166.08333333333334</v>
       </c>
       <c r="K22" s="2">
-        <v>167.28333333333333</v>
+        <v>170.3</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.45">
@@ -1121,25 +1109,31 @@
         <v>16</v>
       </c>
       <c r="B23" s="1">
-        <v>45273</v>
+        <v>45266</v>
       </c>
       <c r="C23">
-        <v>346.84210526315792</v>
+        <v>249.5</v>
       </c>
       <c r="D23">
-        <v>8.0526315789473681</v>
+        <v>5.4</v>
+      </c>
+      <c r="F23">
+        <v>0.21781349165461303</v>
+      </c>
+      <c r="G23">
+        <v>3.0473870842271603E-2</v>
       </c>
       <c r="H23">
-        <v>0.30819838056680166</v>
+        <v>0.20528846153846153</v>
       </c>
       <c r="I23">
-        <v>4.4581672466543681E-2</v>
+        <v>3.5743400843100848E-2</v>
       </c>
       <c r="J23">
-        <v>168.93333333333331</v>
+        <v>182.61666666666667</v>
       </c>
       <c r="K23" s="2">
-        <v>158.08333333333334</v>
+        <v>167.28333333333333</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.45">
@@ -1147,13 +1141,25 @@
         <v>16</v>
       </c>
       <c r="B24" s="1">
-        <v>45274</v>
-      </c>
-      <c r="F24">
-        <v>0.45692237396557861</v>
-      </c>
-      <c r="G24">
-        <v>5.1146750325636835E-2</v>
+        <v>45273</v>
+      </c>
+      <c r="C24">
+        <v>346.84210526315792</v>
+      </c>
+      <c r="D24">
+        <v>8.0526315789473681</v>
+      </c>
+      <c r="H24">
+        <v>0.30819838056680166</v>
+      </c>
+      <c r="I24">
+        <v>4.4581672466543681E-2</v>
+      </c>
+      <c r="J24">
+        <v>168.93333333333331</v>
+      </c>
+      <c r="K24" s="2">
+        <v>158.08333333333334</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.45">
@@ -1161,43 +1167,13 @@
         <v>16</v>
       </c>
       <c r="B25" s="1">
-        <v>45279</v>
-      </c>
-      <c r="C25">
-        <v>462</v>
-      </c>
-      <c r="D25">
-        <v>10.15</v>
-      </c>
-      <c r="E25">
-        <v>21.25</v>
+        <v>45274</v>
       </c>
       <c r="F25">
-        <v>0.90377009469093894</v>
+        <v>0.45692237396557861</v>
       </c>
       <c r="G25">
-        <v>0.17957612594849667</v>
-      </c>
-      <c r="H25">
-        <v>0.40192307692307694</v>
-      </c>
-      <c r="I25">
-        <v>5.4543711246622169E-2</v>
-      </c>
-      <c r="J25">
-        <v>158.51666666666665</v>
-      </c>
-      <c r="K25">
-        <v>137.65</v>
-      </c>
-      <c r="L25">
-        <v>60.377926120494841</v>
-      </c>
-      <c r="M25">
-        <v>47.44502885132195</v>
-      </c>
-      <c r="O25">
-        <v>107.82295497181678</v>
+        <v>5.1146750325636835E-2</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.45">
@@ -1205,31 +1181,43 @@
         <v>16</v>
       </c>
       <c r="B26" s="1">
-        <v>45288</v>
+        <v>45279</v>
       </c>
       <c r="C26">
-        <v>586.5</v>
+        <v>462</v>
       </c>
       <c r="D26">
-        <v>12.2</v>
+        <v>10.15</v>
+      </c>
+      <c r="E26">
+        <v>21.25</v>
       </c>
       <c r="F26">
-        <v>2.1000585963396539</v>
+        <v>0.90377009469093894</v>
       </c>
       <c r="G26">
-        <v>0.16175497233014249</v>
+        <v>0.17957612594849667</v>
       </c>
       <c r="H26">
-        <v>0.61923076923076925</v>
+        <v>0.40192307692307694</v>
       </c>
       <c r="I26">
-        <v>5.8313123992568404E-2</v>
+        <v>5.4543711246622169E-2</v>
       </c>
       <c r="J26">
-        <v>183.81666666666663</v>
-      </c>
-      <c r="K26" s="2">
-        <v>185.81666666666663</v>
+        <v>158.51666666666665</v>
+      </c>
+      <c r="K26">
+        <v>137.65</v>
+      </c>
+      <c r="L26">
+        <v>60.377926120494841</v>
+      </c>
+      <c r="M26">
+        <v>47.44502885132195</v>
+      </c>
+      <c r="O26">
+        <v>107.82295497181678</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.45">
@@ -1237,40 +1225,31 @@
         <v>16</v>
       </c>
       <c r="B27" s="1">
-        <v>45296</v>
+        <v>45288</v>
       </c>
       <c r="C27">
-        <v>793</v>
-      </c>
-      <c r="E27">
-        <v>40</v>
+        <v>586.5</v>
+      </c>
+      <c r="D27">
+        <v>12.2</v>
       </c>
       <c r="F27">
-        <v>3.0317071477592523</v>
+        <v>2.1000585963396539</v>
       </c>
       <c r="G27">
-        <v>0.33366923094714623</v>
+        <v>0.16175497233014249</v>
       </c>
       <c r="H27">
-        <v>0.76298076923076918</v>
+        <v>0.61923076923076925</v>
       </c>
       <c r="I27">
-        <v>7.3246859198435113E-2</v>
+        <v>5.8313123992568404E-2</v>
       </c>
       <c r="J27">
-        <v>174.58333333333334</v>
+        <v>183.81666666666663</v>
       </c>
       <c r="K27" s="2">
-        <v>149.88333333333335</v>
-      </c>
-      <c r="L27">
-        <v>143.94914186456293</v>
-      </c>
-      <c r="M27">
-        <v>181.99552389227946</v>
-      </c>
-      <c r="O27">
-        <v>325.94466575684237</v>
+        <v>185.81666666666663</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.45">
@@ -1278,19 +1257,40 @@
         <v>16</v>
       </c>
       <c r="B28" s="1">
-        <v>45302</v>
+        <v>45296</v>
       </c>
       <c r="C28">
-        <v>956.5</v>
-      </c>
-      <c r="D28">
-        <v>16.2</v>
+        <v>793</v>
+      </c>
+      <c r="E28">
+        <v>40</v>
+      </c>
+      <c r="F28">
+        <v>3.0317071477592523</v>
+      </c>
+      <c r="G28">
+        <v>0.33366923094714623</v>
       </c>
       <c r="H28">
-        <v>0.86442307692307696</v>
+        <v>0.76298076923076918</v>
       </c>
       <c r="I28">
-        <v>5.5622450987683897E-2</v>
+        <v>7.3246859198435113E-2</v>
+      </c>
+      <c r="J28">
+        <v>174.58333333333334</v>
+      </c>
+      <c r="K28" s="2">
+        <v>149.88333333333335</v>
+      </c>
+      <c r="L28">
+        <v>143.94914186456293</v>
+      </c>
+      <c r="M28">
+        <v>181.99552389227946</v>
+      </c>
+      <c r="O28">
+        <v>325.94466575684237</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.45">
@@ -1298,22 +1298,19 @@
         <v>16</v>
       </c>
       <c r="B29" s="1">
-        <v>45306</v>
+        <v>45302</v>
       </c>
       <c r="C29">
-        <v>1006</v>
+        <v>956.5</v>
+      </c>
+      <c r="D29">
+        <v>16.2</v>
       </c>
       <c r="H29">
-        <v>0.9259615384615385</v>
+        <v>0.86442307692307696</v>
       </c>
       <c r="I29">
-        <v>4.7935013232664241E-2</v>
-      </c>
-      <c r="J29">
-        <v>133.11666666666665</v>
-      </c>
-      <c r="K29" s="2">
-        <v>100.80000000000001</v>
+        <v>5.5622450987683897E-2</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.45">
@@ -1321,31 +1318,22 @@
         <v>16</v>
       </c>
       <c r="B30" s="1">
-        <v>45307</v>
-      </c>
-      <c r="D30">
-        <v>17</v>
-      </c>
-      <c r="E30">
-        <v>54.5</v>
-      </c>
-      <c r="F30">
-        <v>4.0425206810776277</v>
-      </c>
-      <c r="G30">
-        <v>0.37827040810057388</v>
-      </c>
-      <c r="L30">
-        <v>216.8302565533308</v>
-      </c>
-      <c r="M30">
-        <v>304.20829456947212</v>
-      </c>
-      <c r="N30">
-        <v>35.676835928243406</v>
-      </c>
-      <c r="O30">
-        <v>556.71538705104638</v>
+        <v>45306</v>
+      </c>
+      <c r="C30">
+        <v>1006</v>
+      </c>
+      <c r="H30">
+        <v>0.9259615384615385</v>
+      </c>
+      <c r="I30">
+        <v>4.7935013232664241E-2</v>
+      </c>
+      <c r="J30">
+        <v>133.11666666666665</v>
+      </c>
+      <c r="K30" s="2">
+        <v>100.80000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.45">
@@ -1353,32 +1341,64 @@
         <v>16</v>
       </c>
       <c r="B31" s="1">
+        <v>45307</v>
+      </c>
+      <c r="D31">
+        <v>17</v>
+      </c>
+      <c r="E31">
+        <v>54.5</v>
+      </c>
+      <c r="F31">
+        <v>4.0425206810776277</v>
+      </c>
+      <c r="G31">
+        <v>0.37827040810057388</v>
+      </c>
+      <c r="L31">
+        <v>216.8302565533308</v>
+      </c>
+      <c r="M31">
+        <v>304.20829456947212</v>
+      </c>
+      <c r="N31">
+        <v>35.676835928243406</v>
+      </c>
+      <c r="O31">
+        <v>556.71538705104638</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="1">
         <v>45314</v>
       </c>
-      <c r="C31">
+      <c r="C32">
         <v>1191.5</v>
       </c>
-      <c r="D31">
+      <c r="D32">
         <v>18.25</v>
       </c>
-      <c r="H31">
+      <c r="H32">
         <v>0.9802884615384615</v>
       </c>
-      <c r="I31">
+      <c r="I32">
         <v>6.4726008422452033E-2</v>
       </c>
-      <c r="J31">
+      <c r="J32">
         <v>150.83333333333334</v>
       </c>
-      <c r="K31">
+      <c r="K32">
         <v>119.81666666666666</v>
       </c>
     </row>
-    <row r="1655" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="1656" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1633:EP1812">
-    <sortCondition ref="B2:B2263"/>
-    <sortCondition ref="C2:C2263"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1634:EP1813">
+    <sortCondition ref="B2:B2264"/>
+    <sortCondition ref="C2:C2264"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated lai, cover and node number data
</commit_message>
<xml_diff>
--- a/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
+++ b/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Prototypes\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C956BF-F5FD-49FA-953D-9DD29E30F496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B319DC19-8BAB-4E9D-8042-9AECCA0BB8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
@@ -452,11 +452,11 @@
   <dimension ref="A1:O1656"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="9970" ySplit="760" topLeftCell="B1" activePane="bottomRight"/>
+      <pane xSplit="9970" ySplit="760" topLeftCell="G1" activePane="bottomRight"/>
       <selection sqref="A1:A1048576"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomRight" activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1023,6 +1023,24 @@
       <c r="C18">
         <v>1246.5</v>
       </c>
+      <c r="D18">
+        <v>19.649999999999999</v>
+      </c>
+      <c r="E18">
+        <v>66.849999999999994</v>
+      </c>
+      <c r="F18">
+        <v>5.312378794687266</v>
+      </c>
+      <c r="G18">
+        <v>0.32232021196016941</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0.98990384615384619</v>
+      </c>
+      <c r="I18">
+        <v>6.3817475023250456E-2</v>
+      </c>
       <c r="J18">
         <v>93.333333333333329</v>
       </c>

</xml_diff>

<commit_message>
Updated with data from 1-Feb
</commit_message>
<xml_diff>
--- a/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
+++ b/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Prototypes\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B319DC19-8BAB-4E9D-8042-9AECCA0BB8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D93209-E269-4DE5-A070-06175756E958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="17">
   <si>
     <t>SimulationName</t>
   </si>
@@ -93,16 +93,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -134,7 +126,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,11 +444,11 @@
   <dimension ref="A1:O1656"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="9970" ySplit="760" topLeftCell="G1" activePane="bottomRight"/>
+      <pane xSplit="9970" ySplit="760" activePane="bottomLeft"/>
       <selection sqref="A1:A1048576"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
-      <selection pane="bottomRight" activeCell="L18" sqref="L18"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1012,6 +1004,33 @@
       <c r="B17" s="1">
         <v>45323</v>
       </c>
+      <c r="C17">
+        <v>1246.5</v>
+      </c>
+      <c r="D17">
+        <v>19.649999999999999</v>
+      </c>
+      <c r="E17">
+        <v>66.849999999999994</v>
+      </c>
+      <c r="F17">
+        <v>5.312378794687266</v>
+      </c>
+      <c r="G17">
+        <v>0.32232021196016941</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0.98990384615384619</v>
+      </c>
+      <c r="I17">
+        <v>6.3817475023250456E-2</v>
+      </c>
+      <c r="J17">
+        <v>204.26666666666665</v>
+      </c>
+      <c r="K17" s="2">
+        <v>180.61666666666667</v>
+      </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
@@ -1020,27 +1039,6 @@
       <c r="B18" s="1">
         <v>45236</v>
       </c>
-      <c r="C18">
-        <v>1246.5</v>
-      </c>
-      <c r="D18">
-        <v>19.649999999999999</v>
-      </c>
-      <c r="E18">
-        <v>66.849999999999994</v>
-      </c>
-      <c r="F18">
-        <v>5.312378794687266</v>
-      </c>
-      <c r="G18">
-        <v>0.32232021196016941</v>
-      </c>
-      <c r="H18" s="2">
-        <v>0.98990384615384619</v>
-      </c>
-      <c r="I18">
-        <v>6.3817475023250456E-2</v>
-      </c>
       <c r="J18">
         <v>93.333333333333329</v>
       </c>
@@ -1410,6 +1408,20 @@
       </c>
       <c r="K32">
         <v>119.81666666666666</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="1">
+        <v>45323</v>
+      </c>
+      <c r="J33">
+        <v>188.48333333333335</v>
+      </c>
+      <c r="K33">
+        <v>172.45000000000005</v>
       </c>
     </row>
     <row r="1656" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Added data from Feb 9
</commit_message>
<xml_diff>
--- a/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
+++ b/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Prototypes\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D93209-E269-4DE5-A070-06175756E958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B072ED1D-724E-43E1-975C-28D5A6D4D8DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="CottonObserved" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CottonObserved!$A$1:$EP$2577</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CottonObserved!$A$1:$EP$2578</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="17">
   <si>
     <t>SimulationName</t>
   </si>
@@ -122,11 +122,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -145,9 +144,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -185,7 +184,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -291,7 +290,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -433,7 +432,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -441,14 +440,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C911DF83-7300-4B7A-8A42-16858D40307A}">
-  <dimension ref="A1:O1656"/>
+  <dimension ref="A1:O1657"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="9970" ySplit="760" activePane="bottomLeft"/>
+      <pane xSplit="9970" ySplit="760" topLeftCell="F11" activePane="bottomRight"/>
       <selection sqref="A1:A1048576"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
+      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1033,17 +1032,24 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A18" s="3" t="s">
-        <v>16</v>
+      <c r="A18" t="s">
+        <v>15</v>
       </c>
       <c r="B18" s="1">
-        <v>45236</v>
-      </c>
-      <c r="J18">
-        <v>93.333333333333329</v>
+        <v>45331</v>
+      </c>
+      <c r="F18">
+        <v>5.8926489999999996</v>
+      </c>
+      <c r="G18">
+        <v>0.16848393942648088</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="J18" s="2">
+        <v>175.71666666666667</v>
       </c>
       <c r="K18" s="2">
-        <v>82.300000000000011</v>
+        <v>124.45</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.45">
@@ -1051,13 +1057,13 @@
         <v>16</v>
       </c>
       <c r="B19" s="1">
-        <v>45243</v>
+        <v>45236</v>
       </c>
       <c r="J19">
-        <v>104.5</v>
+        <v>93.333333333333329</v>
       </c>
       <c r="K19" s="2">
-        <v>135.1</v>
+        <v>82.300000000000011</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.45">
@@ -1065,13 +1071,13 @@
         <v>16</v>
       </c>
       <c r="B20" s="1">
-        <v>45248</v>
+        <v>45243</v>
       </c>
       <c r="J20">
-        <v>124.35000000000002</v>
+        <v>104.5</v>
       </c>
       <c r="K20" s="2">
-        <v>158.38333333333333</v>
+        <v>135.1</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.45">
@@ -1079,19 +1085,13 @@
         <v>16</v>
       </c>
       <c r="B21" s="1">
-        <v>45254</v>
-      </c>
-      <c r="C21">
-        <v>70</v>
-      </c>
-      <c r="D21">
-        <v>1.2</v>
+        <v>45248</v>
       </c>
       <c r="J21">
-        <v>158.5</v>
+        <v>124.35000000000002</v>
       </c>
       <c r="K21" s="2">
-        <v>170.91666666666666</v>
+        <v>158.38333333333333</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.45">
@@ -1099,25 +1099,19 @@
         <v>16</v>
       </c>
       <c r="B22" s="1">
-        <v>45259</v>
+        <v>45254</v>
       </c>
       <c r="C22">
-        <v>122.5</v>
+        <v>70</v>
       </c>
       <c r="D22">
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="F22">
-        <v>0.10798078444273128</v>
-      </c>
-      <c r="G22">
-        <v>1.0286612192528072E-2</v>
+        <v>1.2</v>
       </c>
       <c r="J22">
-        <v>166.08333333333334</v>
+        <v>158.5</v>
       </c>
       <c r="K22" s="2">
-        <v>170.3</v>
+        <v>170.91666666666666</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.45">
@@ -1125,31 +1119,25 @@
         <v>16</v>
       </c>
       <c r="B23" s="1">
-        <v>45266</v>
+        <v>45259</v>
       </c>
       <c r="C23">
-        <v>249.5</v>
+        <v>122.5</v>
       </c>
       <c r="D23">
-        <v>5.4</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="F23">
-        <v>0.21781349165461303</v>
+        <v>0.10798078444273128</v>
       </c>
       <c r="G23">
-        <v>3.0473870842271603E-2</v>
-      </c>
-      <c r="H23">
-        <v>0.20528846153846153</v>
-      </c>
-      <c r="I23">
-        <v>3.5743400843100848E-2</v>
+        <v>1.0286612192528072E-2</v>
       </c>
       <c r="J23">
-        <v>182.61666666666667</v>
+        <v>166.08333333333334</v>
       </c>
       <c r="K23" s="2">
-        <v>167.28333333333333</v>
+        <v>170.3</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.45">
@@ -1157,25 +1145,31 @@
         <v>16</v>
       </c>
       <c r="B24" s="1">
-        <v>45273</v>
+        <v>45266</v>
       </c>
       <c r="C24">
-        <v>346.84210526315792</v>
+        <v>249.5</v>
       </c>
       <c r="D24">
-        <v>8.0526315789473681</v>
+        <v>5.4</v>
+      </c>
+      <c r="F24">
+        <v>0.21781349165461303</v>
+      </c>
+      <c r="G24">
+        <v>3.0473870842271603E-2</v>
       </c>
       <c r="H24">
-        <v>0.30819838056680166</v>
+        <v>0.20528846153846153</v>
       </c>
       <c r="I24">
-        <v>4.4581672466543681E-2</v>
+        <v>3.5743400843100848E-2</v>
       </c>
       <c r="J24">
-        <v>168.93333333333331</v>
+        <v>182.61666666666667</v>
       </c>
       <c r="K24" s="2">
-        <v>158.08333333333334</v>
+        <v>167.28333333333333</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.45">
@@ -1183,13 +1177,25 @@
         <v>16</v>
       </c>
       <c r="B25" s="1">
-        <v>45274</v>
-      </c>
-      <c r="F25">
-        <v>0.45692237396557861</v>
-      </c>
-      <c r="G25">
-        <v>5.1146750325636835E-2</v>
+        <v>45273</v>
+      </c>
+      <c r="C25">
+        <v>346.84210526315792</v>
+      </c>
+      <c r="D25">
+        <v>8.0526315789473681</v>
+      </c>
+      <c r="H25">
+        <v>0.30819838056680166</v>
+      </c>
+      <c r="I25">
+        <v>4.4581672466543681E-2</v>
+      </c>
+      <c r="J25">
+        <v>168.93333333333331</v>
+      </c>
+      <c r="K25" s="2">
+        <v>158.08333333333334</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.45">
@@ -1197,43 +1203,13 @@
         <v>16</v>
       </c>
       <c r="B26" s="1">
-        <v>45279</v>
-      </c>
-      <c r="C26">
-        <v>462</v>
-      </c>
-      <c r="D26">
-        <v>10.15</v>
-      </c>
-      <c r="E26">
-        <v>21.25</v>
+        <v>45274</v>
       </c>
       <c r="F26">
-        <v>0.90377009469093894</v>
+        <v>0.45692237396557861</v>
       </c>
       <c r="G26">
-        <v>0.17957612594849667</v>
-      </c>
-      <c r="H26">
-        <v>0.40192307692307694</v>
-      </c>
-      <c r="I26">
-        <v>5.4543711246622169E-2</v>
-      </c>
-      <c r="J26">
-        <v>158.51666666666665</v>
-      </c>
-      <c r="K26">
-        <v>137.65</v>
-      </c>
-      <c r="L26">
-        <v>60.377926120494841</v>
-      </c>
-      <c r="M26">
-        <v>47.44502885132195</v>
-      </c>
-      <c r="O26">
-        <v>107.82295497181678</v>
+        <v>5.1146750325636835E-2</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.45">
@@ -1241,31 +1217,43 @@
         <v>16</v>
       </c>
       <c r="B27" s="1">
-        <v>45288</v>
+        <v>45279</v>
       </c>
       <c r="C27">
-        <v>586.5</v>
+        <v>462</v>
       </c>
       <c r="D27">
-        <v>12.2</v>
+        <v>10.15</v>
+      </c>
+      <c r="E27">
+        <v>21.25</v>
       </c>
       <c r="F27">
-        <v>2.1000585963396539</v>
+        <v>0.90377009469093894</v>
       </c>
       <c r="G27">
-        <v>0.16175497233014249</v>
+        <v>0.17957612594849667</v>
       </c>
       <c r="H27">
-        <v>0.61923076923076925</v>
+        <v>0.40192307692307694</v>
       </c>
       <c r="I27">
-        <v>5.8313123992568404E-2</v>
+        <v>5.4543711246622169E-2</v>
       </c>
       <c r="J27">
-        <v>183.81666666666663</v>
-      </c>
-      <c r="K27" s="2">
-        <v>185.81666666666663</v>
+        <v>158.51666666666665</v>
+      </c>
+      <c r="K27">
+        <v>137.65</v>
+      </c>
+      <c r="L27">
+        <v>60.377926120494841</v>
+      </c>
+      <c r="M27">
+        <v>47.44502885132195</v>
+      </c>
+      <c r="O27">
+        <v>107.82295497181678</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.45">
@@ -1273,40 +1261,31 @@
         <v>16</v>
       </c>
       <c r="B28" s="1">
-        <v>45296</v>
+        <v>45288</v>
       </c>
       <c r="C28">
-        <v>793</v>
-      </c>
-      <c r="E28">
-        <v>40</v>
+        <v>586.5</v>
+      </c>
+      <c r="D28">
+        <v>12.2</v>
       </c>
       <c r="F28">
-        <v>3.0317071477592523</v>
+        <v>2.1000585963396539</v>
       </c>
       <c r="G28">
-        <v>0.33366923094714623</v>
+        <v>0.16175497233014249</v>
       </c>
       <c r="H28">
-        <v>0.76298076923076918</v>
+        <v>0.61923076923076925</v>
       </c>
       <c r="I28">
-        <v>7.3246859198435113E-2</v>
+        <v>5.8313123992568404E-2</v>
       </c>
       <c r="J28">
-        <v>174.58333333333334</v>
+        <v>183.81666666666663</v>
       </c>
       <c r="K28" s="2">
-        <v>149.88333333333335</v>
-      </c>
-      <c r="L28">
-        <v>143.94914186456293</v>
-      </c>
-      <c r="M28">
-        <v>181.99552389227946</v>
-      </c>
-      <c r="O28">
-        <v>325.94466575684237</v>
+        <v>185.81666666666663</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.45">
@@ -1314,19 +1293,40 @@
         <v>16</v>
       </c>
       <c r="B29" s="1">
-        <v>45302</v>
+        <v>45296</v>
       </c>
       <c r="C29">
-        <v>956.5</v>
-      </c>
-      <c r="D29">
-        <v>16.2</v>
+        <v>793</v>
+      </c>
+      <c r="E29">
+        <v>40</v>
+      </c>
+      <c r="F29">
+        <v>3.0317071477592523</v>
+      </c>
+      <c r="G29">
+        <v>0.33366923094714623</v>
       </c>
       <c r="H29">
-        <v>0.86442307692307696</v>
+        <v>0.76298076923076918</v>
       </c>
       <c r="I29">
-        <v>5.5622450987683897E-2</v>
+        <v>7.3246859198435113E-2</v>
+      </c>
+      <c r="J29">
+        <v>174.58333333333334</v>
+      </c>
+      <c r="K29" s="2">
+        <v>149.88333333333335</v>
+      </c>
+      <c r="L29">
+        <v>143.94914186456293</v>
+      </c>
+      <c r="M29">
+        <v>181.99552389227946</v>
+      </c>
+      <c r="O29">
+        <v>325.94466575684237</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.45">
@@ -1334,22 +1334,19 @@
         <v>16</v>
       </c>
       <c r="B30" s="1">
-        <v>45306</v>
+        <v>45302</v>
       </c>
       <c r="C30">
-        <v>1006</v>
+        <v>956.5</v>
+      </c>
+      <c r="D30">
+        <v>16.2</v>
       </c>
       <c r="H30">
-        <v>0.9259615384615385</v>
+        <v>0.86442307692307696</v>
       </c>
       <c r="I30">
-        <v>4.7935013232664241E-2</v>
-      </c>
-      <c r="J30">
-        <v>133.11666666666665</v>
-      </c>
-      <c r="K30" s="2">
-        <v>100.80000000000001</v>
+        <v>5.5622450987683897E-2</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.45">
@@ -1357,31 +1354,22 @@
         <v>16</v>
       </c>
       <c r="B31" s="1">
-        <v>45307</v>
-      </c>
-      <c r="D31">
-        <v>17</v>
-      </c>
-      <c r="E31">
-        <v>54.5</v>
-      </c>
-      <c r="F31">
-        <v>4.0425206810776277</v>
-      </c>
-      <c r="G31">
-        <v>0.37827040810057388</v>
-      </c>
-      <c r="L31">
-        <v>216.8302565533308</v>
-      </c>
-      <c r="M31">
-        <v>304.20829456947212</v>
-      </c>
-      <c r="N31">
-        <v>35.676835928243406</v>
-      </c>
-      <c r="O31">
-        <v>556.71538705104638</v>
+        <v>45306</v>
+      </c>
+      <c r="C31">
+        <v>1006</v>
+      </c>
+      <c r="H31">
+        <v>0.9259615384615385</v>
+      </c>
+      <c r="I31">
+        <v>4.7935013232664241E-2</v>
+      </c>
+      <c r="J31">
+        <v>133.11666666666665</v>
+      </c>
+      <c r="K31" s="2">
+        <v>100.80000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.45">
@@ -1389,25 +1377,31 @@
         <v>16</v>
       </c>
       <c r="B32" s="1">
-        <v>45314</v>
-      </c>
-      <c r="C32">
-        <v>1191.5</v>
+        <v>45307</v>
       </c>
       <c r="D32">
-        <v>18.25</v>
-      </c>
-      <c r="H32">
-        <v>0.9802884615384615</v>
-      </c>
-      <c r="I32">
-        <v>6.4726008422452033E-2</v>
-      </c>
-      <c r="J32">
-        <v>150.83333333333334</v>
-      </c>
-      <c r="K32">
-        <v>119.81666666666666</v>
+        <v>17</v>
+      </c>
+      <c r="E32">
+        <v>54.5</v>
+      </c>
+      <c r="F32">
+        <v>4.0425206810776277</v>
+      </c>
+      <c r="G32">
+        <v>0.37827040810057388</v>
+      </c>
+      <c r="L32">
+        <v>216.8302565533308</v>
+      </c>
+      <c r="M32">
+        <v>304.20829456947212</v>
+      </c>
+      <c r="N32">
+        <v>35.676835928243406</v>
+      </c>
+      <c r="O32">
+        <v>556.71538705104638</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.45">
@@ -1415,20 +1409,66 @@
         <v>16</v>
       </c>
       <c r="B33" s="1">
+        <v>45314</v>
+      </c>
+      <c r="C33">
+        <v>1191.5</v>
+      </c>
+      <c r="D33">
+        <v>18.25</v>
+      </c>
+      <c r="H33">
+        <v>0.9802884615384615</v>
+      </c>
+      <c r="I33">
+        <v>6.4726008422452033E-2</v>
+      </c>
+      <c r="J33">
+        <v>150.83333333333334</v>
+      </c>
+      <c r="K33">
+        <v>119.81666666666666</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="1">
         <v>45323</v>
       </c>
-      <c r="J33">
+      <c r="J34">
         <v>188.48333333333335</v>
       </c>
-      <c r="K33">
+      <c r="K34">
         <v>172.45000000000005</v>
       </c>
     </row>
-    <row r="1656" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="1">
+        <v>45331</v>
+      </c>
+      <c r="F35">
+        <v>5.5032705000000002</v>
+      </c>
+      <c r="G35">
+        <v>1.6615774246742543E-2</v>
+      </c>
+      <c r="J35">
+        <v>165.13333333333333</v>
+      </c>
+      <c r="K35">
+        <v>133.63333333333333</v>
+      </c>
+    </row>
+    <row r="1657" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1634:EP1813">
-    <sortCondition ref="B2:B2264"/>
-    <sortCondition ref="C2:C2264"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1635:EP1814">
+    <sortCondition ref="B2:B2265"/>
+    <sortCondition ref="C2:C2265"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated to simulate to 9-feb
</commit_message>
<xml_diff>
--- a/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
+++ b/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Prototypes\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B072ED1D-724E-43E1-975C-28D5A6D4D8DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030C81E5-E649-43B8-BA46-C88151F75A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="CottonObserved" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CottonObserved!$A$1:$EP$2578</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CottonObserved!$A$1:$EQ$2578</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="18">
   <si>
     <t>SimulationName</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>ForestHill2023IrrigationPartial</t>
+  </si>
+  <si>
+    <t>Cotton.Leaf.SpecificArea</t>
   </si>
 </sst>
 </file>
@@ -440,14 +443,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C911DF83-7300-4B7A-8A42-16858D40307A}">
-  <dimension ref="A1:O1657"/>
+  <dimension ref="A1:P1657"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="9970" ySplit="760" topLeftCell="F11" activePane="bottomRight"/>
+      <pane xSplit="9970" ySplit="760" topLeftCell="H11" activePane="bottomRight"/>
       <selection sqref="A1:A1048576"/>
-      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
-      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomRight" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -456,131 +459,131 @@
     <col min="2" max="2" width="24.265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.3984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="25.73046875" customWidth="1"/>
-    <col min="10" max="10" width="38.1328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.06640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="36.265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.3984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="33.3984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.3984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.86328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="27.1328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="34.3984375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="32.3984375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="33.59765625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="30.265625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="34.1328125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="31.86328125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="35.59765625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16.265625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="18" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="21.1328125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16.73046875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="17.86328125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="24.73046875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="20.73046875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="26" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="24.86328125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="27.3984375" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="16.73046875" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="17.265625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="33.265625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="32.3984375" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="32.86328125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="7.73046875" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="7.1328125" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="69" max="70" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="74" max="75" width="14.1328125" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="23" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="23" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="23" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="23" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="23" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="23" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="23" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="23" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="23" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="24" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="24" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="24" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="19" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="19" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="19" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="19" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="19" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="19" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="19" bestFit="1" customWidth="1"/>
-    <col min="127" max="127" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="19" bestFit="1" customWidth="1"/>
-    <col min="129" max="129" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="130" max="137" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="138" max="138" width="6.1328125" bestFit="1" customWidth="1"/>
-    <col min="139" max="146" width="24.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="10" width="25.73046875" customWidth="1"/>
+    <col min="11" max="11" width="38.1328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.06640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="36.265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.3984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="33.3984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.3984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.86328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.1328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="34.3984375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="32.3984375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="33.59765625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="30.265625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="34.1328125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="31.86328125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="35.59765625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.1328125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="18" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="21.1328125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="16.73046875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="24.73046875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.1328125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="17.59765625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="20.73046875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="26" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="24.86328125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="27.3984375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="16.73046875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="14.73046875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="17.265625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="33.265625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="32.3984375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="32.86328125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="14.73046875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="7.1328125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="16.1328125" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="70" max="71" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="17.59765625" bestFit="1" customWidth="1"/>
+    <col min="75" max="76" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="23" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="23" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="23" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="23" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="23" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="23" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="23" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="23" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="23" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="24" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="24" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="24" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="7.59765625" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="19" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="19" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="19" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="19" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="19" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="19" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="19" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="19" bestFit="1" customWidth="1"/>
+    <col min="130" max="130" width="7.59765625" bestFit="1" customWidth="1"/>
+    <col min="131" max="138" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="139" max="139" width="6.1328125" bestFit="1" customWidth="1"/>
+    <col min="140" max="147" width="24.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -603,73 +606,76 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>4</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="1">
         <v>45236</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>105.68333333333334</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>96.683333333333337</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="1">
         <v>45243</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>120.93333333333334</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>139.43333333333331</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="1">
         <v>45248</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>144.7833333333333</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>162.56666666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -682,14 +688,14 @@
       <c r="D5">
         <v>1.45</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>163.91666666666666</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>183.21666666666667</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -708,14 +714,14 @@
       <c r="G6">
         <v>2.4123522851920851E-2</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>178.29999999999998</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>172.93333333333331</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -734,20 +740,20 @@
       <c r="G7">
         <v>1.3732764172807894E-2</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>0.19663461538461538</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>3.5770618361488406E-2</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>178.16666666666666</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>192.94999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -763,20 +769,20 @@
       <c r="G8">
         <v>3.605272908788857E-2</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>0.27596153846153848</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>4.7629496970109417E-2</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>182.6</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>161.20000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -790,7 +796,7 @@
         <v>3.605272908788857E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -812,29 +818,29 @@
       <c r="G10">
         <v>0.14620537270042952</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>0.41602564102564105</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>4.632333044943851E-2</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>176.85714285714286</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>142.31428571428572</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>61.869882044725493</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>47.219165425471701</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>109.08904747019719</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -847,14 +853,14 @@
       <c r="G11">
         <v>4.1026933330751199E-2</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>198.48333333333335</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>190.58333333333337</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -874,28 +880,32 @@
         <v>7.4730791031138666E-2</v>
       </c>
       <c r="H12">
+        <f>F12/M12</f>
+        <v>1.9955521573186027E-2</v>
+      </c>
+      <c r="I12">
         <v>0.75</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>8.4403488823438802E-2</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>195.43333333333337</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>145.15</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>148.32379686792672</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>182.30627017799995</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>330.63006704592664</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -908,14 +918,14 @@
       <c r="D13">
         <v>16.3</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>0.92307692307692313</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>0.10013140610136738</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -925,20 +935,20 @@
       <c r="C14">
         <v>1014</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>0.9028846153846154</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>7.0723752109358815E-2</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>158.63333333333333</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>104.5</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -957,20 +967,24 @@
       <c r="G15">
         <v>0.46875655267478084</v>
       </c>
-      <c r="L15">
+      <c r="H15">
+        <f>F15/M15</f>
+        <v>1.8194598470576563E-2</v>
+      </c>
+      <c r="M15">
         <v>235.61860053445332</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>329.13664247461998</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>39.927173460593856</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>604.68241646966715</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -983,20 +997,20 @@
       <c r="D16">
         <v>18.149999999999999</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>0.98701923076923082</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>7.2646492320450506E-2</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>202.79999999999998</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>173.93333333333331</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1018,20 +1032,20 @@
       <c r="G17">
         <v>0.32232021196016941</v>
       </c>
-      <c r="H17" s="2">
+      <c r="I17" s="2">
         <v>0.98990384615384619</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>6.3817475023250456E-2</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>204.26666666666665</v>
       </c>
-      <c r="K17" s="2">
+      <c r="L17" s="2">
         <v>180.61666666666667</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1044,57 +1058,67 @@
       <c r="G18">
         <v>0.16848393942648088</v>
       </c>
-      <c r="H18" s="2"/>
-      <c r="J18" s="2">
+      <c r="H18">
+        <f>F18/M18</f>
+        <v>2.0823552901265103E-2</v>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="K18" s="2">
         <v>175.71666666666667</v>
       </c>
-      <c r="K18" s="2">
+      <c r="L18" s="2">
         <v>124.45</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M18">
+        <v>282.98</v>
+      </c>
+      <c r="N18" s="2">
+        <v>425.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="1">
         <v>45236</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>93.333333333333329</v>
       </c>
-      <c r="K19" s="2">
+      <c r="L19" s="2">
         <v>82.300000000000011</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="1">
         <v>45243</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>104.5</v>
       </c>
-      <c r="K20" s="2">
+      <c r="L20" s="2">
         <v>135.1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="1">
         <v>45248</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>124.35000000000002</v>
       </c>
-      <c r="K21" s="2">
+      <c r="L21" s="2">
         <v>158.38333333333333</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -1107,14 +1131,14 @@
       <c r="D22">
         <v>1.2</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>158.5</v>
       </c>
-      <c r="K22" s="2">
+      <c r="L22" s="2">
         <v>170.91666666666666</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -1133,14 +1157,14 @@
       <c r="G23">
         <v>1.0286612192528072E-2</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>166.08333333333334</v>
       </c>
-      <c r="K23" s="2">
+      <c r="L23" s="2">
         <v>170.3</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -1159,20 +1183,20 @@
       <c r="G24">
         <v>3.0473870842271603E-2</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>0.20528846153846153</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>3.5743400843100848E-2</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>182.61666666666667</v>
       </c>
-      <c r="K24" s="2">
+      <c r="L24" s="2">
         <v>167.28333333333333</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -1185,20 +1209,20 @@
       <c r="D25">
         <v>8.0526315789473681</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>0.30819838056680166</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>4.4581672466543681E-2</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>168.93333333333331</v>
       </c>
-      <c r="K25" s="2">
+      <c r="L25" s="2">
         <v>158.08333333333334</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -1212,7 +1236,7 @@
         <v>5.1146750325636835E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -1235,28 +1259,32 @@
         <v>0.17957612594849667</v>
       </c>
       <c r="H27">
+        <f>F27/M27</f>
+        <v>1.4968551468417543E-2</v>
+      </c>
+      <c r="I27">
         <v>0.40192307692307694</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>5.4543711246622169E-2</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <v>158.51666666666665</v>
       </c>
-      <c r="K27">
+      <c r="L27">
         <v>137.65</v>
       </c>
-      <c r="L27">
+      <c r="M27">
         <v>60.377926120494841</v>
       </c>
-      <c r="M27">
+      <c r="N27">
         <v>47.44502885132195</v>
       </c>
-      <c r="O27">
+      <c r="P27">
         <v>107.82295497181678</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -1275,20 +1303,20 @@
       <c r="G28">
         <v>0.16175497233014249</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>0.61923076923076925</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>5.8313123992568404E-2</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <v>183.81666666666663</v>
       </c>
-      <c r="K28" s="2">
+      <c r="L28" s="2">
         <v>185.81666666666663</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -1308,28 +1336,32 @@
         <v>0.33366923094714623</v>
       </c>
       <c r="H29">
+        <f>F29/M29</f>
+        <v>2.1060960200872104E-2</v>
+      </c>
+      <c r="I29">
         <v>0.76298076923076918</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>7.3246859198435113E-2</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <v>174.58333333333334</v>
       </c>
-      <c r="K29" s="2">
+      <c r="L29" s="2">
         <v>149.88333333333335</v>
       </c>
-      <c r="L29">
+      <c r="M29">
         <v>143.94914186456293</v>
       </c>
-      <c r="M29">
+      <c r="N29">
         <v>181.99552389227946</v>
       </c>
-      <c r="O29">
+      <c r="P29">
         <v>325.94466575684237</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -1342,14 +1374,14 @@
       <c r="D30">
         <v>16.2</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>0.86442307692307696</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>5.5622450987683897E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1359,20 +1391,20 @@
       <c r="C31">
         <v>1006</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <v>0.9259615384615385</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <v>4.7935013232664241E-2</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <v>133.11666666666665</v>
       </c>
-      <c r="K31" s="2">
+      <c r="L31" s="2">
         <v>100.80000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -1391,20 +1423,24 @@
       <c r="G32">
         <v>0.37827040810057388</v>
       </c>
-      <c r="L32">
+      <c r="H32">
+        <f>F32/M32</f>
+        <v>1.8643711192968791E-2</v>
+      </c>
+      <c r="M32">
         <v>216.8302565533308</v>
       </c>
-      <c r="M32">
+      <c r="N32">
         <v>304.20829456947212</v>
       </c>
-      <c r="N32">
+      <c r="O32">
         <v>35.676835928243406</v>
       </c>
-      <c r="O32">
+      <c r="P32">
         <v>556.71538705104638</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -1417,34 +1453,34 @@
       <c r="D33">
         <v>18.25</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <v>0.9802884615384615</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>6.4726008422452033E-2</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <v>150.83333333333334</v>
       </c>
-      <c r="K33">
+      <c r="L33">
         <v>119.81666666666666</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>16</v>
       </c>
       <c r="B34" s="1">
         <v>45323</v>
       </c>
-      <c r="J34">
+      <c r="K34">
         <v>188.48333333333335</v>
       </c>
-      <c r="K34">
+      <c r="L34">
         <v>172.45000000000005</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -1457,16 +1493,16 @@
       <c r="G35">
         <v>1.6615774246742543E-2</v>
       </c>
-      <c r="J35">
+      <c r="K35">
         <v>165.13333333333333</v>
       </c>
-      <c r="K35">
+      <c r="L35">
         <v>133.63333333333333</v>
       </c>
     </row>
     <row r="1657" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1635:EP1814">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1635:EQ1814">
     <sortCondition ref="B2:B2265"/>
     <sortCondition ref="C2:C2265"/>
   </sortState>

</xml_diff>

<commit_message>
Added EM data for 13/2/2024
</commit_message>
<xml_diff>
--- a/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
+++ b/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Prototypes\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030C81E5-E649-43B8-BA46-C88151F75A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080A02B2-07AA-43CA-944D-A444DCDFD5D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="CottonObserved" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CottonObserved!$A$1:$EQ$2578</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CottonObserved!$A$1:$EQ$2579</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="18">
   <si>
     <t>SimulationName</t>
   </si>
@@ -125,10 +125,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,14 +444,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C911DF83-7300-4B7A-8A42-16858D40307A}">
-  <dimension ref="A1:P1657"/>
+  <dimension ref="A1:P1658"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="9970" ySplit="760" topLeftCell="H11" activePane="bottomRight"/>
       <selection sqref="A1:A1048576"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
-      <selection pane="bottomRight" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
+      <selection pane="bottomRight" activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1078,30 +1079,32 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="1">
-        <v>45236</v>
-      </c>
+        <v>45335</v>
+      </c>
+      <c r="I19" s="2"/>
       <c r="K19">
-        <v>93.333333333333329</v>
+        <v>191.41666666666666</v>
       </c>
       <c r="L19" s="2">
-        <v>82.300000000000011</v>
-      </c>
+        <v>164.79999999999998</v>
+      </c>
+      <c r="N19" s="2"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="1">
-        <v>45243</v>
+        <v>45236</v>
       </c>
       <c r="K20">
-        <v>104.5</v>
+        <v>93.333333333333329</v>
       </c>
       <c r="L20" s="2">
-        <v>135.1</v>
+        <v>82.300000000000011</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.45">
@@ -1109,13 +1112,13 @@
         <v>16</v>
       </c>
       <c r="B21" s="1">
-        <v>45248</v>
+        <v>45243</v>
       </c>
       <c r="K21">
-        <v>124.35000000000002</v>
+        <v>104.5</v>
       </c>
       <c r="L21" s="2">
-        <v>158.38333333333333</v>
+        <v>135.1</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.45">
@@ -1123,19 +1126,13 @@
         <v>16</v>
       </c>
       <c r="B22" s="1">
-        <v>45254</v>
-      </c>
-      <c r="C22">
-        <v>70</v>
-      </c>
-      <c r="D22">
-        <v>1.2</v>
+        <v>45248</v>
       </c>
       <c r="K22">
-        <v>158.5</v>
+        <v>124.35000000000002</v>
       </c>
       <c r="L22" s="2">
-        <v>170.91666666666666</v>
+        <v>158.38333333333333</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.45">
@@ -1143,25 +1140,19 @@
         <v>16</v>
       </c>
       <c r="B23" s="1">
-        <v>45259</v>
+        <v>45254</v>
       </c>
       <c r="C23">
-        <v>122.5</v>
+        <v>70</v>
       </c>
       <c r="D23">
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="F23">
-        <v>0.10798078444273128</v>
-      </c>
-      <c r="G23">
-        <v>1.0286612192528072E-2</v>
+        <v>1.2</v>
       </c>
       <c r="K23">
-        <v>166.08333333333334</v>
+        <v>158.5</v>
       </c>
       <c r="L23" s="2">
-        <v>170.3</v>
+        <v>170.91666666666666</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.45">
@@ -1169,31 +1160,25 @@
         <v>16</v>
       </c>
       <c r="B24" s="1">
-        <v>45266</v>
+        <v>45259</v>
       </c>
       <c r="C24">
-        <v>249.5</v>
+        <v>122.5</v>
       </c>
       <c r="D24">
-        <v>5.4</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="F24">
-        <v>0.21781349165461303</v>
+        <v>0.10798078444273128</v>
       </c>
       <c r="G24">
-        <v>3.0473870842271603E-2</v>
-      </c>
-      <c r="I24">
-        <v>0.20528846153846153</v>
-      </c>
-      <c r="J24">
-        <v>3.5743400843100848E-2</v>
+        <v>1.0286612192528072E-2</v>
       </c>
       <c r="K24">
-        <v>182.61666666666667</v>
+        <v>166.08333333333334</v>
       </c>
       <c r="L24" s="2">
-        <v>167.28333333333333</v>
+        <v>170.3</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.45">
@@ -1201,25 +1186,31 @@
         <v>16</v>
       </c>
       <c r="B25" s="1">
-        <v>45273</v>
+        <v>45266</v>
       </c>
       <c r="C25">
-        <v>346.84210526315792</v>
+        <v>249.5</v>
       </c>
       <c r="D25">
-        <v>8.0526315789473681</v>
+        <v>5.4</v>
+      </c>
+      <c r="F25">
+        <v>0.21781349165461303</v>
+      </c>
+      <c r="G25">
+        <v>3.0473870842271603E-2</v>
       </c>
       <c r="I25">
-        <v>0.30819838056680166</v>
+        <v>0.20528846153846153</v>
       </c>
       <c r="J25">
-        <v>4.4581672466543681E-2</v>
+        <v>3.5743400843100848E-2</v>
       </c>
       <c r="K25">
-        <v>168.93333333333331</v>
+        <v>182.61666666666667</v>
       </c>
       <c r="L25" s="2">
-        <v>158.08333333333334</v>
+        <v>167.28333333333333</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.45">
@@ -1227,13 +1218,25 @@
         <v>16</v>
       </c>
       <c r="B26" s="1">
-        <v>45274</v>
-      </c>
-      <c r="F26">
-        <v>0.45692237396557861</v>
-      </c>
-      <c r="G26">
-        <v>5.1146750325636835E-2</v>
+        <v>45273</v>
+      </c>
+      <c r="C26">
+        <v>346.84210526315792</v>
+      </c>
+      <c r="D26">
+        <v>8.0526315789473681</v>
+      </c>
+      <c r="I26">
+        <v>0.30819838056680166</v>
+      </c>
+      <c r="J26">
+        <v>4.4581672466543681E-2</v>
+      </c>
+      <c r="K26">
+        <v>168.93333333333331</v>
+      </c>
+      <c r="L26" s="2">
+        <v>158.08333333333334</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.45">
@@ -1241,47 +1244,13 @@
         <v>16</v>
       </c>
       <c r="B27" s="1">
-        <v>45279</v>
-      </c>
-      <c r="C27">
-        <v>462</v>
-      </c>
-      <c r="D27">
-        <v>10.15</v>
-      </c>
-      <c r="E27">
-        <v>21.25</v>
+        <v>45274</v>
       </c>
       <c r="F27">
-        <v>0.90377009469093894</v>
+        <v>0.45692237396557861</v>
       </c>
       <c r="G27">
-        <v>0.17957612594849667</v>
-      </c>
-      <c r="H27">
-        <f>F27/M27</f>
-        <v>1.4968551468417543E-2</v>
-      </c>
-      <c r="I27">
-        <v>0.40192307692307694</v>
-      </c>
-      <c r="J27">
-        <v>5.4543711246622169E-2</v>
-      </c>
-      <c r="K27">
-        <v>158.51666666666665</v>
-      </c>
-      <c r="L27">
-        <v>137.65</v>
-      </c>
-      <c r="M27">
-        <v>60.377926120494841</v>
-      </c>
-      <c r="N27">
-        <v>47.44502885132195</v>
-      </c>
-      <c r="P27">
-        <v>107.82295497181678</v>
+        <v>5.1146750325636835E-2</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.45">
@@ -1289,31 +1258,47 @@
         <v>16</v>
       </c>
       <c r="B28" s="1">
-        <v>45288</v>
+        <v>45279</v>
       </c>
       <c r="C28">
-        <v>586.5</v>
+        <v>462</v>
       </c>
       <c r="D28">
-        <v>12.2</v>
+        <v>10.15</v>
+      </c>
+      <c r="E28">
+        <v>21.25</v>
       </c>
       <c r="F28">
-        <v>2.1000585963396539</v>
+        <v>0.90377009469093894</v>
       </c>
       <c r="G28">
-        <v>0.16175497233014249</v>
+        <v>0.17957612594849667</v>
+      </c>
+      <c r="H28">
+        <f>F28/M28</f>
+        <v>1.4968551468417543E-2</v>
       </c>
       <c r="I28">
-        <v>0.61923076923076925</v>
+        <v>0.40192307692307694</v>
       </c>
       <c r="J28">
-        <v>5.8313123992568404E-2</v>
+        <v>5.4543711246622169E-2</v>
       </c>
       <c r="K28">
-        <v>183.81666666666663</v>
-      </c>
-      <c r="L28" s="2">
-        <v>185.81666666666663</v>
+        <v>158.51666666666665</v>
+      </c>
+      <c r="L28">
+        <v>137.65</v>
+      </c>
+      <c r="M28">
+        <v>60.377926120494841</v>
+      </c>
+      <c r="N28">
+        <v>47.44502885132195</v>
+      </c>
+      <c r="P28">
+        <v>107.82295497181678</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.45">
@@ -1321,44 +1306,31 @@
         <v>16</v>
       </c>
       <c r="B29" s="1">
-        <v>45296</v>
+        <v>45288</v>
       </c>
       <c r="C29">
-        <v>793</v>
-      </c>
-      <c r="E29">
-        <v>40</v>
+        <v>586.5</v>
+      </c>
+      <c r="D29">
+        <v>12.2</v>
       </c>
       <c r="F29">
-        <v>3.0317071477592523</v>
+        <v>2.1000585963396539</v>
       </c>
       <c r="G29">
-        <v>0.33366923094714623</v>
-      </c>
-      <c r="H29">
-        <f>F29/M29</f>
-        <v>2.1060960200872104E-2</v>
+        <v>0.16175497233014249</v>
       </c>
       <c r="I29">
-        <v>0.76298076923076918</v>
+        <v>0.61923076923076925</v>
       </c>
       <c r="J29">
-        <v>7.3246859198435113E-2</v>
+        <v>5.8313123992568404E-2</v>
       </c>
       <c r="K29">
-        <v>174.58333333333334</v>
+        <v>183.81666666666663</v>
       </c>
       <c r="L29" s="2">
-        <v>149.88333333333335</v>
-      </c>
-      <c r="M29">
-        <v>143.94914186456293</v>
-      </c>
-      <c r="N29">
-        <v>181.99552389227946</v>
-      </c>
-      <c r="P29">
-        <v>325.94466575684237</v>
+        <v>185.81666666666663</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.45">
@@ -1366,19 +1338,44 @@
         <v>16</v>
       </c>
       <c r="B30" s="1">
-        <v>45302</v>
+        <v>45296</v>
       </c>
       <c r="C30">
-        <v>956.5</v>
-      </c>
-      <c r="D30">
-        <v>16.2</v>
+        <v>793</v>
+      </c>
+      <c r="E30">
+        <v>40</v>
+      </c>
+      <c r="F30">
+        <v>3.0317071477592523</v>
+      </c>
+      <c r="G30">
+        <v>0.33366923094714623</v>
+      </c>
+      <c r="H30">
+        <f>F30/M30</f>
+        <v>2.1060960200872104E-2</v>
       </c>
       <c r="I30">
-        <v>0.86442307692307696</v>
+        <v>0.76298076923076918</v>
       </c>
       <c r="J30">
-        <v>5.5622450987683897E-2</v>
+        <v>7.3246859198435113E-2</v>
+      </c>
+      <c r="K30">
+        <v>174.58333333333334</v>
+      </c>
+      <c r="L30" s="2">
+        <v>149.88333333333335</v>
+      </c>
+      <c r="M30">
+        <v>143.94914186456293</v>
+      </c>
+      <c r="N30">
+        <v>181.99552389227946</v>
+      </c>
+      <c r="P30">
+        <v>325.94466575684237</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.45">
@@ -1386,22 +1383,19 @@
         <v>16</v>
       </c>
       <c r="B31" s="1">
-        <v>45306</v>
+        <v>45302</v>
       </c>
       <c r="C31">
-        <v>1006</v>
+        <v>956.5</v>
+      </c>
+      <c r="D31">
+        <v>16.2</v>
       </c>
       <c r="I31">
-        <v>0.9259615384615385</v>
+        <v>0.86442307692307696</v>
       </c>
       <c r="J31">
-        <v>4.7935013232664241E-2</v>
-      </c>
-      <c r="K31">
-        <v>133.11666666666665</v>
-      </c>
-      <c r="L31" s="2">
-        <v>100.80000000000001</v>
+        <v>5.5622450987683897E-2</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.45">
@@ -1409,102 +1403,139 @@
         <v>16</v>
       </c>
       <c r="B32" s="1">
+        <v>45306</v>
+      </c>
+      <c r="C32">
+        <v>1006</v>
+      </c>
+      <c r="I32">
+        <v>0.9259615384615385</v>
+      </c>
+      <c r="J32">
+        <v>4.7935013232664241E-2</v>
+      </c>
+      <c r="K32">
+        <v>133.11666666666665</v>
+      </c>
+      <c r="L32" s="2">
+        <v>100.80000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="1">
         <v>45307</v>
       </c>
-      <c r="D32">
+      <c r="D33">
         <v>17</v>
       </c>
-      <c r="E32">
+      <c r="E33">
         <v>54.5</v>
       </c>
-      <c r="F32">
+      <c r="F33">
         <v>4.0425206810776277</v>
       </c>
-      <c r="G32">
+      <c r="G33">
         <v>0.37827040810057388</v>
       </c>
-      <c r="H32">
-        <f>F32/M32</f>
+      <c r="H33">
+        <f>F33/M33</f>
         <v>1.8643711192968791E-2</v>
       </c>
-      <c r="M32">
+      <c r="M33">
         <v>216.8302565533308</v>
       </c>
-      <c r="N32">
+      <c r="N33">
         <v>304.20829456947212</v>
       </c>
-      <c r="O32">
+      <c r="O33">
         <v>35.676835928243406</v>
       </c>
-      <c r="P32">
+      <c r="P33">
         <v>556.71538705104638</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
-        <v>16</v>
-      </c>
-      <c r="B33" s="1">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="1">
         <v>45314</v>
       </c>
-      <c r="C33">
+      <c r="C34">
         <v>1191.5</v>
       </c>
-      <c r="D33">
+      <c r="D34">
         <v>18.25</v>
       </c>
-      <c r="I33">
+      <c r="I34">
         <v>0.9802884615384615</v>
       </c>
-      <c r="J33">
+      <c r="J34">
         <v>6.4726008422452033E-2</v>
       </c>
-      <c r="K33">
+      <c r="K34">
         <v>150.83333333333334</v>
       </c>
-      <c r="L33">
+      <c r="L34">
         <v>119.81666666666666</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34" s="1">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="1">
         <v>45323</v>
       </c>
-      <c r="K34">
+      <c r="K35">
         <v>188.48333333333335</v>
       </c>
-      <c r="L34">
+      <c r="L35">
         <v>172.45000000000005</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
-        <v>16</v>
-      </c>
-      <c r="B35" s="1">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="1">
         <v>45331</v>
       </c>
-      <c r="F35">
+      <c r="F36">
         <v>5.5032705000000002</v>
       </c>
-      <c r="G35">
+      <c r="G36">
         <v>1.6615774246742543E-2</v>
       </c>
-      <c r="K35">
+      <c r="K36">
         <v>165.13333333333333</v>
       </c>
-      <c r="L35">
+      <c r="L36">
         <v>133.63333333333333</v>
       </c>
     </row>
-    <row r="1657" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="3">
+        <v>45335</v>
+      </c>
+      <c r="K37" s="2">
+        <v>146.33333333333334</v>
+      </c>
+      <c r="L37">
+        <v>103.91666666666669</v>
+      </c>
+    </row>
+    <row r="1658" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1635:EQ1814">
-    <sortCondition ref="B2:B2265"/>
-    <sortCondition ref="C2:C2265"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1636:EQ1815">
+    <sortCondition ref="B2:B2266"/>
+    <sortCondition ref="C2:C2266"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Biomass data from 1-2-24
</commit_message>
<xml_diff>
--- a/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
+++ b/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Prototypes\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080A02B2-07AA-43CA-944D-A444DCDFD5D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C35DDAE-7A66-43AF-9331-ED6B15031EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="19">
   <si>
     <t>SimulationName</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Cotton.Leaf.SpecificArea</t>
+  </si>
+  <si>
+    <t>Cotton.Bur.Wt</t>
   </si>
 </sst>
 </file>
@@ -444,14 +447,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C911DF83-7300-4B7A-8A42-16858D40307A}">
-  <dimension ref="A1:P1658"/>
+  <dimension ref="A1:Q1658"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="9970" ySplit="760" topLeftCell="H11" activePane="bottomRight"/>
+      <pane xSplit="9970" ySplit="760" topLeftCell="L11" activePane="topRight"/>
       <selection sqref="A1:A1048576"/>
-      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <selection pane="topRight" activeCell="Q2" sqref="Q2"/>
       <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
-      <selection pane="bottomRight" activeCell="K19" sqref="K19"/>
+      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -584,7 +587,7 @@
     <col min="140" max="147" width="24.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -633,8 +636,11 @@
       <c r="P1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -648,7 +654,7 @@
         <v>96.683333333333337</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -662,7 +668,7 @@
         <v>139.43333333333331</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -676,7 +682,7 @@
         <v>162.56666666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -696,7 +702,7 @@
         <v>183.21666666666667</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -722,7 +728,7 @@
         <v>172.93333333333331</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -754,7 +760,7 @@
         <v>192.94999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -783,7 +789,7 @@
         <v>161.20000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -797,7 +803,7 @@
         <v>3.605272908788857E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -841,7 +847,7 @@
         <v>109.08904747019719</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -861,7 +867,7 @@
         <v>190.58333333333337</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -906,7 +912,7 @@
         <v>330.63006704592664</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -926,7 +932,7 @@
         <v>0.10013140610136738</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -949,7 +955,7 @@
         <v>104.5</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -985,7 +991,7 @@
         <v>604.68241646966715</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1011,7 +1017,7 @@
         <v>173.93333333333331</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1033,6 +1039,10 @@
       <c r="G17">
         <v>0.32232021196016941</v>
       </c>
+      <c r="H17">
+        <f>F18/M17</f>
+        <v>2.0823552901265103E-2</v>
+      </c>
       <c r="I17" s="2">
         <v>0.98990384615384619</v>
       </c>
@@ -1045,8 +1055,24 @@
       <c r="L17" s="2">
         <v>180.61666666666667</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="M17">
+        <v>282.98</v>
+      </c>
+      <c r="N17" s="2">
+        <v>425.3</v>
+      </c>
+      <c r="O17">
+        <v>175.6</v>
+      </c>
+      <c r="P17">
+        <v>883.9</v>
+      </c>
+      <c r="Q17">
+        <f>O17*0.4156</f>
+        <v>72.97936</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1058,10 +1084,6 @@
       </c>
       <c r="G18">
         <v>0.16848393942648088</v>
-      </c>
-      <c r="H18">
-        <f>F18/M18</f>
-        <v>2.0823552901265103E-2</v>
       </c>
       <c r="I18" s="2"/>
       <c r="K18" s="2">
@@ -1070,14 +1092,8 @@
       <c r="L18" s="2">
         <v>124.45</v>
       </c>
-      <c r="M18">
-        <v>282.98</v>
-      </c>
-      <c r="N18" s="2">
-        <v>425.3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -1093,7 +1109,7 @@
       </c>
       <c r="N19" s="2"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -1107,7 +1123,7 @@
         <v>82.300000000000011</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -1121,7 +1137,7 @@
         <v>135.1</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -1135,7 +1151,7 @@
         <v>158.38333333333333</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -1155,7 +1171,7 @@
         <v>170.91666666666666</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -1181,7 +1197,7 @@
         <v>170.3</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -1213,7 +1229,7 @@
         <v>167.28333333333333</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -1239,7 +1255,7 @@
         <v>158.08333333333334</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -1253,7 +1269,7 @@
         <v>5.1146750325636835E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -1301,7 +1317,7 @@
         <v>107.82295497181678</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -1333,7 +1349,7 @@
         <v>185.81666666666663</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -1378,7 +1394,7 @@
         <v>325.94466575684237</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1398,7 +1414,7 @@
         <v>5.5622450987683897E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
added data for Feb 22-23
</commit_message>
<xml_diff>
--- a/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
+++ b/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Prototypes\Cotton\Observed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\APSIMX\Prototypes\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C35DDAE-7A66-43AF-9331-ED6B15031EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AFFC07-795A-4DA0-B8CA-BD9149C7531A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
+    <workbookView xWindow="-38520" yWindow="870" windowWidth="38640" windowHeight="21120" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
   <sheets>
     <sheet name="CottonObserved" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CottonObserved!$A$1:$EQ$2579</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CottonObserved!$A$1:$EQ$2580</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="19">
   <si>
     <t>SimulationName</t>
   </si>
@@ -151,9 +151,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -191,7 +191,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -297,7 +297,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -439,7 +439,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -447,14 +447,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C911DF83-7300-4B7A-8A42-16858D40307A}">
-  <dimension ref="A1:Q1658"/>
+  <dimension ref="A1:Q1659"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="9970" ySplit="760" topLeftCell="L11" activePane="topRight"/>
+      <pane xSplit="9975" ySplit="765" topLeftCell="B11" activePane="bottomRight"/>
       <selection sqref="A1:A1048576"/>
       <selection pane="topRight" activeCell="Q2" sqref="Q2"/>
-      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
-      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
+      <selection pane="bottomRight" activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1111,30 +1111,41 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" s="1">
-        <v>45236</v>
-      </c>
-      <c r="K20">
-        <v>93.333333333333329</v>
+        <v>45345</v>
+      </c>
+      <c r="C20">
+        <v>1420</v>
+      </c>
+      <c r="F20">
+        <v>7.135758</v>
+      </c>
+      <c r="G20">
+        <v>0.25569019509642193</v>
+      </c>
+      <c r="I20" s="2"/>
+      <c r="K20" s="2">
+        <v>170.18571428571428</v>
       </c>
       <c r="L20" s="2">
-        <v>82.300000000000011</v>
-      </c>
+        <v>147.1142857142857</v>
+      </c>
+      <c r="N20" s="2"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="1">
-        <v>45243</v>
+        <v>45236</v>
       </c>
       <c r="K21">
-        <v>104.5</v>
+        <v>93.333333333333329</v>
       </c>
       <c r="L21" s="2">
-        <v>135.1</v>
+        <v>82.300000000000011</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.45">
@@ -1142,13 +1153,13 @@
         <v>16</v>
       </c>
       <c r="B22" s="1">
-        <v>45248</v>
+        <v>45243</v>
       </c>
       <c r="K22">
-        <v>124.35000000000002</v>
+        <v>104.5</v>
       </c>
       <c r="L22" s="2">
-        <v>158.38333333333333</v>
+        <v>135.1</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.45">
@@ -1156,19 +1167,13 @@
         <v>16</v>
       </c>
       <c r="B23" s="1">
-        <v>45254</v>
-      </c>
-      <c r="C23">
-        <v>70</v>
-      </c>
-      <c r="D23">
-        <v>1.2</v>
+        <v>45248</v>
       </c>
       <c r="K23">
-        <v>158.5</v>
+        <v>124.35000000000002</v>
       </c>
       <c r="L23" s="2">
-        <v>170.91666666666666</v>
+        <v>158.38333333333333</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.45">
@@ -1176,25 +1181,19 @@
         <v>16</v>
       </c>
       <c r="B24" s="1">
-        <v>45259</v>
+        <v>45254</v>
       </c>
       <c r="C24">
-        <v>122.5</v>
+        <v>70</v>
       </c>
       <c r="D24">
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="F24">
-        <v>0.10798078444273128</v>
-      </c>
-      <c r="G24">
-        <v>1.0286612192528072E-2</v>
+        <v>1.2</v>
       </c>
       <c r="K24">
-        <v>166.08333333333334</v>
+        <v>158.5</v>
       </c>
       <c r="L24" s="2">
-        <v>170.3</v>
+        <v>170.91666666666666</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.45">
@@ -1202,31 +1201,25 @@
         <v>16</v>
       </c>
       <c r="B25" s="1">
-        <v>45266</v>
+        <v>45259</v>
       </c>
       <c r="C25">
-        <v>249.5</v>
+        <v>122.5</v>
       </c>
       <c r="D25">
-        <v>5.4</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="F25">
-        <v>0.21781349165461303</v>
+        <v>0.10798078444273128</v>
       </c>
       <c r="G25">
-        <v>3.0473870842271603E-2</v>
-      </c>
-      <c r="I25">
-        <v>0.20528846153846153</v>
-      </c>
-      <c r="J25">
-        <v>3.5743400843100848E-2</v>
+        <v>1.0286612192528072E-2</v>
       </c>
       <c r="K25">
-        <v>182.61666666666667</v>
+        <v>166.08333333333334</v>
       </c>
       <c r="L25" s="2">
-        <v>167.28333333333333</v>
+        <v>170.3</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.45">
@@ -1234,25 +1227,31 @@
         <v>16</v>
       </c>
       <c r="B26" s="1">
-        <v>45273</v>
+        <v>45266</v>
       </c>
       <c r="C26">
-        <v>346.84210526315792</v>
+        <v>249.5</v>
       </c>
       <c r="D26">
-        <v>8.0526315789473681</v>
+        <v>5.4</v>
+      </c>
+      <c r="F26">
+        <v>0.21781349165461303</v>
+      </c>
+      <c r="G26">
+        <v>3.0473870842271603E-2</v>
       </c>
       <c r="I26">
-        <v>0.30819838056680166</v>
+        <v>0.20528846153846153</v>
       </c>
       <c r="J26">
-        <v>4.4581672466543681E-2</v>
+        <v>3.5743400843100848E-2</v>
       </c>
       <c r="K26">
-        <v>168.93333333333331</v>
+        <v>182.61666666666667</v>
       </c>
       <c r="L26" s="2">
-        <v>158.08333333333334</v>
+        <v>167.28333333333333</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.45">
@@ -1260,13 +1259,25 @@
         <v>16</v>
       </c>
       <c r="B27" s="1">
-        <v>45274</v>
-      </c>
-      <c r="F27">
-        <v>0.45692237396557861</v>
-      </c>
-      <c r="G27">
-        <v>5.1146750325636835E-2</v>
+        <v>45273</v>
+      </c>
+      <c r="C27">
+        <v>346.84210526315792</v>
+      </c>
+      <c r="D27">
+        <v>8.0526315789473681</v>
+      </c>
+      <c r="I27">
+        <v>0.30819838056680166</v>
+      </c>
+      <c r="J27">
+        <v>4.4581672466543681E-2</v>
+      </c>
+      <c r="K27">
+        <v>168.93333333333331</v>
+      </c>
+      <c r="L27" s="2">
+        <v>158.08333333333334</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.45">
@@ -1274,47 +1285,13 @@
         <v>16</v>
       </c>
       <c r="B28" s="1">
-        <v>45279</v>
-      </c>
-      <c r="C28">
-        <v>462</v>
-      </c>
-      <c r="D28">
-        <v>10.15</v>
-      </c>
-      <c r="E28">
-        <v>21.25</v>
+        <v>45274</v>
       </c>
       <c r="F28">
-        <v>0.90377009469093894</v>
+        <v>0.45692237396557861</v>
       </c>
       <c r="G28">
-        <v>0.17957612594849667</v>
-      </c>
-      <c r="H28">
-        <f>F28/M28</f>
-        <v>1.4968551468417543E-2</v>
-      </c>
-      <c r="I28">
-        <v>0.40192307692307694</v>
-      </c>
-      <c r="J28">
-        <v>5.4543711246622169E-2</v>
-      </c>
-      <c r="K28">
-        <v>158.51666666666665</v>
-      </c>
-      <c r="L28">
-        <v>137.65</v>
-      </c>
-      <c r="M28">
-        <v>60.377926120494841</v>
-      </c>
-      <c r="N28">
-        <v>47.44502885132195</v>
-      </c>
-      <c r="P28">
-        <v>107.82295497181678</v>
+        <v>5.1146750325636835E-2</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.45">
@@ -1322,31 +1299,47 @@
         <v>16</v>
       </c>
       <c r="B29" s="1">
-        <v>45288</v>
+        <v>45279</v>
       </c>
       <c r="C29">
-        <v>586.5</v>
+        <v>462</v>
       </c>
       <c r="D29">
-        <v>12.2</v>
+        <v>10.15</v>
+      </c>
+      <c r="E29">
+        <v>21.25</v>
       </c>
       <c r="F29">
-        <v>2.1000585963396539</v>
+        <v>0.90377009469093894</v>
       </c>
       <c r="G29">
-        <v>0.16175497233014249</v>
+        <v>0.17957612594849667</v>
+      </c>
+      <c r="H29">
+        <f>F29/M29</f>
+        <v>1.4968551468417543E-2</v>
       </c>
       <c r="I29">
-        <v>0.61923076923076925</v>
+        <v>0.40192307692307694</v>
       </c>
       <c r="J29">
-        <v>5.8313123992568404E-2</v>
+        <v>5.4543711246622169E-2</v>
       </c>
       <c r="K29">
-        <v>183.81666666666663</v>
-      </c>
-      <c r="L29" s="2">
-        <v>185.81666666666663</v>
+        <v>158.51666666666665</v>
+      </c>
+      <c r="L29">
+        <v>137.65</v>
+      </c>
+      <c r="M29">
+        <v>60.377926120494841</v>
+      </c>
+      <c r="N29">
+        <v>47.44502885132195</v>
+      </c>
+      <c r="P29">
+        <v>107.82295497181678</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.45">
@@ -1354,44 +1347,31 @@
         <v>16</v>
       </c>
       <c r="B30" s="1">
-        <v>45296</v>
+        <v>45288</v>
       </c>
       <c r="C30">
-        <v>793</v>
-      </c>
-      <c r="E30">
-        <v>40</v>
+        <v>586.5</v>
+      </c>
+      <c r="D30">
+        <v>12.2</v>
       </c>
       <c r="F30">
-        <v>3.0317071477592523</v>
+        <v>2.1000585963396539</v>
       </c>
       <c r="G30">
-        <v>0.33366923094714623</v>
-      </c>
-      <c r="H30">
-        <f>F30/M30</f>
-        <v>2.1060960200872104E-2</v>
+        <v>0.16175497233014249</v>
       </c>
       <c r="I30">
-        <v>0.76298076923076918</v>
+        <v>0.61923076923076925</v>
       </c>
       <c r="J30">
-        <v>7.3246859198435113E-2</v>
+        <v>5.8313123992568404E-2</v>
       </c>
       <c r="K30">
-        <v>174.58333333333334</v>
+        <v>183.81666666666663</v>
       </c>
       <c r="L30" s="2">
-        <v>149.88333333333335</v>
-      </c>
-      <c r="M30">
-        <v>143.94914186456293</v>
-      </c>
-      <c r="N30">
-        <v>181.99552389227946</v>
-      </c>
-      <c r="P30">
-        <v>325.94466575684237</v>
+        <v>185.81666666666663</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.45">
@@ -1399,19 +1379,44 @@
         <v>16</v>
       </c>
       <c r="B31" s="1">
-        <v>45302</v>
+        <v>45296</v>
       </c>
       <c r="C31">
-        <v>956.5</v>
-      </c>
-      <c r="D31">
-        <v>16.2</v>
+        <v>793</v>
+      </c>
+      <c r="E31">
+        <v>40</v>
+      </c>
+      <c r="F31">
+        <v>3.0317071477592523</v>
+      </c>
+      <c r="G31">
+        <v>0.33366923094714623</v>
+      </c>
+      <c r="H31">
+        <f>F31/M31</f>
+        <v>2.1060960200872104E-2</v>
       </c>
       <c r="I31">
-        <v>0.86442307692307696</v>
+        <v>0.76298076923076918</v>
       </c>
       <c r="J31">
-        <v>5.5622450987683897E-2</v>
+        <v>7.3246859198435113E-2</v>
+      </c>
+      <c r="K31">
+        <v>174.58333333333334</v>
+      </c>
+      <c r="L31" s="2">
+        <v>149.88333333333335</v>
+      </c>
+      <c r="M31">
+        <v>143.94914186456293</v>
+      </c>
+      <c r="N31">
+        <v>181.99552389227946</v>
+      </c>
+      <c r="P31">
+        <v>325.94466575684237</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.45">
@@ -1419,22 +1424,19 @@
         <v>16</v>
       </c>
       <c r="B32" s="1">
-        <v>45306</v>
+        <v>45302</v>
       </c>
       <c r="C32">
-        <v>1006</v>
+        <v>956.5</v>
+      </c>
+      <c r="D32">
+        <v>16.2</v>
       </c>
       <c r="I32">
-        <v>0.9259615384615385</v>
+        <v>0.86442307692307696</v>
       </c>
       <c r="J32">
-        <v>4.7935013232664241E-2</v>
-      </c>
-      <c r="K32">
-        <v>133.11666666666665</v>
-      </c>
-      <c r="L32" s="2">
-        <v>100.80000000000001</v>
+        <v>5.5622450987683897E-2</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.45">
@@ -1442,35 +1444,22 @@
         <v>16</v>
       </c>
       <c r="B33" s="1">
-        <v>45307</v>
-      </c>
-      <c r="D33">
-        <v>17</v>
-      </c>
-      <c r="E33">
-        <v>54.5</v>
-      </c>
-      <c r="F33">
-        <v>4.0425206810776277</v>
-      </c>
-      <c r="G33">
-        <v>0.37827040810057388</v>
-      </c>
-      <c r="H33">
-        <f>F33/M33</f>
-        <v>1.8643711192968791E-2</v>
-      </c>
-      <c r="M33">
-        <v>216.8302565533308</v>
-      </c>
-      <c r="N33">
-        <v>304.20829456947212</v>
-      </c>
-      <c r="O33">
-        <v>35.676835928243406</v>
-      </c>
-      <c r="P33">
-        <v>556.71538705104638</v>
+        <v>45306</v>
+      </c>
+      <c r="C33">
+        <v>1006</v>
+      </c>
+      <c r="I33">
+        <v>0.9259615384615385</v>
+      </c>
+      <c r="J33">
+        <v>4.7935013232664241E-2</v>
+      </c>
+      <c r="K33">
+        <v>133.11666666666665</v>
+      </c>
+      <c r="L33" s="2">
+        <v>100.80000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.45">
@@ -1478,25 +1467,35 @@
         <v>16</v>
       </c>
       <c r="B34" s="1">
-        <v>45314</v>
-      </c>
-      <c r="C34">
-        <v>1191.5</v>
+        <v>45307</v>
       </c>
       <c r="D34">
-        <v>18.25</v>
-      </c>
-      <c r="I34">
-        <v>0.9802884615384615</v>
-      </c>
-      <c r="J34">
-        <v>6.4726008422452033E-2</v>
-      </c>
-      <c r="K34">
-        <v>150.83333333333334</v>
-      </c>
-      <c r="L34">
-        <v>119.81666666666666</v>
+        <v>17</v>
+      </c>
+      <c r="E34">
+        <v>54.5</v>
+      </c>
+      <c r="F34">
+        <v>4.0425206810776277</v>
+      </c>
+      <c r="G34">
+        <v>0.37827040810057388</v>
+      </c>
+      <c r="H34">
+        <f>F34/M34</f>
+        <v>1.8643711192968791E-2</v>
+      </c>
+      <c r="M34">
+        <v>216.8302565533308</v>
+      </c>
+      <c r="N34">
+        <v>304.20829456947212</v>
+      </c>
+      <c r="O34">
+        <v>35.676835928243406</v>
+      </c>
+      <c r="P34">
+        <v>556.71538705104638</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.45">
@@ -1504,13 +1503,25 @@
         <v>16</v>
       </c>
       <c r="B35" s="1">
-        <v>45323</v>
+        <v>45314</v>
+      </c>
+      <c r="C35">
+        <v>1191.5</v>
+      </c>
+      <c r="D35">
+        <v>18.25</v>
+      </c>
+      <c r="I35">
+        <v>0.9802884615384615</v>
+      </c>
+      <c r="J35">
+        <v>6.4726008422452033E-2</v>
       </c>
       <c r="K35">
-        <v>188.48333333333335</v>
+        <v>150.83333333333334</v>
       </c>
       <c r="L35">
-        <v>172.45000000000005</v>
+        <v>119.81666666666666</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.45">
@@ -1518,40 +1529,77 @@
         <v>16</v>
       </c>
       <c r="B36" s="1">
-        <v>45331</v>
-      </c>
-      <c r="F36">
-        <v>5.5032705000000002</v>
-      </c>
-      <c r="G36">
-        <v>1.6615774246742543E-2</v>
+        <v>45323</v>
       </c>
       <c r="K36">
-        <v>165.13333333333333</v>
+        <v>188.48333333333335</v>
       </c>
       <c r="L36">
-        <v>133.63333333333333</v>
+        <v>172.45000000000005</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="1">
+        <v>45331</v>
+      </c>
+      <c r="F37">
+        <v>5.5032705000000002</v>
+      </c>
+      <c r="G37">
+        <v>1.6615774246742543E-2</v>
+      </c>
+      <c r="K37">
+        <v>165.13333333333333</v>
+      </c>
+      <c r="L37">
+        <v>133.63333333333333</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="3">
         <v>45335</v>
       </c>
-      <c r="K37" s="2">
+      <c r="K38" s="2">
         <v>146.33333333333334</v>
       </c>
-      <c r="L37">
+      <c r="L38">
         <v>103.91666666666669</v>
       </c>
     </row>
-    <row r="1658" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="1">
+        <v>45345</v>
+      </c>
+      <c r="C39">
+        <v>1375</v>
+      </c>
+      <c r="F39">
+        <v>6.2965385000000005</v>
+      </c>
+      <c r="G39">
+        <v>0.3468610456650591</v>
+      </c>
+      <c r="K39" s="2">
+        <v>126.25000000000001</v>
+      </c>
+      <c r="L39">
+        <v>83.516666666666666</v>
+      </c>
+    </row>
+    <row r="1659" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1636:EQ1815">
-    <sortCondition ref="B2:B2266"/>
-    <sortCondition ref="C2:C2266"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1637:EQ1816">
+    <sortCondition ref="B2:B2267"/>
+    <sortCondition ref="C2:C2267"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Start adding extra obs data
</commit_message>
<xml_diff>
--- a/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
+++ b/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\APSIMX\Prototypes\Cotton\Observed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Prototypes\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AFFC07-795A-4DA0-B8CA-BD9149C7531A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440A839D-2AA2-4428-B677-34BF749BC53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="870" windowWidth="38640" windowHeight="21120" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
+    <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
   <sheets>
     <sheet name="CottonObserved" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CottonObserved!$A$1:$EQ$2580</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CottonObserved!$A$1:$EQ$2581</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="19">
   <si>
     <t>SimulationName</t>
   </si>
@@ -151,9 +151,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -191,7 +191,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -297,7 +297,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -439,7 +439,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -447,14 +447,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C911DF83-7300-4B7A-8A42-16858D40307A}">
-  <dimension ref="A1:Q1659"/>
+  <dimension ref="A1:Q1660"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="9975" ySplit="765" topLeftCell="B11" activePane="bottomRight"/>
+      <pane xSplit="9980" ySplit="770" activePane="bottomRight"/>
       <selection sqref="A1:A1048576"/>
       <selection pane="topRight" activeCell="Q2" sqref="Q2"/>
       <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
-      <selection pane="bottomRight" activeCell="G39" sqref="G39"/>
+      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1136,30 +1136,40 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" s="1">
-        <v>45236</v>
-      </c>
-      <c r="K21">
-        <v>93.333333333333329</v>
-      </c>
-      <c r="L21" s="2">
-        <v>82.300000000000011</v>
-      </c>
+        <v>45355</v>
+      </c>
+      <c r="D21">
+        <v>23</v>
+      </c>
+      <c r="E21">
+        <v>79</v>
+      </c>
+      <c r="F21">
+        <v>5.51</v>
+      </c>
+      <c r="G21">
+        <v>0.53</v>
+      </c>
+      <c r="I21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="N21" s="2"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="1">
-        <v>45243</v>
+        <v>45236</v>
       </c>
       <c r="K22">
-        <v>104.5</v>
+        <v>93.333333333333329</v>
       </c>
       <c r="L22" s="2">
-        <v>135.1</v>
+        <v>82.300000000000011</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.45">
@@ -1167,13 +1177,13 @@
         <v>16</v>
       </c>
       <c r="B23" s="1">
-        <v>45248</v>
+        <v>45243</v>
       </c>
       <c r="K23">
-        <v>124.35000000000002</v>
+        <v>104.5</v>
       </c>
       <c r="L23" s="2">
-        <v>158.38333333333333</v>
+        <v>135.1</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.45">
@@ -1181,19 +1191,13 @@
         <v>16</v>
       </c>
       <c r="B24" s="1">
-        <v>45254</v>
-      </c>
-      <c r="C24">
-        <v>70</v>
-      </c>
-      <c r="D24">
-        <v>1.2</v>
+        <v>45248</v>
       </c>
       <c r="K24">
-        <v>158.5</v>
+        <v>124.35000000000002</v>
       </c>
       <c r="L24" s="2">
-        <v>170.91666666666666</v>
+        <v>158.38333333333333</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.45">
@@ -1201,25 +1205,19 @@
         <v>16</v>
       </c>
       <c r="B25" s="1">
-        <v>45259</v>
+        <v>45254</v>
       </c>
       <c r="C25">
-        <v>122.5</v>
+        <v>70</v>
       </c>
       <c r="D25">
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="F25">
-        <v>0.10798078444273128</v>
-      </c>
-      <c r="G25">
-        <v>1.0286612192528072E-2</v>
+        <v>1.2</v>
       </c>
       <c r="K25">
-        <v>166.08333333333334</v>
+        <v>158.5</v>
       </c>
       <c r="L25" s="2">
-        <v>170.3</v>
+        <v>170.91666666666666</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.45">
@@ -1227,31 +1225,25 @@
         <v>16</v>
       </c>
       <c r="B26" s="1">
-        <v>45266</v>
+        <v>45259</v>
       </c>
       <c r="C26">
-        <v>249.5</v>
+        <v>122.5</v>
       </c>
       <c r="D26">
-        <v>5.4</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="F26">
-        <v>0.21781349165461303</v>
+        <v>0.10798078444273128</v>
       </c>
       <c r="G26">
-        <v>3.0473870842271603E-2</v>
-      </c>
-      <c r="I26">
-        <v>0.20528846153846153</v>
-      </c>
-      <c r="J26">
-        <v>3.5743400843100848E-2</v>
+        <v>1.0286612192528072E-2</v>
       </c>
       <c r="K26">
-        <v>182.61666666666667</v>
+        <v>166.08333333333334</v>
       </c>
       <c r="L26" s="2">
-        <v>167.28333333333333</v>
+        <v>170.3</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.45">
@@ -1259,25 +1251,31 @@
         <v>16</v>
       </c>
       <c r="B27" s="1">
-        <v>45273</v>
+        <v>45266</v>
       </c>
       <c r="C27">
-        <v>346.84210526315792</v>
+        <v>249.5</v>
       </c>
       <c r="D27">
-        <v>8.0526315789473681</v>
+        <v>5.4</v>
+      </c>
+      <c r="F27">
+        <v>0.21781349165461303</v>
+      </c>
+      <c r="G27">
+        <v>3.0473870842271603E-2</v>
       </c>
       <c r="I27">
-        <v>0.30819838056680166</v>
+        <v>0.20528846153846153</v>
       </c>
       <c r="J27">
-        <v>4.4581672466543681E-2</v>
+        <v>3.5743400843100848E-2</v>
       </c>
       <c r="K27">
-        <v>168.93333333333331</v>
+        <v>182.61666666666667</v>
       </c>
       <c r="L27" s="2">
-        <v>158.08333333333334</v>
+        <v>167.28333333333333</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.45">
@@ -1285,13 +1283,25 @@
         <v>16</v>
       </c>
       <c r="B28" s="1">
-        <v>45274</v>
-      </c>
-      <c r="F28">
-        <v>0.45692237396557861</v>
-      </c>
-      <c r="G28">
-        <v>5.1146750325636835E-2</v>
+        <v>45273</v>
+      </c>
+      <c r="C28">
+        <v>346.84210526315792</v>
+      </c>
+      <c r="D28">
+        <v>8.0526315789473681</v>
+      </c>
+      <c r="I28">
+        <v>0.30819838056680166</v>
+      </c>
+      <c r="J28">
+        <v>4.4581672466543681E-2</v>
+      </c>
+      <c r="K28">
+        <v>168.93333333333331</v>
+      </c>
+      <c r="L28" s="2">
+        <v>158.08333333333334</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.45">
@@ -1299,47 +1309,13 @@
         <v>16</v>
       </c>
       <c r="B29" s="1">
-        <v>45279</v>
-      </c>
-      <c r="C29">
-        <v>462</v>
-      </c>
-      <c r="D29">
-        <v>10.15</v>
-      </c>
-      <c r="E29">
-        <v>21.25</v>
+        <v>45274</v>
       </c>
       <c r="F29">
-        <v>0.90377009469093894</v>
+        <v>0.45692237396557861</v>
       </c>
       <c r="G29">
-        <v>0.17957612594849667</v>
-      </c>
-      <c r="H29">
-        <f>F29/M29</f>
-        <v>1.4968551468417543E-2</v>
-      </c>
-      <c r="I29">
-        <v>0.40192307692307694</v>
-      </c>
-      <c r="J29">
-        <v>5.4543711246622169E-2</v>
-      </c>
-      <c r="K29">
-        <v>158.51666666666665</v>
-      </c>
-      <c r="L29">
-        <v>137.65</v>
-      </c>
-      <c r="M29">
-        <v>60.377926120494841</v>
-      </c>
-      <c r="N29">
-        <v>47.44502885132195</v>
-      </c>
-      <c r="P29">
-        <v>107.82295497181678</v>
+        <v>5.1146750325636835E-2</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.45">
@@ -1347,31 +1323,47 @@
         <v>16</v>
       </c>
       <c r="B30" s="1">
-        <v>45288</v>
+        <v>45279</v>
       </c>
       <c r="C30">
-        <v>586.5</v>
+        <v>462</v>
       </c>
       <c r="D30">
-        <v>12.2</v>
+        <v>10.15</v>
+      </c>
+      <c r="E30">
+        <v>21.25</v>
       </c>
       <c r="F30">
-        <v>2.1000585963396539</v>
+        <v>0.90377009469093894</v>
       </c>
       <c r="G30">
-        <v>0.16175497233014249</v>
+        <v>0.17957612594849667</v>
+      </c>
+      <c r="H30">
+        <f>F30/M30</f>
+        <v>1.4968551468417543E-2</v>
       </c>
       <c r="I30">
-        <v>0.61923076923076925</v>
+        <v>0.40192307692307694</v>
       </c>
       <c r="J30">
-        <v>5.8313123992568404E-2</v>
+        <v>5.4543711246622169E-2</v>
       </c>
       <c r="K30">
-        <v>183.81666666666663</v>
-      </c>
-      <c r="L30" s="2">
-        <v>185.81666666666663</v>
+        <v>158.51666666666665</v>
+      </c>
+      <c r="L30">
+        <v>137.65</v>
+      </c>
+      <c r="M30">
+        <v>60.377926120494841</v>
+      </c>
+      <c r="N30">
+        <v>47.44502885132195</v>
+      </c>
+      <c r="P30">
+        <v>107.82295497181678</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.45">
@@ -1379,44 +1371,31 @@
         <v>16</v>
       </c>
       <c r="B31" s="1">
-        <v>45296</v>
+        <v>45288</v>
       </c>
       <c r="C31">
-        <v>793</v>
-      </c>
-      <c r="E31">
-        <v>40</v>
+        <v>586.5</v>
+      </c>
+      <c r="D31">
+        <v>12.2</v>
       </c>
       <c r="F31">
-        <v>3.0317071477592523</v>
+        <v>2.1000585963396539</v>
       </c>
       <c r="G31">
-        <v>0.33366923094714623</v>
-      </c>
-      <c r="H31">
-        <f>F31/M31</f>
-        <v>2.1060960200872104E-2</v>
+        <v>0.16175497233014249</v>
       </c>
       <c r="I31">
-        <v>0.76298076923076918</v>
+        <v>0.61923076923076925</v>
       </c>
       <c r="J31">
-        <v>7.3246859198435113E-2</v>
+        <v>5.8313123992568404E-2</v>
       </c>
       <c r="K31">
-        <v>174.58333333333334</v>
+        <v>183.81666666666663</v>
       </c>
       <c r="L31" s="2">
-        <v>149.88333333333335</v>
-      </c>
-      <c r="M31">
-        <v>143.94914186456293</v>
-      </c>
-      <c r="N31">
-        <v>181.99552389227946</v>
-      </c>
-      <c r="P31">
-        <v>325.94466575684237</v>
+        <v>185.81666666666663</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.45">
@@ -1424,19 +1403,44 @@
         <v>16</v>
       </c>
       <c r="B32" s="1">
-        <v>45302</v>
+        <v>45296</v>
       </c>
       <c r="C32">
-        <v>956.5</v>
-      </c>
-      <c r="D32">
-        <v>16.2</v>
+        <v>793</v>
+      </c>
+      <c r="E32">
+        <v>40</v>
+      </c>
+      <c r="F32">
+        <v>3.0317071477592523</v>
+      </c>
+      <c r="G32">
+        <v>0.33366923094714623</v>
+      </c>
+      <c r="H32">
+        <f>F32/M32</f>
+        <v>2.1060960200872104E-2</v>
       </c>
       <c r="I32">
-        <v>0.86442307692307696</v>
+        <v>0.76298076923076918</v>
       </c>
       <c r="J32">
-        <v>5.5622450987683897E-2</v>
+        <v>7.3246859198435113E-2</v>
+      </c>
+      <c r="K32">
+        <v>174.58333333333334</v>
+      </c>
+      <c r="L32" s="2">
+        <v>149.88333333333335</v>
+      </c>
+      <c r="M32">
+        <v>143.94914186456293</v>
+      </c>
+      <c r="N32">
+        <v>181.99552389227946</v>
+      </c>
+      <c r="P32">
+        <v>325.94466575684237</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.45">
@@ -1444,22 +1448,19 @@
         <v>16</v>
       </c>
       <c r="B33" s="1">
-        <v>45306</v>
+        <v>45302</v>
       </c>
       <c r="C33">
-        <v>1006</v>
+        <v>956.5</v>
+      </c>
+      <c r="D33">
+        <v>16.2</v>
       </c>
       <c r="I33">
-        <v>0.9259615384615385</v>
+        <v>0.86442307692307696</v>
       </c>
       <c r="J33">
-        <v>4.7935013232664241E-2</v>
-      </c>
-      <c r="K33">
-        <v>133.11666666666665</v>
-      </c>
-      <c r="L33" s="2">
-        <v>100.80000000000001</v>
+        <v>5.5622450987683897E-2</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.45">
@@ -1467,35 +1468,22 @@
         <v>16</v>
       </c>
       <c r="B34" s="1">
-        <v>45307</v>
-      </c>
-      <c r="D34">
-        <v>17</v>
-      </c>
-      <c r="E34">
-        <v>54.5</v>
-      </c>
-      <c r="F34">
-        <v>4.0425206810776277</v>
-      </c>
-      <c r="G34">
-        <v>0.37827040810057388</v>
-      </c>
-      <c r="H34">
-        <f>F34/M34</f>
-        <v>1.8643711192968791E-2</v>
-      </c>
-      <c r="M34">
-        <v>216.8302565533308</v>
-      </c>
-      <c r="N34">
-        <v>304.20829456947212</v>
-      </c>
-      <c r="O34">
-        <v>35.676835928243406</v>
-      </c>
-      <c r="P34">
-        <v>556.71538705104638</v>
+        <v>45306</v>
+      </c>
+      <c r="C34">
+        <v>1006</v>
+      </c>
+      <c r="I34">
+        <v>0.9259615384615385</v>
+      </c>
+      <c r="J34">
+        <v>4.7935013232664241E-2</v>
+      </c>
+      <c r="K34">
+        <v>133.11666666666665</v>
+      </c>
+      <c r="L34" s="2">
+        <v>100.80000000000001</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.45">
@@ -1503,25 +1491,35 @@
         <v>16</v>
       </c>
       <c r="B35" s="1">
-        <v>45314</v>
-      </c>
-      <c r="C35">
-        <v>1191.5</v>
+        <v>45307</v>
       </c>
       <c r="D35">
-        <v>18.25</v>
-      </c>
-      <c r="I35">
-        <v>0.9802884615384615</v>
-      </c>
-      <c r="J35">
-        <v>6.4726008422452033E-2</v>
-      </c>
-      <c r="K35">
-        <v>150.83333333333334</v>
-      </c>
-      <c r="L35">
-        <v>119.81666666666666</v>
+        <v>17</v>
+      </c>
+      <c r="E35">
+        <v>54.5</v>
+      </c>
+      <c r="F35">
+        <v>4.0425206810776277</v>
+      </c>
+      <c r="G35">
+        <v>0.37827040810057388</v>
+      </c>
+      <c r="H35">
+        <f>F35/M35</f>
+        <v>1.8643711192968791E-2</v>
+      </c>
+      <c r="M35">
+        <v>216.8302565533308</v>
+      </c>
+      <c r="N35">
+        <v>304.20829456947212</v>
+      </c>
+      <c r="O35">
+        <v>35.676835928243406</v>
+      </c>
+      <c r="P35">
+        <v>556.71538705104638</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.45">
@@ -1529,13 +1527,25 @@
         <v>16</v>
       </c>
       <c r="B36" s="1">
-        <v>45323</v>
+        <v>45314</v>
+      </c>
+      <c r="C36">
+        <v>1191.5</v>
+      </c>
+      <c r="D36">
+        <v>18.25</v>
+      </c>
+      <c r="I36">
+        <v>0.9802884615384615</v>
+      </c>
+      <c r="J36">
+        <v>6.4726008422452033E-2</v>
       </c>
       <c r="K36">
-        <v>188.48333333333335</v>
+        <v>150.83333333333334</v>
       </c>
       <c r="L36">
-        <v>172.45000000000005</v>
+        <v>119.81666666666666</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.45">
@@ -1543,63 +1553,77 @@
         <v>16</v>
       </c>
       <c r="B37" s="1">
-        <v>45331</v>
-      </c>
-      <c r="F37">
-        <v>5.5032705000000002</v>
-      </c>
-      <c r="G37">
-        <v>1.6615774246742543E-2</v>
+        <v>45323</v>
       </c>
       <c r="K37">
-        <v>165.13333333333333</v>
+        <v>188.48333333333335</v>
       </c>
       <c r="L37">
-        <v>133.63333333333333</v>
+        <v>172.45000000000005</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="3">
-        <v>45335</v>
-      </c>
-      <c r="K38" s="2">
-        <v>146.33333333333334</v>
+      <c r="B38" s="1">
+        <v>45331</v>
+      </c>
+      <c r="F38">
+        <v>5.5032705000000002</v>
+      </c>
+      <c r="G38">
+        <v>1.6615774246742543E-2</v>
+      </c>
+      <c r="K38">
+        <v>165.13333333333333</v>
       </c>
       <c r="L38">
-        <v>103.91666666666669</v>
+        <v>133.63333333333333</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>16</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="3">
+        <v>45335</v>
+      </c>
+      <c r="K39" s="2">
+        <v>146.33333333333334</v>
+      </c>
+      <c r="L39">
+        <v>103.91666666666669</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" s="1">
         <v>45345</v>
       </c>
-      <c r="C39">
+      <c r="C40">
         <v>1375</v>
       </c>
-      <c r="F39">
+      <c r="F40">
         <v>6.2965385000000005</v>
       </c>
-      <c r="G39">
+      <c r="G40">
         <v>0.3468610456650591</v>
       </c>
-      <c r="K39" s="2">
+      <c r="K40" s="2">
         <v>126.25000000000001</v>
       </c>
-      <c r="L39">
+      <c r="L40">
         <v>83.516666666666666</v>
       </c>
     </row>
-    <row r="1659" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="1660" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1637:EQ1816">
-    <sortCondition ref="B2:B2267"/>
-    <sortCondition ref="C2:C2267"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1638:EQ1817">
+    <sortCondition ref="B2:B2268"/>
+    <sortCondition ref="C2:C2268"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add some canopy data
</commit_message>
<xml_diff>
--- a/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
+++ b/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Prototypes\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440A839D-2AA2-4428-B677-34BF749BC53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DAD8F0-50CD-4AB1-BB40-C00263FDDB77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="19">
   <si>
     <t>SimulationName</t>
   </si>
@@ -450,10 +450,10 @@
   <dimension ref="A1:Q1660"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="9980" ySplit="770" activePane="bottomRight"/>
+      <pane xSplit="9980" ySplit="770" activePane="bottomLeft"/>
       <selection sqref="A1:A1048576"/>
       <selection pane="topRight" activeCell="Q2" sqref="Q2"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
+      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
       <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -1619,6 +1619,26 @@
         <v>83.516666666666666</v>
       </c>
     </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="1">
+        <v>45356</v>
+      </c>
+      <c r="D41">
+        <v>22.1</v>
+      </c>
+      <c r="E41">
+        <v>76.900000000000006</v>
+      </c>
+      <c r="F41">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="G41">
+        <v>0.16900000000000001</v>
+      </c>
+    </row>
     <row r="1660" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1638:EQ1817">

</xml_diff>

<commit_message>
Added biomass data from last 4-mar harvest
</commit_message>
<xml_diff>
--- a/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
+++ b/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Prototypes\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DAD8F0-50CD-4AB1-BB40-C00263FDDB77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337A8DCE-6AE1-4E67-A99F-84CD0FBAA806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
@@ -450,11 +450,11 @@
   <dimension ref="A1:Q1660"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="9980" ySplit="770" activePane="bottomLeft"/>
+      <pane xSplit="9980" ySplit="770" topLeftCell="L1" activePane="bottomRight"/>
       <selection sqref="A1:A1048576"/>
       <selection pane="topRight" activeCell="Q2" sqref="Q2"/>
       <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
-      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomRight" activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1156,7 +1156,22 @@
       <c r="I21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
-      <c r="N21" s="2"/>
+      <c r="M21">
+        <v>337.92520602731139</v>
+      </c>
+      <c r="N21">
+        <v>523.52460726068648</v>
+      </c>
+      <c r="O21">
+        <v>776.86871345544523</v>
+      </c>
+      <c r="P21">
+        <v>1638.318526743443</v>
+      </c>
+      <c r="Q21">
+        <f>O21*0.299</f>
+        <v>232.28374532317812</v>
+      </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
@@ -1443,7 +1458,7 @@
         <v>325.94466575684237</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -1463,7 +1478,7 @@
         <v>5.5622450987683897E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -1486,7 +1501,7 @@
         <v>100.80000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -1522,7 +1537,7 @@
         <v>556.71538705104638</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>16</v>
       </c>
@@ -1548,7 +1563,7 @@
         <v>119.81666666666666</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -1562,7 +1577,7 @@
         <v>172.45000000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -1582,7 +1597,7 @@
         <v>133.63333333333333</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>16</v>
       </c>
@@ -1596,7 +1611,7 @@
         <v>103.91666666666669</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>16</v>
       </c>
@@ -1619,7 +1634,7 @@
         <v>83.516666666666666</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -1637,6 +1652,22 @@
       </c>
       <c r="G41">
         <v>0.16900000000000001</v>
+      </c>
+      <c r="M41">
+        <v>294.8704949629435</v>
+      </c>
+      <c r="N41">
+        <v>516.04750033059599</v>
+      </c>
+      <c r="O41">
+        <v>670.32696541298287</v>
+      </c>
+      <c r="P41">
+        <v>1481.2449607065223</v>
+      </c>
+      <c r="Q41">
+        <f>O41*0.299</f>
+        <v>200.42776265848187</v>
       </c>
     </row>
     <row r="1660" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Add new EM data, extend met file to this sample date, and change clock to new sample date
</commit_message>
<xml_diff>
--- a/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
+++ b/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Prototypes\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337A8DCE-6AE1-4E67-A99F-84CD0FBAA806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB56620-E53C-46C0-9234-080816C948CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="CottonObserved" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CottonObserved!$A$1:$EQ$2581</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CottonObserved!$A$1:$EQ$2582</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="19">
   <si>
     <t>SimulationName</t>
   </si>
@@ -447,14 +447,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C911DF83-7300-4B7A-8A42-16858D40307A}">
-  <dimension ref="A1:Q1660"/>
+  <dimension ref="A1:Q1661"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="9980" ySplit="770" topLeftCell="L1" activePane="bottomRight"/>
+      <pane xSplit="9980" ySplit="770" topLeftCell="H3" activePane="bottomRight"/>
       <selection sqref="A1:A1048576"/>
       <selection pane="topRight" activeCell="Q2" sqref="Q2"/>
-      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
-      <selection pane="bottomRight" activeCell="P35" sqref="P35"/>
+      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
+      <selection pane="bottomRight" activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1175,16 +1175,17 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B22" s="1">
-        <v>45236</v>
-      </c>
-      <c r="K22">
-        <v>93.333333333333329</v>
+        <v>45365</v>
+      </c>
+      <c r="I22" s="2"/>
+      <c r="K22" s="2">
+        <v>133.20000000000002</v>
       </c>
       <c r="L22" s="2">
-        <v>82.300000000000011</v>
+        <v>108.51666666666667</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.45">
@@ -1192,13 +1193,13 @@
         <v>16</v>
       </c>
       <c r="B23" s="1">
-        <v>45243</v>
+        <v>45236</v>
       </c>
       <c r="K23">
-        <v>104.5</v>
+        <v>93.333333333333329</v>
       </c>
       <c r="L23" s="2">
-        <v>135.1</v>
+        <v>82.300000000000011</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.45">
@@ -1206,13 +1207,13 @@
         <v>16</v>
       </c>
       <c r="B24" s="1">
-        <v>45248</v>
+        <v>45243</v>
       </c>
       <c r="K24">
-        <v>124.35000000000002</v>
+        <v>104.5</v>
       </c>
       <c r="L24" s="2">
-        <v>158.38333333333333</v>
+        <v>135.1</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.45">
@@ -1220,19 +1221,13 @@
         <v>16</v>
       </c>
       <c r="B25" s="1">
-        <v>45254</v>
-      </c>
-      <c r="C25">
-        <v>70</v>
-      </c>
-      <c r="D25">
-        <v>1.2</v>
+        <v>45248</v>
       </c>
       <c r="K25">
-        <v>158.5</v>
+        <v>124.35000000000002</v>
       </c>
       <c r="L25" s="2">
-        <v>170.91666666666666</v>
+        <v>158.38333333333333</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.45">
@@ -1240,25 +1235,19 @@
         <v>16</v>
       </c>
       <c r="B26" s="1">
-        <v>45259</v>
+        <v>45254</v>
       </c>
       <c r="C26">
-        <v>122.5</v>
+        <v>70</v>
       </c>
       <c r="D26">
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="F26">
-        <v>0.10798078444273128</v>
-      </c>
-      <c r="G26">
-        <v>1.0286612192528072E-2</v>
+        <v>1.2</v>
       </c>
       <c r="K26">
-        <v>166.08333333333334</v>
+        <v>158.5</v>
       </c>
       <c r="L26" s="2">
-        <v>170.3</v>
+        <v>170.91666666666666</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.45">
@@ -1266,31 +1255,25 @@
         <v>16</v>
       </c>
       <c r="B27" s="1">
-        <v>45266</v>
+        <v>45259</v>
       </c>
       <c r="C27">
-        <v>249.5</v>
+        <v>122.5</v>
       </c>
       <c r="D27">
-        <v>5.4</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="F27">
-        <v>0.21781349165461303</v>
+        <v>0.10798078444273128</v>
       </c>
       <c r="G27">
-        <v>3.0473870842271603E-2</v>
-      </c>
-      <c r="I27">
-        <v>0.20528846153846153</v>
-      </c>
-      <c r="J27">
-        <v>3.5743400843100848E-2</v>
+        <v>1.0286612192528072E-2</v>
       </c>
       <c r="K27">
-        <v>182.61666666666667</v>
+        <v>166.08333333333334</v>
       </c>
       <c r="L27" s="2">
-        <v>167.28333333333333</v>
+        <v>170.3</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.45">
@@ -1298,25 +1281,31 @@
         <v>16</v>
       </c>
       <c r="B28" s="1">
-        <v>45273</v>
+        <v>45266</v>
       </c>
       <c r="C28">
-        <v>346.84210526315792</v>
+        <v>249.5</v>
       </c>
       <c r="D28">
-        <v>8.0526315789473681</v>
+        <v>5.4</v>
+      </c>
+      <c r="F28">
+        <v>0.21781349165461303</v>
+      </c>
+      <c r="G28">
+        <v>3.0473870842271603E-2</v>
       </c>
       <c r="I28">
-        <v>0.30819838056680166</v>
+        <v>0.20528846153846153</v>
       </c>
       <c r="J28">
-        <v>4.4581672466543681E-2</v>
+        <v>3.5743400843100848E-2</v>
       </c>
       <c r="K28">
-        <v>168.93333333333331</v>
+        <v>182.61666666666667</v>
       </c>
       <c r="L28" s="2">
-        <v>158.08333333333334</v>
+        <v>167.28333333333333</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.45">
@@ -1324,13 +1313,25 @@
         <v>16</v>
       </c>
       <c r="B29" s="1">
-        <v>45274</v>
-      </c>
-      <c r="F29">
-        <v>0.45692237396557861</v>
-      </c>
-      <c r="G29">
-        <v>5.1146750325636835E-2</v>
+        <v>45273</v>
+      </c>
+      <c r="C29">
+        <v>346.84210526315792</v>
+      </c>
+      <c r="D29">
+        <v>8.0526315789473681</v>
+      </c>
+      <c r="I29">
+        <v>0.30819838056680166</v>
+      </c>
+      <c r="J29">
+        <v>4.4581672466543681E-2</v>
+      </c>
+      <c r="K29">
+        <v>168.93333333333331</v>
+      </c>
+      <c r="L29" s="2">
+        <v>158.08333333333334</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.45">
@@ -1338,47 +1339,13 @@
         <v>16</v>
       </c>
       <c r="B30" s="1">
-        <v>45279</v>
-      </c>
-      <c r="C30">
-        <v>462</v>
-      </c>
-      <c r="D30">
-        <v>10.15</v>
-      </c>
-      <c r="E30">
-        <v>21.25</v>
+        <v>45274</v>
       </c>
       <c r="F30">
-        <v>0.90377009469093894</v>
+        <v>0.45692237396557861</v>
       </c>
       <c r="G30">
-        <v>0.17957612594849667</v>
-      </c>
-      <c r="H30">
-        <f>F30/M30</f>
-        <v>1.4968551468417543E-2</v>
-      </c>
-      <c r="I30">
-        <v>0.40192307692307694</v>
-      </c>
-      <c r="J30">
-        <v>5.4543711246622169E-2</v>
-      </c>
-      <c r="K30">
-        <v>158.51666666666665</v>
-      </c>
-      <c r="L30">
-        <v>137.65</v>
-      </c>
-      <c r="M30">
-        <v>60.377926120494841</v>
-      </c>
-      <c r="N30">
-        <v>47.44502885132195</v>
-      </c>
-      <c r="P30">
-        <v>107.82295497181678</v>
+        <v>5.1146750325636835E-2</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.45">
@@ -1386,31 +1353,47 @@
         <v>16</v>
       </c>
       <c r="B31" s="1">
-        <v>45288</v>
+        <v>45279</v>
       </c>
       <c r="C31">
-        <v>586.5</v>
+        <v>462</v>
       </c>
       <c r="D31">
-        <v>12.2</v>
+        <v>10.15</v>
+      </c>
+      <c r="E31">
+        <v>21.25</v>
       </c>
       <c r="F31">
-        <v>2.1000585963396539</v>
+        <v>0.90377009469093894</v>
       </c>
       <c r="G31">
-        <v>0.16175497233014249</v>
+        <v>0.17957612594849667</v>
+      </c>
+      <c r="H31">
+        <f>F31/M31</f>
+        <v>1.4968551468417543E-2</v>
       </c>
       <c r="I31">
-        <v>0.61923076923076925</v>
+        <v>0.40192307692307694</v>
       </c>
       <c r="J31">
-        <v>5.8313123992568404E-2</v>
+        <v>5.4543711246622169E-2</v>
       </c>
       <c r="K31">
-        <v>183.81666666666663</v>
-      </c>
-      <c r="L31" s="2">
-        <v>185.81666666666663</v>
+        <v>158.51666666666665</v>
+      </c>
+      <c r="L31">
+        <v>137.65</v>
+      </c>
+      <c r="M31">
+        <v>60.377926120494841</v>
+      </c>
+      <c r="N31">
+        <v>47.44502885132195</v>
+      </c>
+      <c r="P31">
+        <v>107.82295497181678</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.45">
@@ -1418,44 +1401,31 @@
         <v>16</v>
       </c>
       <c r="B32" s="1">
-        <v>45296</v>
+        <v>45288</v>
       </c>
       <c r="C32">
-        <v>793</v>
-      </c>
-      <c r="E32">
-        <v>40</v>
+        <v>586.5</v>
+      </c>
+      <c r="D32">
+        <v>12.2</v>
       </c>
       <c r="F32">
-        <v>3.0317071477592523</v>
+        <v>2.1000585963396539</v>
       </c>
       <c r="G32">
-        <v>0.33366923094714623</v>
-      </c>
-      <c r="H32">
-        <f>F32/M32</f>
-        <v>2.1060960200872104E-2</v>
+        <v>0.16175497233014249</v>
       </c>
       <c r="I32">
-        <v>0.76298076923076918</v>
+        <v>0.61923076923076925</v>
       </c>
       <c r="J32">
-        <v>7.3246859198435113E-2</v>
+        <v>5.8313123992568404E-2</v>
       </c>
       <c r="K32">
-        <v>174.58333333333334</v>
+        <v>183.81666666666663</v>
       </c>
       <c r="L32" s="2">
-        <v>149.88333333333335</v>
-      </c>
-      <c r="M32">
-        <v>143.94914186456293</v>
-      </c>
-      <c r="N32">
-        <v>181.99552389227946</v>
-      </c>
-      <c r="P32">
-        <v>325.94466575684237</v>
+        <v>185.81666666666663</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.45">
@@ -1463,19 +1433,44 @@
         <v>16</v>
       </c>
       <c r="B33" s="1">
-        <v>45302</v>
+        <v>45296</v>
       </c>
       <c r="C33">
-        <v>956.5</v>
-      </c>
-      <c r="D33">
-        <v>16.2</v>
+        <v>793</v>
+      </c>
+      <c r="E33">
+        <v>40</v>
+      </c>
+      <c r="F33">
+        <v>3.0317071477592523</v>
+      </c>
+      <c r="G33">
+        <v>0.33366923094714623</v>
+      </c>
+      <c r="H33">
+        <f>F33/M33</f>
+        <v>2.1060960200872104E-2</v>
       </c>
       <c r="I33">
-        <v>0.86442307692307696</v>
+        <v>0.76298076923076918</v>
       </c>
       <c r="J33">
-        <v>5.5622450987683897E-2</v>
+        <v>7.3246859198435113E-2</v>
+      </c>
+      <c r="K33">
+        <v>174.58333333333334</v>
+      </c>
+      <c r="L33" s="2">
+        <v>149.88333333333335</v>
+      </c>
+      <c r="M33">
+        <v>143.94914186456293</v>
+      </c>
+      <c r="N33">
+        <v>181.99552389227946</v>
+      </c>
+      <c r="P33">
+        <v>325.94466575684237</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.45">
@@ -1483,22 +1478,19 @@
         <v>16</v>
       </c>
       <c r="B34" s="1">
-        <v>45306</v>
+        <v>45302</v>
       </c>
       <c r="C34">
-        <v>1006</v>
+        <v>956.5</v>
+      </c>
+      <c r="D34">
+        <v>16.2</v>
       </c>
       <c r="I34">
-        <v>0.9259615384615385</v>
+        <v>0.86442307692307696</v>
       </c>
       <c r="J34">
-        <v>4.7935013232664241E-2</v>
-      </c>
-      <c r="K34">
-        <v>133.11666666666665</v>
-      </c>
-      <c r="L34" s="2">
-        <v>100.80000000000001</v>
+        <v>5.5622450987683897E-2</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.45">
@@ -1506,35 +1498,22 @@
         <v>16</v>
       </c>
       <c r="B35" s="1">
-        <v>45307</v>
-      </c>
-      <c r="D35">
-        <v>17</v>
-      </c>
-      <c r="E35">
-        <v>54.5</v>
-      </c>
-      <c r="F35">
-        <v>4.0425206810776277</v>
-      </c>
-      <c r="G35">
-        <v>0.37827040810057388</v>
-      </c>
-      <c r="H35">
-        <f>F35/M35</f>
-        <v>1.8643711192968791E-2</v>
-      </c>
-      <c r="M35">
-        <v>216.8302565533308</v>
-      </c>
-      <c r="N35">
-        <v>304.20829456947212</v>
-      </c>
-      <c r="O35">
-        <v>35.676835928243406</v>
-      </c>
-      <c r="P35">
-        <v>556.71538705104638</v>
+        <v>45306</v>
+      </c>
+      <c r="C35">
+        <v>1006</v>
+      </c>
+      <c r="I35">
+        <v>0.9259615384615385</v>
+      </c>
+      <c r="J35">
+        <v>4.7935013232664241E-2</v>
+      </c>
+      <c r="K35">
+        <v>133.11666666666665</v>
+      </c>
+      <c r="L35" s="2">
+        <v>100.80000000000001</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.45">
@@ -1542,25 +1521,35 @@
         <v>16</v>
       </c>
       <c r="B36" s="1">
-        <v>45314</v>
-      </c>
-      <c r="C36">
-        <v>1191.5</v>
+        <v>45307</v>
       </c>
       <c r="D36">
-        <v>18.25</v>
-      </c>
-      <c r="I36">
-        <v>0.9802884615384615</v>
-      </c>
-      <c r="J36">
-        <v>6.4726008422452033E-2</v>
-      </c>
-      <c r="K36">
-        <v>150.83333333333334</v>
-      </c>
-      <c r="L36">
-        <v>119.81666666666666</v>
+        <v>17</v>
+      </c>
+      <c r="E36">
+        <v>54.5</v>
+      </c>
+      <c r="F36">
+        <v>4.0425206810776277</v>
+      </c>
+      <c r="G36">
+        <v>0.37827040810057388</v>
+      </c>
+      <c r="H36">
+        <f>F36/M36</f>
+        <v>1.8643711192968791E-2</v>
+      </c>
+      <c r="M36">
+        <v>216.8302565533308</v>
+      </c>
+      <c r="N36">
+        <v>304.20829456947212</v>
+      </c>
+      <c r="O36">
+        <v>35.676835928243406</v>
+      </c>
+      <c r="P36">
+        <v>556.71538705104638</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.45">
@@ -1568,13 +1557,25 @@
         <v>16</v>
       </c>
       <c r="B37" s="1">
-        <v>45323</v>
+        <v>45314</v>
+      </c>
+      <c r="C37">
+        <v>1191.5</v>
+      </c>
+      <c r="D37">
+        <v>18.25</v>
+      </c>
+      <c r="I37">
+        <v>0.9802884615384615</v>
+      </c>
+      <c r="J37">
+        <v>6.4726008422452033E-2</v>
       </c>
       <c r="K37">
-        <v>188.48333333333335</v>
+        <v>150.83333333333334</v>
       </c>
       <c r="L37">
-        <v>172.45000000000005</v>
+        <v>119.81666666666666</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.45">
@@ -1582,56 +1583,47 @@
         <v>16</v>
       </c>
       <c r="B38" s="1">
-        <v>45331</v>
-      </c>
-      <c r="F38">
-        <v>5.5032705000000002</v>
-      </c>
-      <c r="G38">
-        <v>1.6615774246742543E-2</v>
+        <v>45323</v>
       </c>
       <c r="K38">
-        <v>165.13333333333333</v>
+        <v>188.48333333333335</v>
       </c>
       <c r="L38">
-        <v>133.63333333333333</v>
+        <v>172.45000000000005</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>16</v>
       </c>
-      <c r="B39" s="3">
-        <v>45335</v>
-      </c>
-      <c r="K39" s="2">
-        <v>146.33333333333334</v>
+      <c r="B39" s="1">
+        <v>45331</v>
+      </c>
+      <c r="F39">
+        <v>5.5032705000000002</v>
+      </c>
+      <c r="G39">
+        <v>1.6615774246742543E-2</v>
+      </c>
+      <c r="K39">
+        <v>165.13333333333333</v>
       </c>
       <c r="L39">
-        <v>103.91666666666669</v>
+        <v>133.63333333333333</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>16</v>
       </c>
-      <c r="B40" s="1">
-        <v>45345</v>
-      </c>
-      <c r="C40">
-        <v>1375</v>
-      </c>
-      <c r="F40">
-        <v>6.2965385000000005</v>
-      </c>
-      <c r="G40">
-        <v>0.3468610456650591</v>
+      <c r="B40" s="3">
+        <v>45335</v>
       </c>
       <c r="K40" s="2">
-        <v>126.25000000000001</v>
+        <v>146.33333333333334</v>
       </c>
       <c r="L40">
-        <v>83.516666666666666</v>
+        <v>103.91666666666669</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.45">
@@ -1639,42 +1631,79 @@
         <v>16</v>
       </c>
       <c r="B41" s="1">
+        <v>45345</v>
+      </c>
+      <c r="C41">
+        <v>1375</v>
+      </c>
+      <c r="F41">
+        <v>6.2965385000000005</v>
+      </c>
+      <c r="G41">
+        <v>0.3468610456650591</v>
+      </c>
+      <c r="K41" s="2">
+        <v>126.25000000000001</v>
+      </c>
+      <c r="L41">
+        <v>83.516666666666666</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="1">
         <v>45356</v>
       </c>
-      <c r="D41">
+      <c r="D42">
         <v>22.1</v>
       </c>
-      <c r="E41">
+      <c r="E42">
         <v>76.900000000000006</v>
       </c>
-      <c r="F41">
+      <c r="F42">
         <v>4.8499999999999996</v>
       </c>
-      <c r="G41">
+      <c r="G42">
         <v>0.16900000000000001</v>
       </c>
-      <c r="M41">
+      <c r="M42">
         <v>294.8704949629435</v>
       </c>
-      <c r="N41">
+      <c r="N42">
         <v>516.04750033059599</v>
       </c>
-      <c r="O41">
+      <c r="O42">
         <v>670.32696541298287</v>
       </c>
-      <c r="P41">
+      <c r="P42">
         <v>1481.2449607065223</v>
       </c>
-      <c r="Q41">
-        <f>O41*0.299</f>
+      <c r="Q42">
+        <f>O42*0.299</f>
         <v>200.42776265848187</v>
       </c>
     </row>
-    <row r="1660" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="1">
+        <v>45365</v>
+      </c>
+      <c r="K43">
+        <v>84.583333333333343</v>
+      </c>
+      <c r="L43">
+        <v>48.733333333333341</v>
+      </c>
+    </row>
+    <row r="1661" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1638:EQ1817">
-    <sortCondition ref="B2:B2268"/>
-    <sortCondition ref="C2:C2268"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1639:EQ1818">
+    <sortCondition ref="B2:B2269"/>
+    <sortCondition ref="C2:C2269"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated Forest Hill test data with measurements from toda.
</commit_message>
<xml_diff>
--- a/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
+++ b/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Prototypes\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB56620-E53C-46C0-9234-080816C948CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65E47BE-07DB-408D-BCBF-3CC61E09A3A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="CottonObserved" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CottonObserved!$A$1:$EQ$2582</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CottonObserved!$A$1:$EQ$2583</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="19">
   <si>
     <t>SimulationName</t>
   </si>
@@ -56,15 +56,9 @@
     <t>Cotton.Leaf.LAI</t>
   </si>
   <si>
-    <t>Cotton.Leaf.LAIError</t>
-  </si>
-  <si>
     <t>Cotton.Leaf.CoverGreen</t>
   </si>
   <si>
-    <t>Cotton.Leaf.CoverGreenError</t>
-  </si>
-  <si>
     <t>EMCalculator.Script.EMv100</t>
   </si>
   <si>
@@ -93,6 +87,12 @@
   </si>
   <si>
     <t>Cotton.Bur.Wt</t>
+  </si>
+  <si>
+    <t>Cotton.Leaf.LAIErrorX</t>
+  </si>
+  <si>
+    <t>Cotton.Leaf.CoverGreenErrorX</t>
   </si>
 </sst>
 </file>
@@ -128,11 +128,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,14 +446,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C911DF83-7300-4B7A-8A42-16858D40307A}">
-  <dimension ref="A1:Q1661"/>
+  <dimension ref="A1:Q1662"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="9980" ySplit="770" topLeftCell="H3" activePane="bottomRight"/>
+      <pane xSplit="9980" ySplit="770" topLeftCell="D6" activePane="topRight"/>
       <selection sqref="A1:A1048576"/>
-      <selection pane="topRight" activeCell="Q2" sqref="Q2"/>
-      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
-      <selection pane="bottomRight" activeCell="K43" sqref="K43"/>
+      <selection pane="topRight" activeCell="J1" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
+      <selection pane="bottomRight" activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -601,48 +600,48 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
         <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
       </c>
       <c r="L1" t="s">
         <v>4</v>
       </c>
       <c r="M1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
       <c r="Q1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1">
         <v>45236</v>
@@ -656,7 +655,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1">
         <v>45243</v>
@@ -670,7 +669,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1">
         <v>45248</v>
@@ -684,7 +683,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1">
         <v>45254</v>
@@ -704,7 +703,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1">
         <v>45259</v>
@@ -730,7 +729,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1">
         <v>45266</v>
@@ -762,7 +761,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1">
         <v>45273</v>
@@ -791,7 +790,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1">
         <v>45274</v>
@@ -805,7 +804,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1">
         <v>45279</v>
@@ -849,7 +848,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1">
         <v>45288</v>
@@ -869,7 +868,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1">
         <v>45296</v>
@@ -914,7 +913,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1">
         <v>45302</v>
@@ -934,7 +933,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1">
         <v>45306</v>
@@ -957,7 +956,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1">
         <v>45307</v>
@@ -993,7 +992,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1">
         <v>45314</v>
@@ -1019,7 +1018,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17" s="1">
         <v>45323</v>
@@ -1074,7 +1073,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B18" s="1">
         <v>45331</v>
@@ -1095,7 +1094,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B19" s="1">
         <v>45335</v>
@@ -1111,7 +1110,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B20" s="1">
         <v>45345</v>
@@ -1136,7 +1135,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B21" s="1">
         <v>45355</v>
@@ -1175,7 +1174,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B22" s="1">
         <v>45365</v>
@@ -1190,520 +1189,579 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B23" s="1">
-        <v>45236</v>
-      </c>
-      <c r="K23">
-        <v>93.333333333333329</v>
+        <v>45385</v>
+      </c>
+      <c r="C23">
+        <v>1428.5</v>
+      </c>
+      <c r="D23">
+        <v>23.65</v>
+      </c>
+      <c r="E23">
+        <v>86.85</v>
+      </c>
+      <c r="F23">
+        <v>4.3250000000000002</v>
+      </c>
+      <c r="G23">
+        <v>0.11559999999999999</v>
+      </c>
+      <c r="I23" s="2"/>
+      <c r="K23" s="2">
+        <v>124.89999999999999</v>
       </c>
       <c r="L23" s="2">
-        <v>82.300000000000011</v>
+        <v>79.050000000000011</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B24" s="1">
-        <v>45243</v>
+        <v>45236</v>
       </c>
       <c r="K24">
-        <v>104.5</v>
+        <v>93.333333333333329</v>
       </c>
       <c r="L24" s="2">
-        <v>135.1</v>
+        <v>82.300000000000011</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B25" s="1">
-        <v>45248</v>
+        <v>45243</v>
       </c>
       <c r="K25">
-        <v>124.35000000000002</v>
+        <v>104.5</v>
       </c>
       <c r="L25" s="2">
-        <v>158.38333333333333</v>
+        <v>135.1</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B26" s="1">
-        <v>45254</v>
-      </c>
-      <c r="C26">
-        <v>70</v>
-      </c>
-      <c r="D26">
-        <v>1.2</v>
+        <v>45248</v>
       </c>
       <c r="K26">
-        <v>158.5</v>
+        <v>124.35000000000002</v>
       </c>
       <c r="L26" s="2">
-        <v>170.91666666666666</v>
+        <v>158.38333333333333</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B27" s="1">
-        <v>45259</v>
+        <v>45254</v>
       </c>
       <c r="C27">
-        <v>122.5</v>
+        <v>70</v>
       </c>
       <c r="D27">
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="F27">
-        <v>0.10798078444273128</v>
-      </c>
-      <c r="G27">
-        <v>1.0286612192528072E-2</v>
+        <v>1.2</v>
       </c>
       <c r="K27">
-        <v>166.08333333333334</v>
+        <v>158.5</v>
       </c>
       <c r="L27" s="2">
-        <v>170.3</v>
+        <v>170.91666666666666</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B28" s="1">
-        <v>45266</v>
+        <v>45259</v>
       </c>
       <c r="C28">
-        <v>249.5</v>
+        <v>122.5</v>
       </c>
       <c r="D28">
-        <v>5.4</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="F28">
-        <v>0.21781349165461303</v>
+        <v>0.10798078444273128</v>
       </c>
       <c r="G28">
-        <v>3.0473870842271603E-2</v>
-      </c>
-      <c r="I28">
-        <v>0.20528846153846153</v>
-      </c>
-      <c r="J28">
-        <v>3.5743400843100848E-2</v>
+        <v>1.0286612192528072E-2</v>
       </c>
       <c r="K28">
-        <v>182.61666666666667</v>
+        <v>166.08333333333334</v>
       </c>
       <c r="L28" s="2">
-        <v>167.28333333333333</v>
+        <v>170.3</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B29" s="1">
-        <v>45273</v>
+        <v>45266</v>
       </c>
       <c r="C29">
-        <v>346.84210526315792</v>
+        <v>249.5</v>
       </c>
       <c r="D29">
-        <v>8.0526315789473681</v>
+        <v>5.4</v>
+      </c>
+      <c r="F29">
+        <v>0.21781349165461303</v>
+      </c>
+      <c r="G29">
+        <v>3.0473870842271603E-2</v>
       </c>
       <c r="I29">
-        <v>0.30819838056680166</v>
+        <v>0.20528846153846153</v>
       </c>
       <c r="J29">
-        <v>4.4581672466543681E-2</v>
+        <v>3.5743400843100848E-2</v>
       </c>
       <c r="K29">
-        <v>168.93333333333331</v>
+        <v>182.61666666666667</v>
       </c>
       <c r="L29" s="2">
-        <v>158.08333333333334</v>
+        <v>167.28333333333333</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B30" s="1">
-        <v>45274</v>
-      </c>
-      <c r="F30">
-        <v>0.45692237396557861</v>
-      </c>
-      <c r="G30">
-        <v>5.1146750325636835E-2</v>
+        <v>45273</v>
+      </c>
+      <c r="C30">
+        <v>346.84210526315792</v>
+      </c>
+      <c r="D30">
+        <v>8.0526315789473681</v>
+      </c>
+      <c r="I30">
+        <v>0.30819838056680166</v>
+      </c>
+      <c r="J30">
+        <v>4.4581672466543681E-2</v>
+      </c>
+      <c r="K30">
+        <v>168.93333333333331</v>
+      </c>
+      <c r="L30" s="2">
+        <v>158.08333333333334</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B31" s="1">
-        <v>45279</v>
-      </c>
-      <c r="C31">
-        <v>462</v>
-      </c>
-      <c r="D31">
-        <v>10.15</v>
-      </c>
-      <c r="E31">
-        <v>21.25</v>
+        <v>45274</v>
       </c>
       <c r="F31">
-        <v>0.90377009469093894</v>
+        <v>0.45692237396557861</v>
       </c>
       <c r="G31">
-        <v>0.17957612594849667</v>
-      </c>
-      <c r="H31">
-        <f>F31/M31</f>
-        <v>1.4968551468417543E-2</v>
-      </c>
-      <c r="I31">
-        <v>0.40192307692307694</v>
-      </c>
-      <c r="J31">
-        <v>5.4543711246622169E-2</v>
-      </c>
-      <c r="K31">
-        <v>158.51666666666665</v>
-      </c>
-      <c r="L31">
-        <v>137.65</v>
-      </c>
-      <c r="M31">
-        <v>60.377926120494841</v>
-      </c>
-      <c r="N31">
-        <v>47.44502885132195</v>
-      </c>
-      <c r="P31">
-        <v>107.82295497181678</v>
+        <v>5.1146750325636835E-2</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B32" s="1">
-        <v>45288</v>
+        <v>45279</v>
       </c>
       <c r="C32">
-        <v>586.5</v>
+        <v>462</v>
       </c>
       <c r="D32">
-        <v>12.2</v>
+        <v>10.15</v>
+      </c>
+      <c r="E32">
+        <v>21.25</v>
       </c>
       <c r="F32">
-        <v>2.1000585963396539</v>
+        <v>0.90377009469093894</v>
       </c>
       <c r="G32">
-        <v>0.16175497233014249</v>
+        <v>0.17957612594849667</v>
+      </c>
+      <c r="H32">
+        <f>F32/M32</f>
+        <v>1.4968551468417543E-2</v>
       </c>
       <c r="I32">
-        <v>0.61923076923076925</v>
+        <v>0.40192307692307694</v>
       </c>
       <c r="J32">
-        <v>5.8313123992568404E-2</v>
+        <v>5.4543711246622169E-2</v>
       </c>
       <c r="K32">
-        <v>183.81666666666663</v>
-      </c>
-      <c r="L32" s="2">
-        <v>185.81666666666663</v>
+        <v>158.51666666666665</v>
+      </c>
+      <c r="L32">
+        <v>137.65</v>
+      </c>
+      <c r="M32">
+        <v>60.377926120494841</v>
+      </c>
+      <c r="N32">
+        <v>47.44502885132195</v>
+      </c>
+      <c r="P32">
+        <v>107.82295497181678</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B33" s="1">
-        <v>45296</v>
+        <v>45288</v>
       </c>
       <c r="C33">
-        <v>793</v>
-      </c>
-      <c r="E33">
-        <v>40</v>
+        <v>586.5</v>
+      </c>
+      <c r="D33">
+        <v>12.2</v>
       </c>
       <c r="F33">
-        <v>3.0317071477592523</v>
+        <v>2.1000585963396539</v>
       </c>
       <c r="G33">
-        <v>0.33366923094714623</v>
-      </c>
-      <c r="H33">
-        <f>F33/M33</f>
-        <v>2.1060960200872104E-2</v>
+        <v>0.16175497233014249</v>
       </c>
       <c r="I33">
-        <v>0.76298076923076918</v>
+        <v>0.61923076923076925</v>
       </c>
       <c r="J33">
-        <v>7.3246859198435113E-2</v>
+        <v>5.8313123992568404E-2</v>
       </c>
       <c r="K33">
-        <v>174.58333333333334</v>
+        <v>183.81666666666663</v>
       </c>
       <c r="L33" s="2">
-        <v>149.88333333333335</v>
-      </c>
-      <c r="M33">
-        <v>143.94914186456293</v>
-      </c>
-      <c r="N33">
-        <v>181.99552389227946</v>
-      </c>
-      <c r="P33">
-        <v>325.94466575684237</v>
+        <v>185.81666666666663</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B34" s="1">
-        <v>45302</v>
+        <v>45296</v>
       </c>
       <c r="C34">
-        <v>956.5</v>
-      </c>
-      <c r="D34">
-        <v>16.2</v>
+        <v>793</v>
+      </c>
+      <c r="E34">
+        <v>40</v>
+      </c>
+      <c r="F34">
+        <v>3.0317071477592523</v>
+      </c>
+      <c r="G34">
+        <v>0.33366923094714623</v>
+      </c>
+      <c r="H34">
+        <f>F34/M34</f>
+        <v>2.1060960200872104E-2</v>
       </c>
       <c r="I34">
-        <v>0.86442307692307696</v>
+        <v>0.76298076923076918</v>
       </c>
       <c r="J34">
-        <v>5.5622450987683897E-2</v>
+        <v>7.3246859198435113E-2</v>
+      </c>
+      <c r="K34">
+        <v>174.58333333333334</v>
+      </c>
+      <c r="L34" s="2">
+        <v>149.88333333333335</v>
+      </c>
+      <c r="M34">
+        <v>143.94914186456293</v>
+      </c>
+      <c r="N34">
+        <v>181.99552389227946</v>
+      </c>
+      <c r="P34">
+        <v>325.94466575684237</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B35" s="1">
-        <v>45306</v>
+        <v>45302</v>
       </c>
       <c r="C35">
-        <v>1006</v>
+        <v>956.5</v>
+      </c>
+      <c r="D35">
+        <v>16.2</v>
       </c>
       <c r="I35">
-        <v>0.9259615384615385</v>
+        <v>0.86442307692307696</v>
       </c>
       <c r="J35">
-        <v>4.7935013232664241E-2</v>
-      </c>
-      <c r="K35">
-        <v>133.11666666666665</v>
-      </c>
-      <c r="L35" s="2">
-        <v>100.80000000000001</v>
+        <v>5.5622450987683897E-2</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B36" s="1">
-        <v>45307</v>
-      </c>
-      <c r="D36">
-        <v>17</v>
-      </c>
-      <c r="E36">
-        <v>54.5</v>
-      </c>
-      <c r="F36">
-        <v>4.0425206810776277</v>
-      </c>
-      <c r="G36">
-        <v>0.37827040810057388</v>
-      </c>
-      <c r="H36">
-        <f>F36/M36</f>
-        <v>1.8643711192968791E-2</v>
-      </c>
-      <c r="M36">
-        <v>216.8302565533308</v>
-      </c>
-      <c r="N36">
-        <v>304.20829456947212</v>
-      </c>
-      <c r="O36">
-        <v>35.676835928243406</v>
-      </c>
-      <c r="P36">
-        <v>556.71538705104638</v>
+        <v>45306</v>
+      </c>
+      <c r="C36">
+        <v>1006</v>
+      </c>
+      <c r="I36">
+        <v>0.9259615384615385</v>
+      </c>
+      <c r="J36">
+        <v>4.7935013232664241E-2</v>
+      </c>
+      <c r="K36">
+        <v>133.11666666666665</v>
+      </c>
+      <c r="L36" s="2">
+        <v>100.80000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B37" s="1">
-        <v>45314</v>
-      </c>
-      <c r="C37">
-        <v>1191.5</v>
+        <v>45307</v>
       </c>
       <c r="D37">
-        <v>18.25</v>
-      </c>
-      <c r="I37">
-        <v>0.9802884615384615</v>
-      </c>
-      <c r="J37">
-        <v>6.4726008422452033E-2</v>
-      </c>
-      <c r="K37">
-        <v>150.83333333333334</v>
-      </c>
-      <c r="L37">
-        <v>119.81666666666666</v>
+        <v>17</v>
+      </c>
+      <c r="E37">
+        <v>54.5</v>
+      </c>
+      <c r="F37">
+        <v>4.0425206810776277</v>
+      </c>
+      <c r="G37">
+        <v>0.37827040810057388</v>
+      </c>
+      <c r="H37">
+        <f>F37/M37</f>
+        <v>1.8643711192968791E-2</v>
+      </c>
+      <c r="M37">
+        <v>216.8302565533308</v>
+      </c>
+      <c r="N37">
+        <v>304.20829456947212</v>
+      </c>
+      <c r="O37">
+        <v>35.676835928243406</v>
+      </c>
+      <c r="P37">
+        <v>556.71538705104638</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B38" s="1">
-        <v>45323</v>
+        <v>45314</v>
+      </c>
+      <c r="C38">
+        <v>1191.5</v>
+      </c>
+      <c r="D38">
+        <v>18.25</v>
+      </c>
+      <c r="I38">
+        <v>0.9802884615384615</v>
+      </c>
+      <c r="J38">
+        <v>6.4726008422452033E-2</v>
       </c>
       <c r="K38">
-        <v>188.48333333333335</v>
+        <v>150.83333333333334</v>
       </c>
       <c r="L38">
-        <v>172.45000000000005</v>
+        <v>119.81666666666666</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B39" s="1">
-        <v>45331</v>
-      </c>
-      <c r="F39">
-        <v>5.5032705000000002</v>
-      </c>
-      <c r="G39">
-        <v>1.6615774246742543E-2</v>
+        <v>45323</v>
       </c>
       <c r="K39">
-        <v>165.13333333333333</v>
+        <v>188.48333333333335</v>
       </c>
       <c r="L39">
-        <v>133.63333333333333</v>
+        <v>172.45000000000005</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>16</v>
-      </c>
-      <c r="B40" s="3">
-        <v>45335</v>
-      </c>
-      <c r="K40" s="2">
-        <v>146.33333333333334</v>
+        <v>14</v>
+      </c>
+      <c r="B40" s="1">
+        <v>45331</v>
+      </c>
+      <c r="F40">
+        <v>5.5032705000000002</v>
+      </c>
+      <c r="G40">
+        <v>1.6615774246742543E-2</v>
+      </c>
+      <c r="K40">
+        <v>165.13333333333333</v>
       </c>
       <c r="L40">
-        <v>103.91666666666669</v>
+        <v>133.63333333333333</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B41" s="1">
-        <v>45345</v>
-      </c>
-      <c r="C41">
-        <v>1375</v>
-      </c>
-      <c r="F41">
-        <v>6.2965385000000005</v>
-      </c>
-      <c r="G41">
-        <v>0.3468610456650591</v>
+        <v>45335</v>
       </c>
       <c r="K41" s="2">
-        <v>126.25000000000001</v>
+        <v>146.33333333333334</v>
       </c>
       <c r="L41">
-        <v>83.516666666666666</v>
+        <v>103.91666666666669</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B42" s="1">
-        <v>45356</v>
-      </c>
-      <c r="D42">
-        <v>22.1</v>
-      </c>
-      <c r="E42">
-        <v>76.900000000000006</v>
+        <v>45345</v>
+      </c>
+      <c r="C42">
+        <v>1375</v>
       </c>
       <c r="F42">
-        <v>4.8499999999999996</v>
+        <v>6.2965385000000005</v>
       </c>
       <c r="G42">
-        <v>0.16900000000000001</v>
-      </c>
-      <c r="M42">
-        <v>294.8704949629435</v>
-      </c>
-      <c r="N42">
-        <v>516.04750033059599</v>
-      </c>
-      <c r="O42">
-        <v>670.32696541298287</v>
-      </c>
-      <c r="P42">
-        <v>1481.2449607065223</v>
-      </c>
-      <c r="Q42">
-        <f>O42*0.299</f>
-        <v>200.42776265848187</v>
+        <v>0.3468610456650591</v>
+      </c>
+      <c r="K42" s="2">
+        <v>126.25000000000001</v>
+      </c>
+      <c r="L42">
+        <v>83.516666666666666</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B43" s="1">
+        <v>45356</v>
+      </c>
+      <c r="D43">
+        <v>22.1</v>
+      </c>
+      <c r="E43">
+        <v>76.900000000000006</v>
+      </c>
+      <c r="F43">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="G43">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="M43">
+        <v>294.8704949629435</v>
+      </c>
+      <c r="N43">
+        <v>516.04750033059599</v>
+      </c>
+      <c r="O43">
+        <v>670.32696541298287</v>
+      </c>
+      <c r="P43">
+        <v>1481.2449607065223</v>
+      </c>
+      <c r="Q43">
+        <f>O43*0.299</f>
+        <v>200.42776265848187</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44" s="1">
         <v>45365</v>
       </c>
-      <c r="K43">
+      <c r="K44">
         <v>84.583333333333343</v>
       </c>
-      <c r="L43">
+      <c r="L44">
         <v>48.733333333333341</v>
       </c>
     </row>
-    <row r="1661" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" s="1">
+        <v>45385</v>
+      </c>
+      <c r="C45">
+        <v>1319.5</v>
+      </c>
+      <c r="D45">
+        <v>21.75</v>
+      </c>
+      <c r="E45">
+        <v>71.599999999999994</v>
+      </c>
+      <c r="F45">
+        <v>2.8519999999999999</v>
+      </c>
+      <c r="G45">
+        <v>0.29970000000000002</v>
+      </c>
+      <c r="K45">
+        <v>82.983333333333334</v>
+      </c>
+      <c r="L45">
+        <v>62.15</v>
+      </c>
+    </row>
+    <row r="1662" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1639:EQ1818">
-    <sortCondition ref="B2:B2269"/>
-    <sortCondition ref="C2:C2269"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1640:EQ1819">
+    <sortCondition ref="B2:B2270"/>
+    <sortCondition ref="C2:C2270"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Last changes during Tiemen visit
</commit_message>
<xml_diff>
--- a/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
+++ b/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Prototypes\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65E47BE-07DB-408D-BCBF-3CC61E09A3A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7A1473-CFDB-4095-8969-E27CEAA5806C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
@@ -89,10 +89,10 @@
     <t>Cotton.Bur.Wt</t>
   </si>
   <si>
-    <t>Cotton.Leaf.LAIErrorX</t>
-  </si>
-  <si>
-    <t>Cotton.Leaf.CoverGreenErrorX</t>
+    <t>Cotton.Leaf.LAIError</t>
+  </si>
+  <si>
+    <t>Cotton.Leaf.CoverGreenError</t>
   </si>
 </sst>
 </file>
@@ -449,7 +449,7 @@
   <dimension ref="A1:Q1662"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="9980" ySplit="770" topLeftCell="D6" activePane="topRight"/>
+      <pane xSplit="9980" ySplit="770" topLeftCell="F6" activePane="topRight"/>
       <selection sqref="A1:A1048576"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>

</xml_diff>

<commit_message>
Add updated obs data
</commit_message>
<xml_diff>
--- a/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
+++ b/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Prototypes\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CE9457-79DF-4D5D-B411-7248D0D68478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02DB0E4-62FD-4EC9-A47C-030944571C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
+    <workbookView xWindow="47910" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
   <sheets>
     <sheet name="CottonObserved" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CottonObserved!$A$1:$EQ$2583</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CottonObserved!$A$1:$FC$2584</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="34">
   <si>
     <t>SimulationName</t>
   </si>
@@ -93,6 +93,51 @@
   </si>
   <si>
     <t>Cotton.Leaf.CoverGreenError</t>
+  </si>
+  <si>
+    <t>Cotton.Leaf.WtError</t>
+  </si>
+  <si>
+    <t>Cotton.Stem.WtError</t>
+  </si>
+  <si>
+    <t>Cotton.Boll.WtError</t>
+  </si>
+  <si>
+    <t>Cotton.AboveGround.WtError</t>
+  </si>
+  <si>
+    <t>Cotton.Bur.WtError</t>
+  </si>
+  <si>
+    <t>Cotton.Seed.Wt</t>
+  </si>
+  <si>
+    <t>Cotton.Seed.WtError</t>
+  </si>
+  <si>
+    <t>Cotton.Leaf.N</t>
+  </si>
+  <si>
+    <t>Cotton.Leaf.Nerror</t>
+  </si>
+  <si>
+    <t>Cotton.Leaf.Nconc</t>
+  </si>
+  <si>
+    <t>Cotton.Leaf.NConcError</t>
+  </si>
+  <si>
+    <t>Cotton.Stem.N</t>
+  </si>
+  <si>
+    <t>Cotton.Stem.Nerror</t>
+  </si>
+  <si>
+    <t>Cotton.Stem.Nconc</t>
+  </si>
+  <si>
+    <t>Cotton.Stem.NConcError</t>
   </si>
 </sst>
 </file>
@@ -446,99 +491,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C911DF83-7300-4B7A-8A42-16858D40307A}">
-  <dimension ref="A1:Q1662"/>
+  <dimension ref="A1:AF1663"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="9980" ySplit="770" topLeftCell="L6" activePane="bottomRight"/>
+      <pane xSplit="7020" ySplit="770" topLeftCell="T19" activePane="bottomRight"/>
       <selection sqref="A1:A1048576"/>
-      <selection pane="topRight" activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
-      <selection pane="bottomRight" activeCell="O23" sqref="O23"/>
+      <selection pane="topRight" activeCell="X1" sqref="X1"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomRight" activeCell="U46" sqref="U46:X47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="40.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.9296875" customWidth="1"/>
+    <col min="2" max="2" width="15.265625" customWidth="1"/>
     <col min="3" max="3" width="14.3984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.73046875" bestFit="1" customWidth="1"/>
     <col min="5" max="10" width="25.73046875" customWidth="1"/>
     <col min="11" max="11" width="38.1328125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24.06640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="36.265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="32.3984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="33.3984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.3984375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.86328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="27.1328125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="34.3984375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="32.3984375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="33.59765625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="30.265625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="34.1328125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="31.86328125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="35.59765625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.265625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="18" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="21.1328125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="16.73046875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="17.86328125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="24.73046875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="20.73046875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="26" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="24.86328125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="27.3984375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="16.73046875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="17.265625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="33.265625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="32.3984375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="32.86328125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="7.73046875" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="7.1328125" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="70" max="71" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="75" max="76" width="14.1328125" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="23" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="23" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="23" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="14" max="18" width="17.6640625" customWidth="1"/>
+    <col min="19" max="19" width="16" bestFit="1" customWidth="1"/>
+    <col min="20" max="24" width="16" customWidth="1"/>
+    <col min="25" max="25" width="32.3984375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="32.3984375" customWidth="1"/>
+    <col min="27" max="27" width="33.3984375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="33.3984375" customWidth="1"/>
+    <col min="29" max="29" width="20.3984375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.86328125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="27.1328125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="34.3984375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="32.3984375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="33.59765625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="30.265625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="34.1328125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="31.86328125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="35.59765625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="16.1328125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="18" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="21.1328125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="16.73046875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="24.73046875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="16.1328125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="17.59765625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="20.73046875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="26" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="24.86328125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="27.3984375" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="16.73046875" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="14.73046875" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="17.265625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="33.265625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="32.3984375" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="32.86328125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="14.73046875" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="7.1328125" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="16.1328125" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="82" max="83" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="12.86328125" bestFit="1" customWidth="1"/>
     <col min="85" max="85" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="23" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="17.59765625" bestFit="1" customWidth="1"/>
+    <col min="87" max="88" width="14.1328125" bestFit="1" customWidth="1"/>
     <col min="89" max="89" width="23" bestFit="1" customWidth="1"/>
     <col min="90" max="90" width="11.73046875" bestFit="1" customWidth="1"/>
     <col min="91" max="91" width="12.3984375" bestFit="1" customWidth="1"/>
@@ -554,39 +591,51 @@
     <col min="101" max="101" width="23" bestFit="1" customWidth="1"/>
     <col min="102" max="102" width="11.73046875" bestFit="1" customWidth="1"/>
     <col min="103" max="103" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="24" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="24" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="24" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="19" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="19" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="19" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="19" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="19" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="19" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="23" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="23" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="23" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="23" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="24" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="24" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="24" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="7.59765625" bestFit="1" customWidth="1"/>
     <col min="126" max="126" width="18.59765625" bestFit="1" customWidth="1"/>
     <col min="127" max="127" width="19" bestFit="1" customWidth="1"/>
     <col min="128" max="128" width="18.59765625" bestFit="1" customWidth="1"/>
     <col min="129" max="129" width="19" bestFit="1" customWidth="1"/>
-    <col min="130" max="130" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="131" max="138" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="139" max="139" width="6.1328125" bestFit="1" customWidth="1"/>
-    <col min="140" max="147" width="24.59765625" bestFit="1" customWidth="1"/>
+    <col min="130" max="130" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="19" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="19" bestFit="1" customWidth="1"/>
+    <col min="134" max="134" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="135" max="135" width="19" bestFit="1" customWidth="1"/>
+    <col min="136" max="136" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="137" max="137" width="19" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="139" max="139" width="19" bestFit="1" customWidth="1"/>
+    <col min="140" max="140" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="141" max="141" width="19" bestFit="1" customWidth="1"/>
+    <col min="142" max="142" width="7.59765625" bestFit="1" customWidth="1"/>
+    <col min="143" max="150" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="151" max="151" width="6.1328125" bestFit="1" customWidth="1"/>
+    <col min="152" max="159" width="24.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -627,19 +676,64 @@
         <v>9</v>
       </c>
       <c r="N1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" t="s">
+      <c r="T1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" t="s">
+        <v>30</v>
+      </c>
+      <c r="V1" t="s">
+        <v>31</v>
+      </c>
+      <c r="W1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Z1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="AB1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="AD1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -653,7 +747,7 @@
         <v>96.683333333333337</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -667,7 +761,7 @@
         <v>139.43333333333331</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -681,7 +775,7 @@
         <v>162.56666666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -701,7 +795,7 @@
         <v>183.21666666666667</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -727,7 +821,7 @@
         <v>172.93333333333331</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -759,7 +853,7 @@
         <v>192.94999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -788,7 +882,7 @@
         <v>161.20000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -802,7 +896,7 @@
         <v>3.605272908788857E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -840,13 +934,46 @@
         <v>61.869882044725493</v>
       </c>
       <c r="N10">
+        <v>9.8944061136249797</v>
+      </c>
+      <c r="O10">
+        <v>2.7791398409567232</v>
+      </c>
+      <c r="P10">
+        <v>0.51636545192196637</v>
+      </c>
+      <c r="Q10">
+        <v>4.4797499999999997E-2</v>
+      </c>
+      <c r="R10">
+        <v>2.5078194379448237E-3</v>
+      </c>
+      <c r="S10">
         <v>47.219165425471701</v>
       </c>
-      <c r="P10">
+      <c r="T10">
+        <v>8.1228456876960564</v>
+      </c>
+      <c r="U10">
+        <v>1.2118088803109981</v>
+      </c>
+      <c r="V10">
+        <v>0.18412828321885388</v>
+      </c>
+      <c r="W10">
+        <v>2.57275E-2</v>
+      </c>
+      <c r="X10">
+        <v>6.7158394858723817E-4</v>
+      </c>
+      <c r="AA10">
         <v>109.08904747019719</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="AB10">
+        <v>17.913790990518695</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -866,7 +993,7 @@
         <v>190.58333333333337</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -905,13 +1032,46 @@
         <v>148.32379686792672</v>
       </c>
       <c r="N12">
+        <v>6.8778449919180575</v>
+      </c>
+      <c r="O12">
+        <v>6.2119392764509858</v>
+      </c>
+      <c r="P12">
+        <v>0.43258397929577203</v>
+      </c>
+      <c r="Q12">
+        <v>4.1849999999999998E-2</v>
+      </c>
+      <c r="R12">
+        <v>1.1403800536080946E-3</v>
+      </c>
+      <c r="S12">
         <v>182.30627017799995</v>
       </c>
-      <c r="P12">
+      <c r="T12">
+        <v>22.665866039996502</v>
+      </c>
+      <c r="U12">
+        <v>3.5376681735872255</v>
+      </c>
+      <c r="V12">
+        <v>0.77283952257010957</v>
+      </c>
+      <c r="W12">
+        <v>1.9224999999999999E-2</v>
+      </c>
+      <c r="X12">
+        <v>2.2917606041353133E-3</v>
+      </c>
+      <c r="AA12">
         <v>330.63006704592664</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="AB12">
+        <v>29.284809478125943</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -931,7 +1091,7 @@
         <v>0.10013140610136738</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -954,7 +1114,7 @@
         <v>104.5</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -981,16 +1141,58 @@
         <v>235.61860053445332</v>
       </c>
       <c r="N15">
+        <v>27.886131015250321</v>
+      </c>
+      <c r="O15">
+        <v>9.3830195296014427</v>
+      </c>
+      <c r="P15">
+        <v>1.2147513729806729</v>
+      </c>
+      <c r="Q15">
+        <v>3.9805E-2</v>
+      </c>
+      <c r="R15">
+        <v>1.1691164755205162E-3</v>
+      </c>
+      <c r="S15">
         <v>329.13664247461998</v>
       </c>
-      <c r="O15">
+      <c r="T15">
+        <v>47.906275214333796</v>
+      </c>
+      <c r="U15">
+        <v>4.3640337069750732</v>
+      </c>
+      <c r="V15">
+        <v>1.0235305361576506</v>
+      </c>
+      <c r="W15">
+        <v>1.3165E-2</v>
+      </c>
+      <c r="X15">
+        <v>1.4221697038914437E-3</v>
+      </c>
+      <c r="Y15">
         <v>39.927173460593856</v>
       </c>
-      <c r="P15">
+      <c r="Z15">
+        <v>11.962135909923683</v>
+      </c>
+      <c r="AA15">
         <v>604.68241646966715</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="AB15">
+        <v>85.8105223676002</v>
+      </c>
+      <c r="AC15">
+        <v>26.970805672631151</v>
+      </c>
+      <c r="AD15">
+        <v>8.0804228071534308</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1016,7 +1218,7 @@
         <v>173.93333333333331</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1057,21 +1259,60 @@
       <c r="M17">
         <v>282.98</v>
       </c>
-      <c r="N17" s="2">
+      <c r="N17">
+        <v>14.343476168991488</v>
+      </c>
+      <c r="O17">
+        <v>10.735863447906745</v>
+      </c>
+      <c r="P17">
+        <v>1.0446586237321978</v>
+      </c>
+      <c r="Q17">
+        <v>3.7872499999999996E-2</v>
+      </c>
+      <c r="R17">
+        <v>1.876244031747204E-3</v>
+      </c>
+      <c r="S17" s="2">
         <v>425.3</v>
       </c>
-      <c r="O17">
+      <c r="T17">
+        <v>30.683746252519693</v>
+      </c>
+      <c r="U17">
+        <v>4.5787539320801187</v>
+      </c>
+      <c r="V17">
+        <v>0.56508636038383531</v>
+      </c>
+      <c r="W17">
+        <v>1.07435E-2</v>
+      </c>
+      <c r="X17">
+        <v>7.0551801299945712E-4</v>
+      </c>
+      <c r="Y17">
         <v>175.6</v>
       </c>
-      <c r="P17">
+      <c r="Z17">
+        <v>33.94794110158449</v>
+      </c>
+      <c r="AA17">
         <v>883.9</v>
       </c>
-      <c r="Q17">
-        <f>O17*0.4156</f>
+      <c r="AB17">
+        <v>74.99244449534504</v>
+      </c>
+      <c r="AC17">
+        <f>Y17*0.4156</f>
         <v>72.97936</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="AD17">
+        <v>14.108764321818526</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1092,7 +1333,7 @@
         <v>124.45</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1106,9 +1347,14 @@
       <c r="L19" s="2">
         <v>164.79999999999998</v>
       </c>
-      <c r="N19" s="2"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -1131,9 +1377,14 @@
       <c r="L20" s="2">
         <v>147.1142857142857</v>
       </c>
-      <c r="N20" s="2"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -1159,20 +1410,64 @@
         <v>337.92520602731139</v>
       </c>
       <c r="N21">
+        <v>26.271203900123851</v>
+      </c>
+      <c r="O21">
+        <v>11.867738993747693</v>
+      </c>
+      <c r="P21">
+        <v>1.2816402222262933</v>
+      </c>
+      <c r="Q21">
+        <v>3.5055000000000003E-2</v>
+      </c>
+      <c r="R21">
+        <v>1.2674515112355966E-3</v>
+      </c>
+      <c r="S21">
         <v>523.52460726068648</v>
       </c>
-      <c r="O21">
+      <c r="T21">
+        <v>44.994370618393809</v>
+      </c>
+      <c r="U21">
+        <v>4.8443436499220844</v>
+      </c>
+      <c r="V21">
+        <v>0.6925192542480183</v>
+      </c>
+      <c r="W21">
+        <v>9.2165000000000007E-3</v>
+      </c>
+      <c r="X21">
+        <v>5.799841951869511E-4</v>
+      </c>
+      <c r="Y21">
         <v>776.86871345544523</v>
       </c>
-      <c r="P21">
+      <c r="Z21">
+        <v>159.27897263639983</v>
+      </c>
+      <c r="AA21">
         <v>1638.318526743443</v>
       </c>
-      <c r="Q21">
-        <f>O21*0.299</f>
-        <v>232.28374532317812</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="AB21">
+        <v>221.32118746238078</v>
+      </c>
+      <c r="AC21">
+        <v>231.9729978377959</v>
+      </c>
+      <c r="AD21">
+        <v>47.560701229229082</v>
+      </c>
+      <c r="AE21">
+        <v>219.77615903654547</v>
+      </c>
+      <c r="AF21">
+        <v>45.060021358837425</v>
+      </c>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1187,7 +1482,7 @@
         <v>108.51666666666667</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1219,581 +1514,949 @@
       <c r="M23">
         <v>334.2</v>
       </c>
-      <c r="N23" s="2">
+      <c r="N23">
+        <v>13.419042646376479</v>
+      </c>
+      <c r="O23">
+        <v>11.559452469963013</v>
+      </c>
+      <c r="P23">
+        <v>1.0513685766398784</v>
+      </c>
+      <c r="Q23">
+        <v>3.4540000000000001E-2</v>
+      </c>
+      <c r="R23">
+        <v>1.9491536624904667E-3</v>
+      </c>
+      <c r="S23" s="2">
         <v>630.6</v>
       </c>
-      <c r="O23" s="2">
+      <c r="T23">
+        <v>59.199997434162121</v>
+      </c>
+      <c r="U23">
+        <v>7.1397333860757417</v>
+      </c>
+      <c r="V23">
+        <v>0.91414967363948718</v>
+      </c>
+      <c r="W23">
+        <v>1.1295000000000001E-2</v>
+      </c>
+      <c r="X23">
+        <v>4.5683695121998609E-4</v>
+      </c>
+      <c r="Y23" s="2">
         <v>855.7</v>
       </c>
-      <c r="P23" s="2">
+      <c r="Z23">
+        <v>91.695835177236717</v>
+      </c>
+      <c r="AA23" s="2">
         <v>1820.5</v>
       </c>
-      <c r="Q23">
-        <f>O23*0.219</f>
-        <v>187.39830000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="AB23">
+        <v>146.70194778841221</v>
+      </c>
+      <c r="AC23">
+        <v>187.39514354294664</v>
+      </c>
+      <c r="AD23">
+        <v>20.081387903815017</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B24" s="1">
-        <v>45236</v>
-      </c>
-      <c r="K24">
-        <v>93.333333333333329</v>
-      </c>
-      <c r="L24" s="2">
-        <v>82.300000000000011</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.45">
+        <v>45412</v>
+      </c>
+      <c r="I24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24">
+        <v>61.342563002639388</v>
+      </c>
+      <c r="N24">
+        <v>9.5391475995884676</v>
+      </c>
+      <c r="O24">
+        <v>1.9064599321036442</v>
+      </c>
+      <c r="P24">
+        <v>0.40026684732717238</v>
+      </c>
+      <c r="Q24">
+        <v>3.1032499999999998E-2</v>
+      </c>
+      <c r="R24">
+        <v>3.5977064453157925E-3</v>
+      </c>
+      <c r="S24">
+        <v>598.10592203032706</v>
+      </c>
+      <c r="T24">
+        <v>76.849771781065485</v>
+      </c>
+      <c r="U24">
+        <v>8.2327407991582557</v>
+      </c>
+      <c r="V24">
+        <v>1.7500727476286186</v>
+      </c>
+      <c r="W24">
+        <v>1.3667499999999999E-2</v>
+      </c>
+      <c r="X24">
+        <v>1.4249999999999914E-3</v>
+      </c>
+      <c r="Y24">
+        <v>832.08967648769135</v>
+      </c>
+      <c r="Z24">
+        <v>69.017440607751908</v>
+      </c>
+      <c r="AA24">
+        <v>1491.5381615206577</v>
+      </c>
+      <c r="AB24">
+        <v>137.01665077173698</v>
+      </c>
+      <c r="AC24">
+        <v>176.31980244774178</v>
+      </c>
+      <c r="AD24">
+        <v>14.624795664783132</v>
+      </c>
+      <c r="AE24">
+        <v>352.47318696018601</v>
+      </c>
+      <c r="AF24">
+        <v>29.235787841444349</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>14</v>
       </c>
       <c r="B25" s="1">
-        <v>45243</v>
+        <v>45236</v>
       </c>
       <c r="K25">
-        <v>104.5</v>
+        <v>93.333333333333329</v>
       </c>
       <c r="L25" s="2">
-        <v>135.1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.45">
+        <v>82.300000000000011</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>14</v>
       </c>
       <c r="B26" s="1">
-        <v>45248</v>
+        <v>45243</v>
       </c>
       <c r="K26">
-        <v>124.35000000000002</v>
+        <v>104.5</v>
       </c>
       <c r="L26" s="2">
-        <v>158.38333333333333</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.45">
+        <v>135.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>14</v>
       </c>
       <c r="B27" s="1">
-        <v>45254</v>
-      </c>
-      <c r="C27">
-        <v>70</v>
-      </c>
-      <c r="D27">
-        <v>1.2</v>
+        <v>45248</v>
       </c>
       <c r="K27">
-        <v>158.5</v>
+        <v>124.35000000000002</v>
       </c>
       <c r="L27" s="2">
-        <v>170.91666666666666</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.45">
+        <v>158.38333333333333</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>14</v>
       </c>
       <c r="B28" s="1">
-        <v>45259</v>
+        <v>45254</v>
       </c>
       <c r="C28">
-        <v>122.5</v>
+        <v>70</v>
       </c>
       <c r="D28">
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="F28">
-        <v>0.10798078444273128</v>
-      </c>
-      <c r="G28">
-        <v>1.0286612192528072E-2</v>
+        <v>1.2</v>
       </c>
       <c r="K28">
-        <v>166.08333333333334</v>
+        <v>158.5</v>
       </c>
       <c r="L28" s="2">
-        <v>170.3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.45">
+        <v>170.91666666666666</v>
+      </c>
+    </row>
+    <row r="29" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>14</v>
       </c>
       <c r="B29" s="1">
-        <v>45266</v>
+        <v>45259</v>
       </c>
       <c r="C29">
-        <v>249.5</v>
+        <v>122.5</v>
       </c>
       <c r="D29">
-        <v>5.4</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="F29">
-        <v>0.21781349165461303</v>
+        <v>0.10798078444273128</v>
       </c>
       <c r="G29">
-        <v>3.0473870842271603E-2</v>
-      </c>
-      <c r="I29">
-        <v>0.20528846153846153</v>
-      </c>
-      <c r="J29">
-        <v>3.5743400843100848E-2</v>
+        <v>1.0286612192528072E-2</v>
       </c>
       <c r="K29">
-        <v>182.61666666666667</v>
+        <v>166.08333333333334</v>
       </c>
       <c r="L29" s="2">
-        <v>167.28333333333333</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.45">
+        <v>170.3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>14</v>
       </c>
       <c r="B30" s="1">
-        <v>45273</v>
+        <v>45266</v>
       </c>
       <c r="C30">
-        <v>346.84210526315792</v>
+        <v>249.5</v>
       </c>
       <c r="D30">
-        <v>8.0526315789473681</v>
+        <v>5.4</v>
+      </c>
+      <c r="F30">
+        <v>0.21781349165461303</v>
+      </c>
+      <c r="G30">
+        <v>3.0473870842271603E-2</v>
       </c>
       <c r="I30">
-        <v>0.30819838056680166</v>
+        <v>0.20528846153846153</v>
       </c>
       <c r="J30">
-        <v>4.4581672466543681E-2</v>
+        <v>3.5743400843100848E-2</v>
       </c>
       <c r="K30">
-        <v>168.93333333333331</v>
+        <v>182.61666666666667</v>
       </c>
       <c r="L30" s="2">
-        <v>158.08333333333334</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.45">
+        <v>167.28333333333333</v>
+      </c>
+    </row>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>14</v>
       </c>
       <c r="B31" s="1">
-        <v>45274</v>
-      </c>
-      <c r="F31">
-        <v>0.45692237396557861</v>
-      </c>
-      <c r="G31">
-        <v>5.1146750325636835E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.45">
+        <v>45273</v>
+      </c>
+      <c r="C31">
+        <v>346.84210526315792</v>
+      </c>
+      <c r="D31">
+        <v>8.0526315789473681</v>
+      </c>
+      <c r="I31">
+        <v>0.30819838056680166</v>
+      </c>
+      <c r="J31">
+        <v>4.4581672466543681E-2</v>
+      </c>
+      <c r="K31">
+        <v>168.93333333333331</v>
+      </c>
+      <c r="L31" s="2">
+        <v>158.08333333333334</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>14</v>
       </c>
       <c r="B32" s="1">
-        <v>45279</v>
-      </c>
-      <c r="C32">
-        <v>462</v>
-      </c>
-      <c r="D32">
-        <v>10.15</v>
-      </c>
-      <c r="E32">
-        <v>21.25</v>
+        <v>45274</v>
       </c>
       <c r="F32">
-        <v>0.90377009469093894</v>
+        <v>0.45692237396557861</v>
       </c>
       <c r="G32">
-        <v>0.17957612594849667</v>
-      </c>
-      <c r="H32">
-        <f>F32/M32</f>
-        <v>1.4968551468417543E-2</v>
-      </c>
-      <c r="I32">
-        <v>0.40192307692307694</v>
-      </c>
-      <c r="J32">
-        <v>5.4543711246622169E-2</v>
-      </c>
-      <c r="K32">
-        <v>158.51666666666665</v>
-      </c>
-      <c r="L32">
-        <v>137.65</v>
-      </c>
-      <c r="M32">
-        <v>60.377926120494841</v>
-      </c>
-      <c r="N32">
-        <v>47.44502885132195</v>
-      </c>
-      <c r="P32">
-        <v>107.82295497181678</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.45">
+        <v>5.1146750325636835E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>14</v>
       </c>
       <c r="B33" s="1">
-        <v>45288</v>
+        <v>45279</v>
       </c>
       <c r="C33">
-        <v>586.5</v>
+        <v>462</v>
       </c>
       <c r="D33">
-        <v>12.2</v>
+        <v>10.15</v>
+      </c>
+      <c r="E33">
+        <v>21.25</v>
       </c>
       <c r="F33">
-        <v>2.1000585963396539</v>
+        <v>0.90377009469093894</v>
       </c>
       <c r="G33">
-        <v>0.16175497233014249</v>
+        <v>0.17957612594849667</v>
+      </c>
+      <c r="H33">
+        <f>F33/M33</f>
+        <v>1.4968551468417543E-2</v>
       </c>
       <c r="I33">
-        <v>0.61923076923076925</v>
+        <v>0.40192307692307694</v>
       </c>
       <c r="J33">
-        <v>5.8313123992568404E-2</v>
+        <v>5.4543711246622169E-2</v>
       </c>
       <c r="K33">
-        <v>183.81666666666663</v>
-      </c>
-      <c r="L33" s="2">
-        <v>185.81666666666663</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.45">
+        <v>158.51666666666665</v>
+      </c>
+      <c r="L33">
+        <v>137.65</v>
+      </c>
+      <c r="M33">
+        <v>60.377926120494841</v>
+      </c>
+      <c r="N33">
+        <v>8.9151821165985226</v>
+      </c>
+      <c r="O33">
+        <v>2.7682807975460642</v>
+      </c>
+      <c r="P33">
+        <v>0.45214771285279237</v>
+      </c>
+      <c r="Q33">
+        <v>4.5779999999999994E-2</v>
+      </c>
+      <c r="R33">
+        <v>1.0374969879476535E-3</v>
+      </c>
+      <c r="S33">
+        <v>47.44502885132195</v>
+      </c>
+      <c r="T33">
+        <v>7.0481501468892152</v>
+      </c>
+      <c r="U33">
+        <v>1.2646339945067164</v>
+      </c>
+      <c r="V33">
+        <v>0.13103404119087797</v>
+      </c>
+      <c r="W33">
+        <v>2.6789999999999998E-2</v>
+      </c>
+      <c r="X33">
+        <v>1.5500322577288762E-3</v>
+      </c>
+      <c r="AA33">
+        <v>107.82295497181678</v>
+      </c>
+      <c r="AB33">
+        <v>15.816021408416001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>14</v>
       </c>
       <c r="B34" s="1">
-        <v>45296</v>
+        <v>45288</v>
       </c>
       <c r="C34">
-        <v>793</v>
-      </c>
-      <c r="E34">
-        <v>40</v>
+        <v>586.5</v>
+      </c>
+      <c r="D34">
+        <v>12.2</v>
       </c>
       <c r="F34">
-        <v>3.0317071477592523</v>
+        <v>2.1000585963396539</v>
       </c>
       <c r="G34">
-        <v>0.33366923094714623</v>
-      </c>
-      <c r="H34">
-        <f>F34/M34</f>
-        <v>2.1060960200872104E-2</v>
+        <v>0.16175497233014249</v>
       </c>
       <c r="I34">
-        <v>0.76298076923076918</v>
+        <v>0.61923076923076925</v>
       </c>
       <c r="J34">
-        <v>7.3246859198435113E-2</v>
+        <v>5.8313123992568404E-2</v>
       </c>
       <c r="K34">
-        <v>174.58333333333334</v>
+        <v>183.81666666666663</v>
       </c>
       <c r="L34" s="2">
-        <v>149.88333333333335</v>
-      </c>
-      <c r="M34">
-        <v>143.94914186456293</v>
-      </c>
-      <c r="N34">
-        <v>181.99552389227946</v>
-      </c>
-      <c r="P34">
-        <v>325.94466575684237</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.45">
+        <v>185.81666666666663</v>
+      </c>
+    </row>
+    <row r="35" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>14</v>
       </c>
       <c r="B35" s="1">
-        <v>45302</v>
+        <v>45296</v>
       </c>
       <c r="C35">
-        <v>956.5</v>
-      </c>
-      <c r="D35">
-        <v>16.2</v>
+        <v>793</v>
+      </c>
+      <c r="E35">
+        <v>40</v>
+      </c>
+      <c r="F35">
+        <v>3.0317071477592523</v>
+      </c>
+      <c r="G35">
+        <v>0.33366923094714623</v>
+      </c>
+      <c r="H35">
+        <f>F35/M35</f>
+        <v>2.1060960200872104E-2</v>
       </c>
       <c r="I35">
-        <v>0.86442307692307696</v>
+        <v>0.76298076923076918</v>
       </c>
       <c r="J35">
-        <v>5.5622450987683897E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.45">
+        <v>7.3246859198435113E-2</v>
+      </c>
+      <c r="K35">
+        <v>174.58333333333334</v>
+      </c>
+      <c r="L35" s="2">
+        <v>149.88333333333335</v>
+      </c>
+      <c r="M35">
+        <v>143.94914186456293</v>
+      </c>
+      <c r="N35">
+        <v>14.304627948968733</v>
+      </c>
+      <c r="O35">
+        <v>5.9658226694967524</v>
+      </c>
+      <c r="P35">
+        <v>0.62857236489966073</v>
+      </c>
+      <c r="Q35">
+        <v>4.1440000000000005E-2</v>
+      </c>
+      <c r="R35">
+        <v>1.2549103553637813E-3</v>
+      </c>
+      <c r="S35">
+        <v>181.99552389227946</v>
+      </c>
+      <c r="T35">
+        <v>19.022103704598056</v>
+      </c>
+      <c r="U35">
+        <v>3.2982286229974349</v>
+      </c>
+      <c r="V35">
+        <v>0.53250200411833715</v>
+      </c>
+      <c r="W35">
+        <v>1.805E-2</v>
+      </c>
+      <c r="X35">
+        <v>1.1323721414211428E-3</v>
+      </c>
+      <c r="AA35">
+        <v>325.94466575684237</v>
+      </c>
+      <c r="AB35">
+        <v>32.992140008724505</v>
+      </c>
+    </row>
+    <row r="36" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>14</v>
       </c>
       <c r="B36" s="1">
-        <v>45306</v>
+        <v>45302</v>
       </c>
       <c r="C36">
-        <v>1006</v>
+        <v>956.5</v>
+      </c>
+      <c r="D36">
+        <v>16.2</v>
       </c>
       <c r="I36">
-        <v>0.9259615384615385</v>
+        <v>0.86442307692307696</v>
       </c>
       <c r="J36">
-        <v>4.7935013232664241E-2</v>
-      </c>
-      <c r="K36">
-        <v>133.11666666666665</v>
-      </c>
-      <c r="L36" s="2">
-        <v>100.80000000000001</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.45">
+        <v>5.5622450987683897E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>14</v>
       </c>
       <c r="B37" s="1">
-        <v>45307</v>
-      </c>
-      <c r="D37">
-        <v>17</v>
-      </c>
-      <c r="E37">
-        <v>54.5</v>
-      </c>
-      <c r="F37">
-        <v>4.0425206810776277</v>
-      </c>
-      <c r="G37">
-        <v>0.37827040810057388</v>
-      </c>
-      <c r="H37">
-        <f>F37/M37</f>
-        <v>1.8643711192968791E-2</v>
-      </c>
-      <c r="M37">
-        <v>216.8302565533308</v>
-      </c>
-      <c r="N37">
-        <v>304.20829456947212</v>
-      </c>
-      <c r="O37">
-        <v>35.676835928243406</v>
-      </c>
-      <c r="P37">
-        <v>556.71538705104638</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.45">
+        <v>45306</v>
+      </c>
+      <c r="C37">
+        <v>1006</v>
+      </c>
+      <c r="I37">
+        <v>0.9259615384615385</v>
+      </c>
+      <c r="J37">
+        <v>4.7935013232664241E-2</v>
+      </c>
+      <c r="K37">
+        <v>133.11666666666665</v>
+      </c>
+      <c r="L37" s="2">
+        <v>100.80000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>14</v>
       </c>
       <c r="B38" s="1">
-        <v>45314</v>
-      </c>
-      <c r="C38">
-        <v>1191.5</v>
+        <v>45307</v>
       </c>
       <c r="D38">
-        <v>18.25</v>
-      </c>
-      <c r="I38">
-        <v>0.9802884615384615</v>
-      </c>
-      <c r="J38">
-        <v>6.4726008422452033E-2</v>
-      </c>
-      <c r="K38">
-        <v>150.83333333333334</v>
-      </c>
-      <c r="L38">
-        <v>119.81666666666666</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.45">
+        <v>17</v>
+      </c>
+      <c r="E38">
+        <v>54.5</v>
+      </c>
+      <c r="F38">
+        <v>4.0425206810776277</v>
+      </c>
+      <c r="G38">
+        <v>0.37827040810057388</v>
+      </c>
+      <c r="H38">
+        <f>F38/M38</f>
+        <v>1.8643711192968791E-2</v>
+      </c>
+      <c r="M38">
+        <v>216.8302565533308</v>
+      </c>
+      <c r="N38">
+        <v>22.317232342008793</v>
+      </c>
+      <c r="O38">
+        <v>8.8264483099599538</v>
+      </c>
+      <c r="P38">
+        <v>1.0685174831378961</v>
+      </c>
+      <c r="Q38">
+        <v>4.0665E-2</v>
+      </c>
+      <c r="R38">
+        <v>1.8507025692963406E-3</v>
+      </c>
+      <c r="S38">
+        <v>304.20829456947212</v>
+      </c>
+      <c r="T38">
+        <v>33.049531593508924</v>
+      </c>
+      <c r="U38">
+        <v>4.2006012545515095</v>
+      </c>
+      <c r="V38">
+        <v>0.5042336240389429</v>
+      </c>
+      <c r="W38">
+        <v>1.3805E-2</v>
+      </c>
+      <c r="X38">
+        <v>7.4857642673723196E-4</v>
+      </c>
+      <c r="Y38">
+        <v>35.676835928243406</v>
+      </c>
+      <c r="Z38">
+        <v>4.2802524978283669</v>
+      </c>
+      <c r="AA38">
+        <v>556.71538705104638</v>
+      </c>
+      <c r="AB38">
+        <v>55.869701255861287</v>
+      </c>
+      <c r="AC38">
+        <v>24.099702669528423</v>
+      </c>
+      <c r="AD38">
+        <v>2.8913105622830111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>14</v>
       </c>
       <c r="B39" s="1">
-        <v>45323</v>
+        <v>45314</v>
+      </c>
+      <c r="C39">
+        <v>1191.5</v>
+      </c>
+      <c r="D39">
+        <v>18.25</v>
+      </c>
+      <c r="I39">
+        <v>0.9802884615384615</v>
+      </c>
+      <c r="J39">
+        <v>6.4726008422452033E-2</v>
       </c>
       <c r="K39">
-        <v>188.48333333333335</v>
+        <v>150.83333333333334</v>
       </c>
       <c r="L39">
-        <v>172.45000000000005</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.45">
+        <v>119.81666666666666</v>
+      </c>
+    </row>
+    <row r="40" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>14</v>
       </c>
       <c r="B40" s="1">
-        <v>45331</v>
-      </c>
-      <c r="F40">
-        <v>5.5032705000000002</v>
-      </c>
-      <c r="G40">
-        <v>1.6615774246742543E-2</v>
+        <v>45323</v>
       </c>
       <c r="K40">
-        <v>165.13333333333333</v>
+        <v>188.48333333333335</v>
       </c>
       <c r="L40">
-        <v>133.63333333333333</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.45">
+        <v>172.45000000000005</v>
+      </c>
+    </row>
+    <row r="41" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>14</v>
       </c>
       <c r="B41" s="1">
-        <v>45335</v>
-      </c>
-      <c r="K41" s="2">
-        <v>146.33333333333334</v>
+        <v>45331</v>
+      </c>
+      <c r="F41">
+        <v>5.5032705000000002</v>
+      </c>
+      <c r="G41">
+        <v>1.6615774246742543E-2</v>
+      </c>
+      <c r="K41">
+        <v>165.13333333333333</v>
       </c>
       <c r="L41">
-        <v>103.91666666666669</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.45">
+        <v>133.63333333333333</v>
+      </c>
+    </row>
+    <row r="42" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>14</v>
       </c>
       <c r="B42" s="1">
-        <v>45345</v>
-      </c>
-      <c r="C42">
-        <v>1375</v>
-      </c>
-      <c r="F42">
-        <v>6.2965385000000005</v>
-      </c>
-      <c r="G42">
-        <v>0.3468610456650591</v>
+        <v>45335</v>
       </c>
       <c r="K42" s="2">
-        <v>126.25000000000001</v>
+        <v>146.33333333333334</v>
       </c>
       <c r="L42">
-        <v>83.516666666666666</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.45">
+        <v>103.91666666666669</v>
+      </c>
+    </row>
+    <row r="43" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>14</v>
       </c>
       <c r="B43" s="1">
-        <v>45356</v>
-      </c>
-      <c r="D43">
-        <v>22.1</v>
-      </c>
-      <c r="E43">
-        <v>76.900000000000006</v>
+        <v>45345</v>
+      </c>
+      <c r="C43">
+        <v>1375</v>
       </c>
       <c r="F43">
-        <v>4.8499999999999996</v>
+        <v>6.2965385000000005</v>
       </c>
       <c r="G43">
-        <v>0.16900000000000001</v>
-      </c>
-      <c r="M43">
-        <v>294.8704949629435</v>
-      </c>
-      <c r="N43">
-        <v>516.04750033059599</v>
-      </c>
-      <c r="O43">
-        <v>670.32696541298287</v>
-      </c>
-      <c r="P43">
-        <v>1481.2449607065223</v>
-      </c>
-      <c r="Q43">
-        <f>O43*0.299</f>
-        <v>200.42776265848187</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.45">
+        <v>0.3468610456650591</v>
+      </c>
+      <c r="K43" s="2">
+        <v>126.25000000000001</v>
+      </c>
+      <c r="L43">
+        <v>83.516666666666666</v>
+      </c>
+    </row>
+    <row r="44" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>14</v>
       </c>
       <c r="B44" s="1">
-        <v>45365</v>
-      </c>
-      <c r="K44">
-        <v>84.583333333333343</v>
-      </c>
-      <c r="L44">
-        <v>48.733333333333341</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.45">
+        <v>45356</v>
+      </c>
+      <c r="D44">
+        <v>22.1</v>
+      </c>
+      <c r="E44">
+        <v>76.900000000000006</v>
+      </c>
+      <c r="F44">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="G44">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="M44">
+        <v>294.8704949629435</v>
+      </c>
+      <c r="N44">
+        <v>20.734360281019086</v>
+      </c>
+      <c r="O44">
+        <v>9.7668740022694838</v>
+      </c>
+      <c r="P44">
+        <v>0.95524162106036969</v>
+      </c>
+      <c r="Q44">
+        <v>3.3074999999999993E-2</v>
+      </c>
+      <c r="R44">
+        <v>1.030614703304313E-3</v>
+      </c>
+      <c r="S44">
+        <v>516.04750033059599</v>
+      </c>
+      <c r="T44">
+        <v>24.811124241055534</v>
+      </c>
+      <c r="U44">
+        <v>4.4987569821554123</v>
+      </c>
+      <c r="V44">
+        <v>0.46122572816007251</v>
+      </c>
+      <c r="W44">
+        <v>8.7022499999999999E-3</v>
+      </c>
+      <c r="X44">
+        <v>5.2024185080915637E-4</v>
+      </c>
+      <c r="Y44">
+        <v>670.32696541298287</v>
+      </c>
+      <c r="Z44">
+        <v>176.49667579945191</v>
+      </c>
+      <c r="AA44">
+        <v>1481.2449607065223</v>
+      </c>
+      <c r="AB44">
+        <v>193.14268552539269</v>
+      </c>
+      <c r="AC44">
+        <f>Y44*0.299</f>
+        <v>200.42776265848187</v>
+      </c>
+      <c r="AD44">
+        <v>52.701907393716425</v>
+      </c>
+      <c r="AE44">
+        <v>189.63549851533284</v>
+      </c>
+      <c r="AF44">
+        <v>49.930909583664906</v>
+      </c>
+    </row>
+    <row r="45" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>14</v>
       </c>
       <c r="B45" s="1">
+        <v>45365</v>
+      </c>
+      <c r="K45">
+        <v>84.583333333333343</v>
+      </c>
+      <c r="L45">
+        <v>48.733333333333341</v>
+      </c>
+    </row>
+    <row r="46" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" s="1">
         <v>45385</v>
       </c>
-      <c r="C45">
+      <c r="C46">
         <v>1319.5</v>
       </c>
-      <c r="D45">
+      <c r="D46">
         <v>21.75</v>
       </c>
-      <c r="E45">
+      <c r="E46">
         <v>71.599999999999994</v>
       </c>
-      <c r="F45">
+      <c r="F46">
         <v>2.8519999999999999</v>
       </c>
-      <c r="G45">
+      <c r="G46">
         <v>0.29970000000000002</v>
       </c>
-      <c r="K45">
+      <c r="K46">
         <v>82.983333333333334</v>
       </c>
-      <c r="L45">
+      <c r="L46">
         <v>62.15</v>
       </c>
-      <c r="M45">
+      <c r="M46">
         <v>224.2</v>
       </c>
-      <c r="N45">
+      <c r="N46">
+        <v>32.954685431718381</v>
+      </c>
+      <c r="O46">
+        <v>7.4317257252457098</v>
+      </c>
+      <c r="P46">
+        <v>1.1371749085562419</v>
+      </c>
+      <c r="Q46">
+        <v>3.3134999999999998E-2</v>
+      </c>
+      <c r="R46">
+        <v>2.9771350881952575E-4</v>
+      </c>
+      <c r="S46">
         <v>591.5</v>
       </c>
-      <c r="O45">
+      <c r="T46">
+        <v>25.609865442475606</v>
+      </c>
+      <c r="U46">
+        <v>6.7106484820007593</v>
+      </c>
+      <c r="V46">
+        <v>0.90007576784194165</v>
+      </c>
+      <c r="W46">
+        <v>1.1315E-2</v>
+      </c>
+      <c r="X46">
+        <v>1.0149712639610257E-3</v>
+      </c>
+      <c r="Y46">
         <v>890</v>
       </c>
-      <c r="P45">
+      <c r="Z46">
+        <v>113.28005745031211</v>
+      </c>
+      <c r="AA46">
         <v>1705.6</v>
       </c>
-      <c r="Q45">
-        <f>O45*0.238</f>
-        <v>211.82</v>
-      </c>
-    </row>
-    <row r="1662" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
+      <c r="AB46">
+        <v>150.40049485323803</v>
+      </c>
+      <c r="AC46">
+        <v>211.54468897750871</v>
+      </c>
+      <c r="AD46">
+        <v>26.926669655939463</v>
+      </c>
+    </row>
+    <row r="47" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" s="1">
+        <v>45412</v>
+      </c>
+      <c r="M47">
+        <v>55.377323080508745</v>
+      </c>
+      <c r="N47">
+        <v>16.323194965851901</v>
+      </c>
+      <c r="O47">
+        <v>1.6854307521650567</v>
+      </c>
+      <c r="P47">
+        <v>0.48711354836009996</v>
+      </c>
+      <c r="Q47">
+        <v>3.0525E-2</v>
+      </c>
+      <c r="R47">
+        <v>1.2255202976695161E-3</v>
+      </c>
+      <c r="S47">
+        <v>579.77488595232262</v>
+      </c>
+      <c r="T47">
+        <v>21.582634487979615</v>
+      </c>
+      <c r="U47">
+        <v>7.576394182823563</v>
+      </c>
+      <c r="V47">
+        <v>1.1679757744489696</v>
+      </c>
+      <c r="W47">
+        <v>1.3025000000000002E-2</v>
+      </c>
+      <c r="X47">
+        <v>1.535849384976687E-3</v>
+      </c>
+      <c r="Y47">
+        <v>887.93697486863152</v>
+      </c>
+      <c r="Z47">
+        <v>67.847286123336261</v>
+      </c>
+      <c r="AA47">
+        <v>1523.089183901463</v>
+      </c>
+      <c r="AB47">
+        <v>73.773279696124959</v>
+      </c>
+      <c r="AC47">
+        <v>179.8072374108979</v>
+      </c>
+      <c r="AD47">
+        <v>13.739075439975338</v>
+      </c>
+      <c r="AE47">
+        <v>383.58877314324883</v>
+      </c>
+      <c r="AF47">
+        <v>29.310027605280752</v>
+      </c>
+    </row>
+    <row r="1663" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1640:EQ1819">
-    <sortCondition ref="B2:B2270"/>
-    <sortCondition ref="C2:C2270"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1641:FC1820">
+    <sortCondition ref="B2:B2271"/>
+    <sortCondition ref="C2:C2271"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add N data to simulations, changed N Conc
</commit_message>
<xml_diff>
--- a/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
+++ b/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Prototypes\Cotton\Observed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ApsimX\Prototypes\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7A1473-CFDB-4095-8969-E27CEAA5806C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543C6B41-8DBF-4AFB-B990-B4FA631BB3AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
+    <workbookView xWindow="-28920" yWindow="3360" windowWidth="29040" windowHeight="17640" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
   <sheets>
     <sheet name="CottonObserved" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CottonObserved!$A$1:$EQ$2583</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CottonObserved!$A$1:$EQ$2585</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="24">
   <si>
     <t>SimulationName</t>
   </si>
@@ -93,12 +93,30 @@
   </si>
   <si>
     <t>Cotton.Leaf.CoverGreenError</t>
+  </si>
+  <si>
+    <t>Cotton.Stem.NConc</t>
+  </si>
+  <si>
+    <t>Cotton.Leaf.Live.NConc</t>
+  </si>
+  <si>
+    <t>Bur.NConc</t>
+  </si>
+  <si>
+    <t>Cotton.Fruit.Nconc</t>
+  </si>
+  <si>
+    <t>Cotton.Seed.NConc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -128,10 +146,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,147 +465,146 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C911DF83-7300-4B7A-8A42-16858D40307A}">
-  <dimension ref="A1:Q1662"/>
+  <dimension ref="A1:V1664"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="9980" ySplit="770" topLeftCell="F6" activePane="topRight"/>
-      <selection sqref="A1:A1048576"/>
-      <selection pane="topRight" activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
-      <selection pane="bottomRight" activeCell="G47" sqref="G47"/>
+      <pane xSplit="9345" ySplit="765" topLeftCell="P1"/>
+      <selection pane="topRight" activeCell="R1" sqref="R1:V1048576"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25:XFD25"/>
+      <selection pane="bottomRight" activeCell="R23" sqref="R23:V24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="39.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="39.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="10" width="25.73046875" customWidth="1"/>
-    <col min="11" max="11" width="38.1328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.06640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="36.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="10" width="25.7109375" customWidth="1"/>
+    <col min="11" max="11" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="32.3984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="33.3984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.3984375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.86328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="27.1328125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="34.3984375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="32.3984375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="33.59765625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="30.265625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="34.1328125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="31.86328125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="35.59765625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.265625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="18" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="21.1328125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="16.73046875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="17.86328125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="24.73046875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="20.73046875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="26" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="24.86328125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="27.3984375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="16.73046875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="17.265625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="33.265625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="32.3984375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="32.86328125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="7.73046875" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="7.1328125" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="70" max="71" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="75" max="76" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="70" max="71" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="75" max="76" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="77" max="77" width="23" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="80" max="80" width="23" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="83" max="83" width="23" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="86" max="86" width="23" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="89" max="89" width="23" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="92" max="92" width="23" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="95" max="95" width="23" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="98" max="98" width="23" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="101" max="101" width="23" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="104" max="104" width="24" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="107" max="107" width="24" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="110" max="110" width="24" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="115" max="115" width="19" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="117" max="117" width="19" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="119" max="119" width="19" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="121" max="121" width="19" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="123" max="123" width="19" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="125" max="125" width="19" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="127" max="127" width="19" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="129" max="129" width="19" bestFit="1" customWidth="1"/>
-    <col min="130" max="130" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="131" max="138" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="139" max="139" width="6.1328125" bestFit="1" customWidth="1"/>
-    <col min="140" max="147" width="24.59765625" bestFit="1" customWidth="1"/>
+    <col min="130" max="130" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="131" max="138" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="139" max="139" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="140" max="147" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -638,8 +656,23 @@
       <c r="Q1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="R1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -653,7 +686,7 @@
         <v>96.683333333333337</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -667,7 +700,7 @@
         <v>139.43333333333331</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -681,7 +714,7 @@
         <v>162.56666666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -701,7 +734,7 @@
         <v>183.21666666666667</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -727,7 +760,7 @@
         <v>172.93333333333331</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -759,7 +792,7 @@
         <v>192.94999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -788,7 +821,7 @@
         <v>161.20000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -802,7 +835,7 @@
         <v>3.605272908788857E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -845,8 +878,14 @@
       <c r="P10">
         <v>109.08904747019719</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="R10">
+        <v>2.57275E-2</v>
+      </c>
+      <c r="S10">
+        <v>4.4797500000000004E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -866,7 +905,7 @@
         <v>190.58333333333337</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -910,8 +949,14 @@
       <c r="P12">
         <v>330.63006704592664</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="R12">
+        <v>1.9225000000000003E-2</v>
+      </c>
+      <c r="S12">
+        <v>4.1849999999999998E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -931,7 +976,7 @@
         <v>0.10013140610136738</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -954,7 +999,7 @@
         <v>104.5</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -989,8 +1034,17 @@
       <c r="P15">
         <v>604.68241646966715</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="R15">
+        <v>1.3165E-2</v>
+      </c>
+      <c r="S15">
+        <v>3.9805E-2</v>
+      </c>
+      <c r="U15">
+        <v>3.202E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1016,7 +1070,7 @@
         <v>173.93333333333331</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1071,7 +1125,7 @@
         <v>72.97936</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1092,7 +1146,7 @@
         <v>124.45</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1108,7 +1162,7 @@
       </c>
       <c r="N19" s="2"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -1133,7 +1187,7 @@
       </c>
       <c r="N20" s="2"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -1172,7 +1226,7 @@
         <v>232.28374532317812</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1187,7 +1241,7 @@
         <v>108.51666666666667</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1216,552 +1270,679 @@
       <c r="L23" s="2">
         <v>79.050000000000011</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="R23">
+        <v>1.1295000000000001E-2</v>
+      </c>
+      <c r="S23">
+        <v>3.4539999999999994E-2</v>
+      </c>
+      <c r="T23">
+        <v>1.0438000000000001E-2</v>
+      </c>
+      <c r="V23">
+        <v>4.3422500000000003E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B24" s="1">
+        <v>45412</v>
+      </c>
+      <c r="I24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="R24">
+        <v>1.3667499999999999E-2</v>
+      </c>
+      <c r="S24">
+        <v>3.1032500000000001E-2</v>
+      </c>
+      <c r="T24">
+        <v>9.4684999999999995E-3</v>
+      </c>
+      <c r="V24">
+        <v>4.5307500000000001E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="1">
         <v>45236</v>
       </c>
-      <c r="K24">
+      <c r="K25">
         <v>93.333333333333329</v>
       </c>
-      <c r="L24" s="2">
+      <c r="L25" s="2">
         <v>82.300000000000011</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="1">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="1">
         <v>45243</v>
       </c>
-      <c r="K25">
+      <c r="K26">
         <v>104.5</v>
       </c>
-      <c r="L25" s="2">
+      <c r="L26" s="2">
         <v>135.1</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" s="1">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="1">
         <v>45248</v>
       </c>
-      <c r="K26">
+      <c r="K27">
         <v>124.35000000000002</v>
       </c>
-      <c r="L26" s="2">
+      <c r="L27" s="2">
         <v>158.38333333333333</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" s="1">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="1">
         <v>45254</v>
       </c>
-      <c r="C27">
+      <c r="C28">
         <v>70</v>
       </c>
-      <c r="D27">
+      <c r="D28">
         <v>1.2</v>
       </c>
-      <c r="K27">
+      <c r="K28">
         <v>158.5</v>
       </c>
-      <c r="L27" s="2">
+      <c r="L28" s="2">
         <v>170.91666666666666</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B28" s="1">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="1">
         <v>45259</v>
       </c>
-      <c r="C28">
+      <c r="C29">
         <v>122.5</v>
       </c>
-      <c r="D28">
+      <c r="D29">
         <v>2.5499999999999998</v>
       </c>
-      <c r="F28">
+      <c r="F29">
         <v>0.10798078444273128</v>
       </c>
-      <c r="G28">
+      <c r="G29">
         <v>1.0286612192528072E-2</v>
       </c>
-      <c r="K28">
+      <c r="K29">
         <v>166.08333333333334</v>
       </c>
-      <c r="L28" s="2">
+      <c r="L29" s="2">
         <v>170.3</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" s="1">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="1">
         <v>45266</v>
       </c>
-      <c r="C29">
+      <c r="C30">
         <v>249.5</v>
       </c>
-      <c r="D29">
+      <c r="D30">
         <v>5.4</v>
       </c>
-      <c r="F29">
+      <c r="F30">
         <v>0.21781349165461303</v>
       </c>
-      <c r="G29">
+      <c r="G30">
         <v>3.0473870842271603E-2</v>
       </c>
-      <c r="I29">
+      <c r="I30">
         <v>0.20528846153846153</v>
       </c>
-      <c r="J29">
+      <c r="J30">
         <v>3.5743400843100848E-2</v>
       </c>
-      <c r="K29">
+      <c r="K30">
         <v>182.61666666666667</v>
       </c>
-      <c r="L29" s="2">
+      <c r="L30" s="2">
         <v>167.28333333333333</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" s="1">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="1">
         <v>45273</v>
       </c>
-      <c r="C30">
+      <c r="C31">
         <v>346.84210526315792</v>
       </c>
-      <c r="D30">
+      <c r="D31">
         <v>8.0526315789473681</v>
       </c>
-      <c r="I30">
+      <c r="I31">
         <v>0.30819838056680166</v>
       </c>
-      <c r="J30">
+      <c r="J31">
         <v>4.4581672466543681E-2</v>
       </c>
-      <c r="K30">
+      <c r="K31">
         <v>168.93333333333331</v>
       </c>
-      <c r="L30" s="2">
+      <c r="L31" s="2">
         <v>158.08333333333334</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31" s="1">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="1">
         <v>45274</v>
       </c>
-      <c r="F31">
+      <c r="F32">
         <v>0.45692237396557861</v>
       </c>
-      <c r="G31">
+      <c r="G32">
         <v>5.1146750325636835E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32" s="1">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="1">
         <v>45279</v>
       </c>
-      <c r="C32">
+      <c r="C33">
         <v>462</v>
       </c>
-      <c r="D32">
+      <c r="D33">
         <v>10.15</v>
       </c>
-      <c r="E32">
+      <c r="E33">
         <v>21.25</v>
       </c>
-      <c r="F32">
+      <c r="F33">
         <v>0.90377009469093894</v>
       </c>
-      <c r="G32">
+      <c r="G33">
         <v>0.17957612594849667</v>
       </c>
-      <c r="H32">
-        <f>F32/M32</f>
+      <c r="H33">
+        <f>F33/M33</f>
         <v>1.4968551468417543E-2</v>
       </c>
-      <c r="I32">
+      <c r="I33">
         <v>0.40192307692307694</v>
       </c>
-      <c r="J32">
+      <c r="J33">
         <v>5.4543711246622169E-2</v>
       </c>
-      <c r="K32">
+      <c r="K33">
         <v>158.51666666666665</v>
       </c>
-      <c r="L32">
+      <c r="L33">
         <v>137.65</v>
       </c>
-      <c r="M32">
+      <c r="M33">
         <v>60.377926120494841</v>
       </c>
-      <c r="N32">
+      <c r="N33">
         <v>47.44502885132195</v>
       </c>
-      <c r="P32">
+      <c r="P33">
         <v>107.82295497181678</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" s="1">
+      <c r="R33" s="3">
+        <v>2.6790000000000001E-2</v>
+      </c>
+      <c r="S33" s="3">
+        <v>4.5779999999999994E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="1">
         <v>45288</v>
       </c>
-      <c r="C33">
+      <c r="C34">
         <v>586.5</v>
       </c>
-      <c r="D33">
+      <c r="D34">
         <v>12.2</v>
       </c>
-      <c r="F33">
+      <c r="F34">
         <v>2.1000585963396539</v>
       </c>
-      <c r="G33">
+      <c r="G34">
         <v>0.16175497233014249</v>
       </c>
-      <c r="I33">
+      <c r="I34">
         <v>0.61923076923076925</v>
       </c>
-      <c r="J33">
+      <c r="J34">
         <v>5.8313123992568404E-2</v>
       </c>
-      <c r="K33">
+      <c r="K34">
         <v>183.81666666666663</v>
       </c>
-      <c r="L33" s="2">
+      <c r="L34" s="2">
         <v>185.81666666666663</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B34" s="1">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="1">
         <v>45296</v>
       </c>
-      <c r="C34">
+      <c r="C35">
         <v>793</v>
       </c>
-      <c r="E34">
+      <c r="E35">
         <v>40</v>
       </c>
-      <c r="F34">
+      <c r="F35">
         <v>3.0317071477592523</v>
       </c>
-      <c r="G34">
+      <c r="G35">
         <v>0.33366923094714623</v>
       </c>
-      <c r="H34">
-        <f>F34/M34</f>
+      <c r="H35">
+        <f>F35/M35</f>
         <v>2.1060960200872104E-2</v>
       </c>
-      <c r="I34">
+      <c r="I35">
         <v>0.76298076923076918</v>
       </c>
-      <c r="J34">
+      <c r="J35">
         <v>7.3246859198435113E-2</v>
       </c>
-      <c r="K34">
+      <c r="K35">
         <v>174.58333333333334</v>
       </c>
-      <c r="L34" s="2">
+      <c r="L35" s="2">
         <v>149.88333333333335</v>
       </c>
-      <c r="M34">
+      <c r="M35">
         <v>143.94914186456293</v>
       </c>
-      <c r="N34">
+      <c r="N35">
         <v>181.99552389227946</v>
       </c>
-      <c r="P34">
+      <c r="P35">
         <v>325.94466575684237</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35" s="1">
+      <c r="R35" s="3">
+        <v>1.805E-2</v>
+      </c>
+      <c r="S35" s="3">
+        <v>4.1440000000000005E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="1">
         <v>45302</v>
       </c>
-      <c r="C35">
+      <c r="C36">
         <v>956.5</v>
       </c>
-      <c r="D35">
+      <c r="D36">
         <v>16.2</v>
       </c>
-      <c r="I35">
+      <c r="I36">
         <v>0.86442307692307696</v>
       </c>
-      <c r="J35">
+      <c r="J36">
         <v>5.5622450987683897E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
-        <v>14</v>
-      </c>
-      <c r="B36" s="1">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="1">
         <v>45306</v>
       </c>
-      <c r="C36">
+      <c r="C37">
         <v>1006</v>
       </c>
-      <c r="I36">
+      <c r="I37">
         <v>0.9259615384615385</v>
       </c>
-      <c r="J36">
+      <c r="J37">
         <v>4.7935013232664241E-2</v>
       </c>
-      <c r="K36">
+      <c r="K37">
         <v>133.11666666666665</v>
       </c>
-      <c r="L36" s="2">
+      <c r="L37" s="2">
         <v>100.80000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" s="1">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="1">
         <v>45307</v>
       </c>
-      <c r="D37">
+      <c r="D38">
         <v>17</v>
       </c>
-      <c r="E37">
+      <c r="E38">
         <v>54.5</v>
       </c>
-      <c r="F37">
+      <c r="F38">
         <v>4.0425206810776277</v>
       </c>
-      <c r="G37">
+      <c r="G38">
         <v>0.37827040810057388</v>
       </c>
-      <c r="H37">
-        <f>F37/M37</f>
+      <c r="H38">
+        <f>F38/M38</f>
         <v>1.8643711192968791E-2</v>
       </c>
-      <c r="M37">
+      <c r="M38">
         <v>216.8302565533308</v>
       </c>
-      <c r="N37">
+      <c r="N38">
         <v>304.20829456947212</v>
       </c>
-      <c r="O37">
+      <c r="O38">
         <v>35.676835928243406</v>
       </c>
-      <c r="P37">
+      <c r="P38">
         <v>556.71538705104638</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
-        <v>14</v>
-      </c>
-      <c r="B38" s="1">
+      <c r="R38" s="3">
+        <v>1.3804999999999998E-2</v>
+      </c>
+      <c r="S38" s="3">
+        <v>4.0665000000000007E-2</v>
+      </c>
+      <c r="U38">
+        <v>3.1247499999999997E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="1">
         <v>45314</v>
       </c>
-      <c r="C38">
+      <c r="C39">
         <v>1191.5</v>
       </c>
-      <c r="D38">
+      <c r="D39">
         <v>18.25</v>
       </c>
-      <c r="I38">
+      <c r="I39">
         <v>0.9802884615384615</v>
       </c>
-      <c r="J38">
+      <c r="J39">
         <v>6.4726008422452033E-2</v>
       </c>
-      <c r="K38">
+      <c r="K39">
         <v>150.83333333333334</v>
       </c>
-      <c r="L38">
+      <c r="L39">
         <v>119.81666666666666</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
-        <v>14</v>
-      </c>
-      <c r="B39" s="1">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" s="1">
         <v>45323</v>
       </c>
-      <c r="K39">
+      <c r="K40">
         <v>188.48333333333335</v>
       </c>
-      <c r="L39">
+      <c r="L40">
         <v>172.45000000000005</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
-        <v>14</v>
-      </c>
-      <c r="B40" s="1">
+      <c r="R40" s="3">
+        <v>1.07435E-2</v>
+      </c>
+      <c r="S40" s="3">
+        <v>3.7872499999999996E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" s="1">
         <v>45331</v>
       </c>
-      <c r="F40">
+      <c r="F41">
         <v>5.5032705000000002</v>
       </c>
-      <c r="G40">
+      <c r="G41">
         <v>1.6615774246742543E-2</v>
       </c>
-      <c r="K40">
+      <c r="K41">
         <v>165.13333333333333</v>
       </c>
-      <c r="L40">
+      <c r="L41">
         <v>133.63333333333333</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
-        <v>14</v>
-      </c>
-      <c r="B41" s="1">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" s="1">
         <v>45335</v>
       </c>
-      <c r="K41" s="2">
+      <c r="K42" s="2">
         <v>146.33333333333334</v>
       </c>
-      <c r="L41">
+      <c r="L42">
         <v>103.91666666666669</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
-        <v>14</v>
-      </c>
-      <c r="B42" s="1">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" s="1">
         <v>45345</v>
       </c>
-      <c r="C42">
+      <c r="C43">
         <v>1375</v>
       </c>
-      <c r="F42">
+      <c r="F43">
         <v>6.2965385000000005</v>
       </c>
-      <c r="G42">
+      <c r="G43">
         <v>0.3468610456650591</v>
       </c>
-      <c r="K42" s="2">
+      <c r="K43" s="2">
         <v>126.25000000000001</v>
       </c>
-      <c r="L42">
+      <c r="L43">
         <v>83.516666666666666</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
-        <v>14</v>
-      </c>
-      <c r="B43" s="1">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44" s="1">
+        <v>45355</v>
+      </c>
+      <c r="K44" s="2"/>
+      <c r="R44" s="3">
+        <v>9.216499999999999E-3</v>
+      </c>
+      <c r="S44" s="3">
+        <v>3.5055000000000003E-2</v>
+      </c>
+      <c r="T44" s="3">
+        <v>1.2669999999999999E-2</v>
+      </c>
+      <c r="V44" s="3">
+        <v>4.0005000000000006E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" s="1">
         <v>45356</v>
       </c>
-      <c r="D43">
+      <c r="D45">
         <v>22.1</v>
       </c>
-      <c r="E43">
+      <c r="E45">
         <v>76.900000000000006</v>
       </c>
-      <c r="F43">
+      <c r="F45">
         <v>4.8499999999999996</v>
       </c>
-      <c r="G43">
+      <c r="G45">
         <v>0.16900000000000001</v>
       </c>
-      <c r="M43">
+      <c r="M45">
         <v>294.8704949629435</v>
       </c>
-      <c r="N43">
+      <c r="N45">
         <v>516.04750033059599</v>
       </c>
-      <c r="O43">
+      <c r="O45">
         <v>670.32696541298287</v>
       </c>
-      <c r="P43">
+      <c r="P45">
         <v>1481.2449607065223</v>
       </c>
-      <c r="Q43">
-        <f>O43*0.299</f>
+      <c r="Q45">
+        <f>O45*0.299</f>
         <v>200.42776265848187</v>
       </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
-        <v>14</v>
-      </c>
-      <c r="B44" s="1">
+      <c r="R45" s="3">
+        <v>8.7022499999999999E-3</v>
+      </c>
+      <c r="S45" s="3">
+        <v>3.3075E-2</v>
+      </c>
+      <c r="T45" s="3">
+        <v>1.0208749999999999E-2</v>
+      </c>
+      <c r="V45" s="3">
+        <v>4.1472499999999995E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" s="1">
         <v>45365</v>
       </c>
-      <c r="K44">
+      <c r="K46">
         <v>84.583333333333343</v>
       </c>
-      <c r="L44">
+      <c r="L46">
         <v>48.733333333333341</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
-        <v>14</v>
-      </c>
-      <c r="B45" s="1">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" s="1">
         <v>45385</v>
       </c>
-      <c r="C45">
+      <c r="C47">
         <v>1319.5</v>
       </c>
-      <c r="D45">
+      <c r="D47">
         <v>21.75</v>
       </c>
-      <c r="E45">
+      <c r="E47">
         <v>71.599999999999994</v>
       </c>
-      <c r="F45">
+      <c r="F47">
         <v>2.8519999999999999</v>
       </c>
-      <c r="G45">
+      <c r="G47">
         <v>0.29970000000000002</v>
       </c>
-      <c r="K45">
+      <c r="K47">
         <v>82.983333333333334</v>
       </c>
-      <c r="L45">
+      <c r="L47">
         <v>62.15</v>
       </c>
-    </row>
-    <row r="1662" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
+      <c r="R47" s="3">
+        <v>1.1314999999999999E-2</v>
+      </c>
+      <c r="S47" s="3">
+        <v>3.3135000000000005E-2</v>
+      </c>
+      <c r="T47" s="3">
+        <v>1.57425E-2</v>
+      </c>
+      <c r="V47" s="3">
+        <v>4.2617500000000003E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" s="1">
+        <v>45412</v>
+      </c>
+      <c r="R48" s="3">
+        <v>1.3025E-2</v>
+      </c>
+      <c r="S48" s="3">
+        <v>3.0525000000000004E-2</v>
+      </c>
+      <c r="T48" s="3">
+        <v>9.8587500000000012E-3</v>
+      </c>
+      <c r="V48" s="3">
+        <v>4.5824999999999998E-2</v>
+      </c>
+    </row>
+    <row r="1664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1640:EQ1819">
-    <sortCondition ref="B2:B2270"/>
-    <sortCondition ref="C2:C2270"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1642:EQ1821">
+    <sortCondition ref="B2:B2272"/>
+    <sortCondition ref="C2:C2272"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added SeedCotton weights & Gin TO
</commit_message>
<xml_diff>
--- a/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
+++ b/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ApsimX\Prototypes\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543C6B41-8DBF-4AFB-B990-B4FA631BB3AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0EE3B3E-C9D3-4803-8AF5-14901AA82FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="3360" windowWidth="29040" windowHeight="17640" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="28">
   <si>
     <t>SimulationName</t>
   </si>
@@ -108,6 +108,18 @@
   </si>
   <si>
     <t>Cotton.Seed.NConc</t>
+  </si>
+  <si>
+    <t>Cotton.SeedCotton.Wt</t>
+  </si>
+  <si>
+    <t>percent_l</t>
+  </si>
+  <si>
+    <t>Cotton.Lint.Wt</t>
+  </si>
+  <si>
+    <t>Cotton.Seed.Wt</t>
   </si>
 </sst>
 </file>
@@ -465,13 +477,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C911DF83-7300-4B7A-8A42-16858D40307A}">
-  <dimension ref="A1:V1664"/>
+  <dimension ref="A1:Z1664"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="9345" ySplit="765" topLeftCell="P1"/>
-      <selection pane="topRight" activeCell="R1" sqref="R1:V1048576"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25:XFD25"/>
-      <selection pane="bottomRight" activeCell="R23" sqref="R23:V24"/>
+      <pane xSplit="9345" ySplit="765" topLeftCell="V28" activePane="bottomRight"/>
+      <selection pane="topRight" activeCell="W1" sqref="W1:Z1"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24:XFD24"/>
+      <selection pane="bottomRight" activeCell="Z48" sqref="Z48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,7 +616,7 @@
     <col min="140" max="147" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -671,8 +683,20 @@
       <c r="V1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W1" t="s">
+        <v>24</v>
+      </c>
+      <c r="X1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -686,7 +710,7 @@
         <v>96.683333333333337</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -700,7 +724,7 @@
         <v>139.43333333333331</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -714,7 +738,7 @@
         <v>162.56666666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -734,7 +758,7 @@
         <v>183.21666666666667</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -760,7 +784,7 @@
         <v>172.93333333333331</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -792,7 +816,7 @@
         <v>192.94999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -821,7 +845,7 @@
         <v>161.20000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -835,7 +859,7 @@
         <v>3.605272908788857E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -885,7 +909,7 @@
         <v>4.4797500000000004E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -905,7 +929,7 @@
         <v>190.58333333333337</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -956,7 +980,7 @@
         <v>4.1849999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -976,7 +1000,7 @@
         <v>0.10013140610136738</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -999,7 +1023,7 @@
         <v>104.5</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1044,7 +1068,7 @@
         <v>3.202E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1070,7 +1094,7 @@
         <v>173.93333333333331</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1125,7 +1149,7 @@
         <v>72.97936</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1146,7 +1170,7 @@
         <v>124.45</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1162,7 +1186,7 @@
       </c>
       <c r="N19" s="2"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -1187,7 +1211,7 @@
       </c>
       <c r="N20" s="2"/>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -1226,7 +1250,7 @@
         <v>232.28374532317812</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1241,7 +1265,7 @@
         <v>108.51666666666667</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1283,7 +1307,7 @@
         <v>4.3422500000000003E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1305,8 +1329,20 @@
       <c r="V24">
         <v>4.5307500000000001E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W24">
+        <v>358.7</v>
+      </c>
+      <c r="X24">
+        <v>0.43490381934764427</v>
+      </c>
+      <c r="Y24">
+        <v>156</v>
+      </c>
+      <c r="Z24">
+        <v>202.7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -1320,7 +1356,7 @@
         <v>82.300000000000011</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -1334,7 +1370,7 @@
         <v>135.1</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -1348,7 +1384,7 @@
         <v>158.38333333333333</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -1368,7 +1404,7 @@
         <v>170.91666666666666</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -1394,7 +1430,7 @@
         <v>170.3</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -1426,7 +1462,7 @@
         <v>167.28333333333333</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -1452,7 +1488,7 @@
         <v>158.08333333333334</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -1466,7 +1502,7 @@
         <v>5.1146750325636835E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -1520,7 +1556,7 @@
         <v>4.5779999999999994E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -1552,7 +1588,7 @@
         <v>185.81666666666663</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -1603,7 +1639,7 @@
         <v>4.1440000000000005E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -1623,7 +1659,7 @@
         <v>5.5622450987683897E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -1646,7 +1682,7 @@
         <v>100.80000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -1691,7 +1727,7 @@
         <v>3.1247499999999997E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -1717,7 +1753,7 @@
         <v>119.81666666666666</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -1737,7 +1773,7 @@
         <v>3.7872499999999996E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -1757,7 +1793,7 @@
         <v>133.63333333333333</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -1771,7 +1807,7 @@
         <v>103.91666666666669</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -1794,7 +1830,7 @@
         <v>83.516666666666666</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -1815,7 +1851,7 @@
         <v>4.0005000000000006E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -1863,7 +1899,7 @@
         <v>4.1472499999999995E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -1877,7 +1913,7 @@
         <v>48.733333333333341</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -1918,7 +1954,7 @@
         <v>4.2617500000000003E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>14</v>
       </c>
@@ -1936,6 +1972,18 @@
       </c>
       <c r="V48" s="3">
         <v>4.5824999999999998E-2</v>
+      </c>
+      <c r="W48">
+        <v>314.10000000000002</v>
+      </c>
+      <c r="X48">
+        <v>0.43425660617637696</v>
+      </c>
+      <c r="Y48">
+        <v>136.4</v>
+      </c>
+      <c r="Z48">
+        <v>177.7</v>
       </c>
     </row>
     <row r="1664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated Gin TO data
</commit_message>
<xml_diff>
--- a/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
+++ b/Prototypes/Cotton/Observed/ForestHillObserved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ApsimX\Prototypes\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0EE3B3E-C9D3-4803-8AF5-14901AA82FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C330FC8-1D49-4715-937C-8B6795818B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="3360" windowWidth="29040" windowHeight="17640" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="29">
   <si>
     <t>SimulationName</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>Cotton.Seed.Wt</t>
+  </si>
+  <si>
+    <t>Cotton.Lint.Bales</t>
   </si>
 </sst>
 </file>
@@ -477,13 +480,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C911DF83-7300-4B7A-8A42-16858D40307A}">
-  <dimension ref="A1:Z1664"/>
+  <dimension ref="A1:AA1664"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="9345" ySplit="765" topLeftCell="V28" activePane="bottomRight"/>
-      <selection pane="topRight" activeCell="W1" sqref="W1:Z1"/>
+      <pane xSplit="9345" ySplit="765" topLeftCell="W22" activePane="bottomRight"/>
+      <selection pane="topRight" activeCell="AA2" sqref="AA2"/>
       <selection pane="bottomLeft" activeCell="A24" sqref="A24:XFD24"/>
-      <selection pane="bottomRight" activeCell="Z48" sqref="Z48"/>
+      <selection pane="bottomRight" activeCell="AA48" sqref="AA48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,7 +619,7 @@
     <col min="140" max="147" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -695,8 +698,11 @@
       <c r="Z1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -710,7 +716,7 @@
         <v>96.683333333333337</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -724,7 +730,7 @@
         <v>139.43333333333331</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -738,7 +744,7 @@
         <v>162.56666666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -758,7 +764,7 @@
         <v>183.21666666666667</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -784,7 +790,7 @@
         <v>172.93333333333331</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -816,7 +822,7 @@
         <v>192.94999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -845,7 +851,7 @@
         <v>161.20000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -859,7 +865,7 @@
         <v>3.605272908788857E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -909,7 +915,7 @@
         <v>4.4797500000000004E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -929,7 +935,7 @@
         <v>190.58333333333337</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -980,7 +986,7 @@
         <v>4.1849999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1000,7 +1006,7 @@
         <v>0.10013140610136738</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1023,7 +1029,7 @@
         <v>104.5</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1068,7 +1074,7 @@
         <v>3.202E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1094,7 +1100,7 @@
         <v>173.93333333333331</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1149,7 +1155,7 @@
         <v>72.97936</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1170,7 +1176,7 @@
         <v>124.45</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1186,7 +1192,7 @@
       </c>
       <c r="N19" s="2"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -1211,7 +1217,7 @@
       </c>
       <c r="N20" s="2"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -1250,7 +1256,7 @@
         <v>232.28374532317812</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1265,7 +1271,7 @@
         <v>108.51666666666667</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1307,7 +1313,7 @@
         <v>4.3422500000000003E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1330,19 +1336,25 @@
         <v>4.5307500000000001E-2</v>
       </c>
       <c r="W24">
-        <v>358.7</v>
+        <v>663.71759259259261</v>
       </c>
       <c r="X24">
         <v>0.43490381934764427</v>
       </c>
       <c r="Y24">
-        <v>156</v>
+        <f>W24*X24</f>
+        <v>288.65331598674226</v>
       </c>
       <c r="Z24">
-        <v>202.7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+        <f>W24-Y24</f>
+        <v>375.06427660585035</v>
+      </c>
+      <c r="AA24">
+        <f>Y24/22.7</f>
+        <v>12.716005109548117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -1356,7 +1368,7 @@
         <v>82.300000000000011</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -1370,7 +1382,7 @@
         <v>135.1</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -1384,7 +1396,7 @@
         <v>158.38333333333333</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -1404,7 +1416,7 @@
         <v>170.91666666666666</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -1430,7 +1442,7 @@
         <v>170.3</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -1462,7 +1474,7 @@
         <v>167.28333333333333</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -1488,7 +1500,7 @@
         <v>158.08333333333334</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -1502,7 +1514,7 @@
         <v>5.1146750325636835E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -1556,7 +1568,7 @@
         <v>4.5779999999999994E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -1588,7 +1600,7 @@
         <v>185.81666666666663</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -1639,7 +1651,7 @@
         <v>4.1440000000000005E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -1659,7 +1671,7 @@
         <v>5.5622450987683897E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -1682,7 +1694,7 @@
         <v>100.80000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -1727,7 +1739,7 @@
         <v>3.1247499999999997E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -1753,7 +1765,7 @@
         <v>119.81666666666666</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -1773,7 +1785,7 @@
         <v>3.7872499999999996E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -1793,7 +1805,7 @@
         <v>133.63333333333333</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -1807,7 +1819,7 @@
         <v>103.91666666666669</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -1830,7 +1842,7 @@
         <v>83.516666666666666</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -1851,7 +1863,7 @@
         <v>4.0005000000000006E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -1899,7 +1911,7 @@
         <v>4.1472499999999995E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -1913,7 +1925,7 @@
         <v>48.733333333333341</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -1954,7 +1966,7 @@
         <v>4.2617500000000003E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>14</v>
       </c>
@@ -1974,16 +1986,22 @@
         <v>4.5824999999999998E-2</v>
       </c>
       <c r="W48">
-        <v>314.10000000000002</v>
+        <v>679.21296296296293</v>
       </c>
       <c r="X48">
         <v>0.43425660617637696</v>
       </c>
       <c r="Y48">
-        <v>136.4</v>
+        <f>W48*X48</f>
+        <v>294.95271616729752</v>
       </c>
       <c r="Z48">
-        <v>177.7</v>
+        <f>W48-Y48</f>
+        <v>384.26024679566541</v>
+      </c>
+      <c r="AA48">
+        <f>Y48/22.7</f>
+        <v>12.99351172543161</v>
       </c>
     </row>
     <row r="1664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>